<commit_message>
updated the hw for the lookmatif assignment
</commit_message>
<xml_diff>
--- a/docs/unit1/2_lookup_match_if/(Starter-Workbook)-HW-Lookups-Match-IF.xlsx
+++ b/docs/unit1/2_lookup_match_if/(Starter-Workbook)-HW-Lookups-Match-IF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\CCE270\Starter\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{96617156-F3B0-4DD9-9FBE-BD5B6F6EECB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15D79F5-89BF-478A-8386-1B21DDAD0F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydrometer Analysis" sheetId="1" r:id="rId1"/>
@@ -21,11 +21,9 @@
   </sheets>
   <definedNames>
     <definedName name="GravelCosts">Tables!$V$1:$W$6</definedName>
-    <definedName name="Gs">'Hydrometer Analysis'!$E$4</definedName>
     <definedName name="PricePerTest">Tables!$J$1:$T$9</definedName>
     <definedName name="StokesLaw">Tables!$A$1:$H$17</definedName>
-    <definedName name="Tf">'Hydrometer Analysis'!$E$5</definedName>
-    <definedName name="Ws">'Hydrometer Analysis'!$E$3</definedName>
+    <definedName name="ws">'Hydrometer Analysis'!$E$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="88">
   <si>
     <t>Hydrometer Analysis</t>
   </si>
@@ -304,6 +302,9 @@
   </si>
   <si>
     <t>Median:</t>
+  </si>
+  <si>
+    <t>Median2</t>
   </si>
 </sst>
 </file>
@@ -824,7 +825,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="102">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -986,6 +987,18 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -996,17 +1009,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1015,6 +1017,12 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1038,17 +1046,38 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="6">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <name val="Arial"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -1065,6 +1094,7 @@
         <name val="Arial"/>
         <scheme val="minor"/>
       </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <fill>
@@ -1093,9 +1123,9 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="Soil Services-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="3"/>
-      <tableStyleElement type="firstRowStripe" dxfId="2"/>
-      <tableStyleElement type="secondRowStripe" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="5"/>
+      <tableStyleElement type="firstRowStripe" dxfId="4"/>
+      <tableStyleElement type="secondRowStripe" dxfId="3"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1191,15 +1221,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:G31">
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:H31">
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Customer ID number"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Soil Service"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Test Quantities"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Price per Test"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Total Price"/>
-    <tableColumn id="6" xr3:uid="{E1FBCE2D-3A17-45F8-8CDE-14190854D098}" name="Average" dataDxfId="0"/>
-    <tableColumn id="7" xr3:uid="{7D474FD2-944C-44F2-B763-DB4A11808F26}" name="Median"/>
+    <tableColumn id="6" xr3:uid="{E1FBCE2D-3A17-45F8-8CDE-14190854D098}" name="Average" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{7D474FD2-944C-44F2-B763-DB4A11808F26}" name="Median" dataDxfId="1"/>
+    <tableColumn id="8" xr3:uid="{1611D9D7-110E-4D92-A43F-A2E57908C929}" name="Median2" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Soil Services-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1409,7 +1440,7 @@
   <dimension ref="A1:M28"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="L31" sqref="L31"/>
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1421,12 +1452,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="26.25">
-      <c r="A1" s="79" t="s">
+      <c r="A1" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
       <c r="G1" s="1"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -1436,11 +1467,11 @@
       <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13" ht="15">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="80"/>
-      <c r="C2" s="80"/>
+      <c r="B2" s="75"/>
+      <c r="C2" s="75"/>
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1453,11 +1484,11 @@
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:13" ht="15">
-      <c r="A3" s="71" t="s">
+      <c r="A3" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="72"/>
-      <c r="C3" s="73"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="79"/>
       <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1470,11 +1501,11 @@
       <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:13" ht="15">
-      <c r="A4" s="74" t="s">
+      <c r="A4" s="80" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="75"/>
-      <c r="C4" s="76"/>
+      <c r="B4" s="81"/>
+      <c r="C4" s="82"/>
       <c r="D4" s="9" t="s">
         <v>9</v>
       </c>
@@ -1485,11 +1516,11 @@
       <c r="G4" s="11"/>
     </row>
     <row r="5" spans="1:13" ht="15">
-      <c r="A5" s="82" t="s">
+      <c r="A5" s="83" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="83"/>
-      <c r="C5" s="84"/>
+      <c r="B5" s="84"/>
+      <c r="C5" s="85"/>
       <c r="D5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1502,9 +1533,9 @@
       <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:13" ht="15">
-      <c r="A6" s="85"/>
-      <c r="B6" s="86"/>
-      <c r="C6" s="87"/>
+      <c r="A6" s="86"/>
+      <c r="B6" s="87"/>
+      <c r="C6" s="88"/>
       <c r="D6" s="9" t="s">
         <v>13</v>
       </c>
@@ -1515,11 +1546,11 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:13" ht="15">
-      <c r="A7" s="71" t="s">
+      <c r="A7" s="77" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="72"/>
-      <c r="C7" s="73"/>
+      <c r="B7" s="78"/>
+      <c r="C7" s="79"/>
       <c r="D7" s="6" t="s">
         <v>16</v>
       </c>
@@ -1530,11 +1561,11 @@
       <c r="G7" s="11"/>
     </row>
     <row r="8" spans="1:13" ht="15">
-      <c r="A8" s="74" t="s">
+      <c r="A8" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="75"/>
-      <c r="C8" s="76"/>
+      <c r="B8" s="81"/>
+      <c r="C8" s="82"/>
       <c r="D8" s="9" t="s">
         <v>18</v>
       </c>
@@ -1545,11 +1576,11 @@
       <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:13" ht="15">
-      <c r="A9" s="71" t="s">
+      <c r="A9" s="77" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="72"/>
-      <c r="C9" s="73"/>
+      <c r="B9" s="78"/>
+      <c r="C9" s="79"/>
       <c r="D9" s="6" t="s">
         <v>20</v>
       </c>
@@ -1559,11 +1590,11 @@
       <c r="I9" s="17"/>
     </row>
     <row r="10" spans="1:13" ht="15">
-      <c r="A10" s="74" t="s">
+      <c r="A10" s="80" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="75"/>
-      <c r="C10" s="76"/>
+      <c r="B10" s="81"/>
+      <c r="C10" s="82"/>
       <c r="D10" s="9" t="s">
         <v>22</v>
       </c>
@@ -1572,11 +1603,11 @@
       <c r="G10" s="19"/>
     </row>
     <row r="11" spans="1:13" ht="15">
-      <c r="A11" s="71" t="s">
+      <c r="A11" s="77" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="72"/>
-      <c r="C11" s="73"/>
+      <c r="B11" s="78"/>
+      <c r="C11" s="79"/>
       <c r="D11" s="6" t="s">
         <v>24</v>
       </c>
@@ -1588,25 +1619,25 @@
     </row>
     <row r="12" spans="1:13" ht="18.75" customHeight="1"/>
     <row r="13" spans="1:13" ht="24.75" customHeight="1">
-      <c r="A13" s="77" t="s">
+      <c r="A13" s="89" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="77" t="s">
+      <c r="B13" s="89" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="77" t="s">
+      <c r="C13" s="89" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="77" t="s">
+      <c r="D13" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="77" t="s">
+      <c r="E13" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="77" t="s">
+      <c r="F13" s="89" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="77" t="s">
+      <c r="G13" s="89" t="s">
         <v>31</v>
       </c>
       <c r="H13" s="2"/>
@@ -1617,13 +1648,13 @@
       <c r="M13" s="2"/>
     </row>
     <row r="14" spans="1:13" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A14" s="78"/>
-      <c r="B14" s="78"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
+      <c r="A14" s="90"/>
+      <c r="B14" s="90"/>
+      <c r="C14" s="90"/>
+      <c r="D14" s="90"/>
+      <c r="E14" s="90"/>
+      <c r="F14" s="90"/>
+      <c r="G14" s="90"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1638,21 +1669,13 @@
       <c r="B15" s="22">
         <v>32</v>
       </c>
-      <c r="C15" s="56">
-        <v>30.260999999999999</v>
-      </c>
-      <c r="D15" s="57">
-        <v>0.79890000000000005</v>
-      </c>
-      <c r="E15" s="58">
-        <v>33</v>
-      </c>
+      <c r="C15" s="56"/>
+      <c r="D15" s="57"/>
+      <c r="E15" s="58"/>
       <c r="F15" s="22">
         <v>10.9</v>
       </c>
-      <c r="G15" s="56">
-        <v>8.7159990820000005E-2</v>
-      </c>
+      <c r="G15" s="56"/>
     </row>
     <row r="16" spans="1:13" thickBot="1">
       <c r="A16" s="21">
@@ -1661,21 +1684,13 @@
       <c r="B16" s="22">
         <v>30</v>
       </c>
-      <c r="C16" s="59">
-        <v>28.260999999999999</v>
-      </c>
-      <c r="D16" s="60">
-        <v>0.74609999999999999</v>
-      </c>
-      <c r="E16" s="61">
-        <v>31</v>
-      </c>
+      <c r="C16" s="59"/>
+      <c r="D16" s="60"/>
+      <c r="E16" s="61"/>
       <c r="F16" s="22">
         <v>11.2</v>
       </c>
-      <c r="G16" s="59">
-        <v>6.2473802510000002E-2</v>
-      </c>
+      <c r="G16" s="59"/>
     </row>
     <row r="17" spans="1:7" thickBot="1">
       <c r="A17" s="21">
@@ -1684,21 +1699,13 @@
       <c r="B17" s="22">
         <v>27</v>
       </c>
-      <c r="C17" s="59">
-        <v>25.260999999999999</v>
-      </c>
-      <c r="D17" s="60">
-        <v>0.66690000000000005</v>
-      </c>
-      <c r="E17" s="61">
-        <v>28</v>
-      </c>
+      <c r="C17" s="59"/>
+      <c r="D17" s="60"/>
+      <c r="E17" s="61"/>
       <c r="F17" s="22">
         <v>11.7</v>
       </c>
-      <c r="G17" s="59">
-        <v>4.5150946829999997E-2</v>
-      </c>
+      <c r="G17" s="59"/>
     </row>
     <row r="18" spans="1:7" thickBot="1">
       <c r="A18" s="21">
@@ -1707,21 +1714,13 @@
       <c r="B18" s="22">
         <v>24</v>
       </c>
-      <c r="C18" s="59">
-        <v>22.260999999999999</v>
-      </c>
-      <c r="D18" s="60">
-        <v>0.5877</v>
-      </c>
-      <c r="E18" s="61">
-        <v>25</v>
-      </c>
+      <c r="C18" s="59"/>
+      <c r="D18" s="60"/>
+      <c r="E18" s="61"/>
       <c r="F18" s="22">
         <v>12.2</v>
       </c>
-      <c r="G18" s="59">
-        <v>3.2601595050000001E-2</v>
-      </c>
+      <c r="G18" s="59"/>
     </row>
     <row r="19" spans="1:7" thickBot="1">
       <c r="A19" s="21">
@@ -1730,21 +1729,13 @@
       <c r="B19" s="22">
         <v>22</v>
       </c>
-      <c r="C19" s="59">
-        <v>20.260999999999999</v>
-      </c>
-      <c r="D19" s="60">
-        <v>0.53490000000000004</v>
-      </c>
-      <c r="E19" s="61">
-        <v>23</v>
-      </c>
+      <c r="C19" s="59"/>
+      <c r="D19" s="60"/>
+      <c r="E19" s="61"/>
       <c r="F19" s="22">
         <v>12.5</v>
       </c>
-      <c r="G19" s="59">
-        <v>2.3334523780000001E-2</v>
-      </c>
+      <c r="G19" s="59"/>
     </row>
     <row r="20" spans="1:7" thickBot="1">
       <c r="A20" s="21">
@@ -1753,21 +1744,13 @@
       <c r="B20" s="22">
         <v>20</v>
       </c>
-      <c r="C20" s="59">
-        <v>18.260999999999999</v>
-      </c>
-      <c r="D20" s="60">
-        <v>0.48209999999999997</v>
-      </c>
-      <c r="E20" s="61">
-        <v>21</v>
-      </c>
+      <c r="C20" s="59"/>
+      <c r="D20" s="60"/>
+      <c r="E20" s="61"/>
       <c r="F20" s="22">
         <v>12.9</v>
       </c>
-      <c r="G20" s="59">
-        <v>1.6761921129999999E-2</v>
-      </c>
+      <c r="G20" s="59"/>
     </row>
     <row r="21" spans="1:7" thickBot="1">
       <c r="A21" s="21">
@@ -1776,21 +1759,13 @@
       <c r="B21" s="22">
         <v>17</v>
       </c>
-      <c r="C21" s="59">
-        <v>15.260999999999999</v>
-      </c>
-      <c r="D21" s="60">
-        <v>0.40289999999999998</v>
-      </c>
-      <c r="E21" s="61">
-        <v>18</v>
-      </c>
+      <c r="C21" s="59"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="61"/>
       <c r="F21" s="22">
         <v>13.3</v>
       </c>
-      <c r="G21" s="59">
-        <v>1.242951326E-2</v>
-      </c>
+      <c r="G21" s="59"/>
     </row>
     <row r="22" spans="1:7" thickBot="1">
       <c r="A22" s="21">
@@ -1799,21 +1774,13 @@
       <c r="B22" s="22">
         <v>15</v>
       </c>
-      <c r="C22" s="59">
-        <v>13.260999999999999</v>
-      </c>
-      <c r="D22" s="60">
-        <v>0.35010000000000002</v>
-      </c>
-      <c r="E22" s="61">
-        <v>16</v>
-      </c>
+      <c r="C22" s="59"/>
+      <c r="D22" s="60"/>
+      <c r="E22" s="61"/>
       <c r="F22" s="22">
         <v>13.7</v>
       </c>
-      <c r="G22" s="59">
-        <v>8.9201793699999997E-3</v>
-      </c>
+      <c r="G22" s="59"/>
     </row>
     <row r="23" spans="1:7" thickBot="1">
       <c r="A23" s="21">
@@ -1822,21 +1789,13 @@
       <c r="B23" s="22">
         <v>13</v>
       </c>
-      <c r="C23" s="59">
-        <v>11.260999999999999</v>
-      </c>
-      <c r="D23" s="60">
-        <v>0.29730000000000001</v>
-      </c>
-      <c r="E23" s="61">
-        <v>14</v>
-      </c>
+      <c r="C23" s="59"/>
+      <c r="D23" s="60"/>
+      <c r="E23" s="61"/>
       <c r="F23" s="22">
         <v>14</v>
       </c>
-      <c r="G23" s="59">
-        <v>6.3762057679999998E-3</v>
-      </c>
+      <c r="G23" s="59"/>
     </row>
     <row r="24" spans="1:7" thickBot="1">
       <c r="A24" s="21">
@@ -1845,21 +1804,13 @@
       <c r="B24" s="22">
         <v>9</v>
       </c>
-      <c r="C24" s="59">
-        <v>7.2610000000000001</v>
-      </c>
-      <c r="D24" s="60">
-        <v>0.19170000000000001</v>
-      </c>
-      <c r="E24" s="61">
-        <v>10</v>
-      </c>
+      <c r="C24" s="59"/>
+      <c r="D24" s="60"/>
+      <c r="E24" s="61"/>
       <c r="F24" s="22">
         <v>14.7</v>
       </c>
-      <c r="G24" s="59">
-        <v>1.8040361360000001E-3</v>
-      </c>
+      <c r="G24" s="59"/>
     </row>
     <row r="25" spans="1:7" thickBot="1">
       <c r="A25" s="21">
@@ -1868,21 +1819,13 @@
       <c r="B25" s="22">
         <v>8</v>
       </c>
-      <c r="C25" s="59">
-        <v>6.2610000000000001</v>
-      </c>
-      <c r="D25" s="60">
-        <v>0.1653</v>
-      </c>
-      <c r="E25" s="61">
-        <v>9</v>
-      </c>
+      <c r="C25" s="59"/>
+      <c r="D25" s="60"/>
+      <c r="E25" s="61"/>
       <c r="F25" s="22">
         <v>14.8</v>
       </c>
-      <c r="G25" s="59">
-        <v>1.3294657179999999E-3</v>
-      </c>
+      <c r="G25" s="59"/>
     </row>
     <row r="26" spans="1:7" ht="15">
       <c r="A26" s="23"/>
@@ -1913,11 +1856,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C6"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="E13:E14"/>
@@ -1930,6 +1868,11 @@
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1941,10 +1884,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G35"/>
+  <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1954,10 +1897,10 @@
     <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="55" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" style="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="12.75">
+    <row r="1" spans="1:8" ht="12.75">
       <c r="A1" s="26" t="s">
         <v>32</v>
       </c>
@@ -1973,14 +1916,17 @@
       <c r="E1" s="26" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="97" t="s">
+      <c r="F1" s="72" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="97" t="s">
+      <c r="G1" s="72" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="12.75">
+      <c r="H1" s="72" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" ht="12.75">
       <c r="A2" s="28">
         <v>1124</v>
       </c>
@@ -1992,9 +1938,11 @@
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="28"/>
-    </row>
-    <row r="3" spans="1:7" ht="12.75">
+      <c r="F2" s="100"/>
+      <c r="G2" s="101"/>
+      <c r="H2" s="101"/>
+    </row>
+    <row r="3" spans="1:8" ht="12.75">
       <c r="A3" s="28">
         <v>1107</v>
       </c>
@@ -2006,9 +1954,11 @@
       </c>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-    </row>
-    <row r="4" spans="1:7" ht="12.75">
+      <c r="F3" s="100"/>
+      <c r="G3" s="100"/>
+      <c r="H3" s="101"/>
+    </row>
+    <row r="4" spans="1:8" ht="12.75">
       <c r="A4" s="28">
         <v>1163</v>
       </c>
@@ -2020,9 +1970,11 @@
       </c>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
-      <c r="F4" s="28"/>
-    </row>
-    <row r="5" spans="1:7" ht="12.75">
+      <c r="F4" s="100"/>
+      <c r="G4" s="100"/>
+      <c r="H4" s="101"/>
+    </row>
+    <row r="5" spans="1:8" ht="12.75">
       <c r="A5" s="28">
         <v>1182</v>
       </c>
@@ -2034,9 +1986,11 @@
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
-      <c r="F5" s="28"/>
-    </row>
-    <row r="6" spans="1:7" ht="12.75">
+      <c r="F5" s="100"/>
+      <c r="G5" s="100"/>
+      <c r="H5" s="101"/>
+    </row>
+    <row r="6" spans="1:8" ht="12.75">
       <c r="A6" s="28">
         <v>1175</v>
       </c>
@@ -2048,9 +2002,11 @@
       </c>
       <c r="D6" s="28"/>
       <c r="E6" s="28"/>
-      <c r="F6" s="28"/>
-    </row>
-    <row r="7" spans="1:7" ht="12.75">
+      <c r="F6" s="100"/>
+      <c r="G6" s="101"/>
+      <c r="H6" s="101"/>
+    </row>
+    <row r="7" spans="1:8" ht="12.75">
       <c r="A7" s="28">
         <v>1049</v>
       </c>
@@ -2062,9 +2018,11 @@
       </c>
       <c r="D7" s="28"/>
       <c r="E7" s="28"/>
-      <c r="F7" s="28"/>
-    </row>
-    <row r="8" spans="1:7" ht="12.75">
+      <c r="F7" s="100"/>
+      <c r="G7" s="101"/>
+      <c r="H7" s="101"/>
+    </row>
+    <row r="8" spans="1:8" ht="12.75">
       <c r="A8" s="28">
         <v>1006</v>
       </c>
@@ -2076,9 +2034,11 @@
       </c>
       <c r="D8" s="28"/>
       <c r="E8" s="28"/>
-      <c r="F8" s="28"/>
-    </row>
-    <row r="9" spans="1:7" ht="12.75">
+      <c r="F8" s="100"/>
+      <c r="G8" s="101"/>
+      <c r="H8" s="101"/>
+    </row>
+    <row r="9" spans="1:8" ht="12.75">
       <c r="A9" s="28">
         <v>1129</v>
       </c>
@@ -2090,9 +2050,11 @@
       </c>
       <c r="D9" s="28"/>
       <c r="E9" s="28"/>
-      <c r="F9" s="28"/>
-    </row>
-    <row r="10" spans="1:7" ht="12.75">
+      <c r="F9" s="100"/>
+      <c r="G9" s="101"/>
+      <c r="H9" s="101"/>
+    </row>
+    <row r="10" spans="1:8" ht="12.75">
       <c r="A10" s="28">
         <v>1236</v>
       </c>
@@ -2104,9 +2066,11 @@
       </c>
       <c r="D10" s="28"/>
       <c r="E10" s="28"/>
-      <c r="F10" s="28"/>
-    </row>
-    <row r="11" spans="1:7" ht="12.75">
+      <c r="F10" s="100"/>
+      <c r="G10" s="101"/>
+      <c r="H10" s="101"/>
+    </row>
+    <row r="11" spans="1:8" ht="12.75">
       <c r="A11" s="28">
         <v>1041</v>
       </c>
@@ -2118,9 +2082,11 @@
       </c>
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
-      <c r="F11" s="28"/>
-    </row>
-    <row r="12" spans="1:7" ht="12.75">
+      <c r="F11" s="100"/>
+      <c r="G11" s="101"/>
+      <c r="H11" s="101"/>
+    </row>
+    <row r="12" spans="1:8" ht="12.75">
       <c r="A12" s="28">
         <v>1016</v>
       </c>
@@ -2132,9 +2098,11 @@
       </c>
       <c r="D12" s="28"/>
       <c r="E12" s="28"/>
-      <c r="F12" s="28"/>
-    </row>
-    <row r="13" spans="1:7" ht="12.75">
+      <c r="F12" s="100"/>
+      <c r="G12" s="101"/>
+      <c r="H12" s="101"/>
+    </row>
+    <row r="13" spans="1:8" ht="12.75">
       <c r="A13" s="28">
         <v>1195</v>
       </c>
@@ -2146,9 +2114,11 @@
       </c>
       <c r="D13" s="28"/>
       <c r="E13" s="28"/>
-      <c r="F13" s="28"/>
-    </row>
-    <row r="14" spans="1:7" ht="12.75">
+      <c r="F13" s="100"/>
+      <c r="G13" s="101"/>
+      <c r="H13" s="101"/>
+    </row>
+    <row r="14" spans="1:8" ht="12.75">
       <c r="A14" s="28">
         <v>1072</v>
       </c>
@@ -2160,9 +2130,11 @@
       </c>
       <c r="D14" s="28"/>
       <c r="E14" s="28"/>
-      <c r="F14" s="28"/>
-    </row>
-    <row r="15" spans="1:7" ht="12.75">
+      <c r="F14" s="100"/>
+      <c r="G14" s="101"/>
+      <c r="H14" s="101"/>
+    </row>
+    <row r="15" spans="1:8" ht="12.75">
       <c r="A15" s="28">
         <v>1073</v>
       </c>
@@ -2174,9 +2146,11 @@
       </c>
       <c r="D15" s="28"/>
       <c r="E15" s="28"/>
-      <c r="F15" s="28"/>
-    </row>
-    <row r="16" spans="1:7" ht="12.75">
+      <c r="F15" s="100"/>
+      <c r="G15" s="101"/>
+      <c r="H15" s="101"/>
+    </row>
+    <row r="16" spans="1:8" ht="12.75">
       <c r="A16" s="28">
         <v>1101</v>
       </c>
@@ -2188,9 +2162,11 @@
       </c>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
-      <c r="F16" s="28"/>
-    </row>
-    <row r="17" spans="1:6" ht="12.75">
+      <c r="F16" s="100"/>
+      <c r="G16" s="101"/>
+      <c r="H16" s="101"/>
+    </row>
+    <row r="17" spans="1:8" ht="12.75">
       <c r="A17" s="28">
         <v>1026</v>
       </c>
@@ -2202,9 +2178,11 @@
       </c>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
-      <c r="F17" s="28"/>
-    </row>
-    <row r="18" spans="1:6" ht="12.75">
+      <c r="F17" s="100"/>
+      <c r="G17" s="101"/>
+      <c r="H17" s="101"/>
+    </row>
+    <row r="18" spans="1:8" ht="12.75">
       <c r="A18" s="28">
         <v>1040</v>
       </c>
@@ -2216,9 +2194,11 @@
       </c>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
-      <c r="F18" s="28"/>
-    </row>
-    <row r="19" spans="1:6" ht="12.75">
+      <c r="F18" s="100"/>
+      <c r="G18" s="101"/>
+      <c r="H18" s="101"/>
+    </row>
+    <row r="19" spans="1:8" ht="12.75">
       <c r="A19" s="28">
         <v>1126</v>
       </c>
@@ -2230,9 +2210,11 @@
       </c>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
-      <c r="F19" s="28"/>
-    </row>
-    <row r="20" spans="1:6" ht="12.75">
+      <c r="F19" s="100"/>
+      <c r="G19" s="101"/>
+      <c r="H19" s="101"/>
+    </row>
+    <row r="20" spans="1:8" ht="12.75">
       <c r="A20" s="28">
         <v>1181</v>
       </c>
@@ -2244,9 +2226,11 @@
       </c>
       <c r="D20" s="28"/>
       <c r="E20" s="28"/>
-      <c r="F20" s="28"/>
-    </row>
-    <row r="21" spans="1:6" ht="12.75">
+      <c r="F20" s="100"/>
+      <c r="G20" s="101"/>
+      <c r="H20" s="101"/>
+    </row>
+    <row r="21" spans="1:8" ht="12.75">
       <c r="A21" s="28">
         <v>1002</v>
       </c>
@@ -2258,9 +2242,11 @@
       </c>
       <c r="D21" s="28"/>
       <c r="E21" s="28"/>
-      <c r="F21" s="28"/>
-    </row>
-    <row r="22" spans="1:6" ht="12.75">
+      <c r="F21" s="100"/>
+      <c r="G21" s="101"/>
+      <c r="H21" s="101"/>
+    </row>
+    <row r="22" spans="1:8" ht="12.75">
       <c r="A22" s="28">
         <v>1166</v>
       </c>
@@ -2272,9 +2258,11 @@
       </c>
       <c r="D22" s="28"/>
       <c r="E22" s="28"/>
-      <c r="F22" s="28"/>
-    </row>
-    <row r="23" spans="1:6" ht="12.75">
+      <c r="F22" s="100"/>
+      <c r="G22" s="101"/>
+      <c r="H22" s="101"/>
+    </row>
+    <row r="23" spans="1:8" ht="12.75">
       <c r="A23" s="28">
         <v>1248</v>
       </c>
@@ -2286,9 +2274,11 @@
       </c>
       <c r="D23" s="28"/>
       <c r="E23" s="28"/>
-      <c r="F23" s="28"/>
-    </row>
-    <row r="24" spans="1:6" ht="12.75">
+      <c r="F23" s="100"/>
+      <c r="G23" s="101"/>
+      <c r="H23" s="101"/>
+    </row>
+    <row r="24" spans="1:8" ht="12.75">
       <c r="A24" s="28">
         <v>1138</v>
       </c>
@@ -2300,9 +2290,11 @@
       </c>
       <c r="D24" s="28"/>
       <c r="E24" s="28"/>
-      <c r="F24" s="28"/>
-    </row>
-    <row r="25" spans="1:6" ht="12.75">
+      <c r="F24" s="100"/>
+      <c r="G24" s="101"/>
+      <c r="H24" s="101"/>
+    </row>
+    <row r="25" spans="1:8" ht="12.75">
       <c r="A25" s="28">
         <v>1256</v>
       </c>
@@ -2314,9 +2306,11 @@
       </c>
       <c r="D25" s="28"/>
       <c r="E25" s="28"/>
-      <c r="F25" s="28"/>
-    </row>
-    <row r="26" spans="1:6" ht="12.75">
+      <c r="F25" s="100"/>
+      <c r="G25" s="101"/>
+      <c r="H25" s="101"/>
+    </row>
+    <row r="26" spans="1:8" ht="12.75">
       <c r="A26" s="28">
         <v>1011</v>
       </c>
@@ -2328,9 +2322,11 @@
       </c>
       <c r="D26" s="28"/>
       <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-    </row>
-    <row r="27" spans="1:6" ht="12.75">
+      <c r="F26" s="100"/>
+      <c r="G26" s="101"/>
+      <c r="H26" s="101"/>
+    </row>
+    <row r="27" spans="1:8" ht="12.75">
       <c r="A27" s="28">
         <v>1163</v>
       </c>
@@ -2342,9 +2338,11 @@
       </c>
       <c r="D27" s="28"/>
       <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-    </row>
-    <row r="28" spans="1:6" ht="12.75">
+      <c r="F27" s="100"/>
+      <c r="G27" s="101"/>
+      <c r="H27" s="101"/>
+    </row>
+    <row r="28" spans="1:8" ht="12.75">
       <c r="A28" s="28">
         <v>1002</v>
       </c>
@@ -2356,9 +2354,11 @@
       </c>
       <c r="D28" s="28"/>
       <c r="E28" s="28"/>
-      <c r="F28" s="28"/>
-    </row>
-    <row r="29" spans="1:6" ht="12.75">
+      <c r="F28" s="100"/>
+      <c r="G28" s="101"/>
+      <c r="H28" s="101"/>
+    </row>
+    <row r="29" spans="1:8" ht="12.75">
       <c r="A29" s="28">
         <v>1078</v>
       </c>
@@ -2370,9 +2370,11 @@
       </c>
       <c r="D29" s="28"/>
       <c r="E29" s="28"/>
-      <c r="F29" s="28"/>
-    </row>
-    <row r="30" spans="1:6" ht="12.75">
+      <c r="F29" s="100"/>
+      <c r="G29" s="101"/>
+      <c r="H29" s="101"/>
+    </row>
+    <row r="30" spans="1:8" ht="12.75">
       <c r="A30" s="28">
         <v>1058</v>
       </c>
@@ -2384,9 +2386,11 @@
       </c>
       <c r="D30" s="28"/>
       <c r="E30" s="28"/>
-      <c r="F30" s="28"/>
-    </row>
-    <row r="31" spans="1:6" ht="12.75">
+      <c r="F30" s="100"/>
+      <c r="G30" s="101"/>
+      <c r="H30" s="101"/>
+    </row>
+    <row r="31" spans="1:8" ht="12.75">
       <c r="A31" s="28">
         <v>1135</v>
       </c>
@@ -2398,28 +2402,30 @@
       </c>
       <c r="D31" s="28"/>
       <c r="E31" s="28"/>
-      <c r="F31" s="28"/>
+      <c r="F31" s="100"/>
+      <c r="G31" s="101"/>
+      <c r="H31" s="101"/>
     </row>
     <row r="33" spans="4:6" ht="12.75">
-      <c r="D33" s="98" t="s">
+      <c r="D33" s="73" t="s">
         <v>85</v>
       </c>
       <c r="E33" s="31"/>
-      <c r="F33" s="31"/>
+      <c r="F33" s="71"/>
     </row>
     <row r="34" spans="4:6" ht="15.75" customHeight="1">
-      <c r="D34" s="98" t="s">
+      <c r="D34" s="73" t="s">
         <v>86</v>
       </c>
       <c r="E34" s="31"/>
-      <c r="F34" s="31"/>
+      <c r="F34" s="71"/>
     </row>
     <row r="35" spans="4:6" ht="15.75" customHeight="1">
       <c r="D35" s="30" t="s">
         <v>44</v>
       </c>
       <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
+      <c r="F35" s="71"/>
     </row>
   </sheetData>
   <phoneticPr fontId="22" type="noConversion"/>
@@ -2462,18 +2468,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="88" t="s">
+      <c r="A1" s="91" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="89"/>
-      <c r="C2" s="73"/>
+      <c r="B2" s="92"/>
+      <c r="C2" s="79"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="33" t="s">
@@ -2524,8 +2530,8 @@
       <c r="A8" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="90"/>
-      <c r="C8" s="73"/>
+      <c r="B8" s="93"/>
+      <c r="C8" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3007,47 +3013,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="12.75">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="94" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="80"/>
-      <c r="C1" s="80"/>
-      <c r="D1" s="80"/>
-      <c r="E1" s="80"/>
-      <c r="F1" s="80"/>
-      <c r="G1" s="80"/>
-      <c r="H1" s="80"/>
-      <c r="J1" s="92" t="s">
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="J1" s="95" t="s">
         <v>59</v>
       </c>
-      <c r="K1" s="93"/>
-      <c r="L1" s="93"/>
-      <c r="M1" s="93"/>
-      <c r="N1" s="93"/>
-      <c r="O1" s="93"/>
-      <c r="P1" s="93"/>
-      <c r="Q1" s="93"/>
-      <c r="R1" s="93"/>
-      <c r="S1" s="93"/>
-      <c r="T1" s="94"/>
-      <c r="V1" s="95" t="s">
+      <c r="K1" s="96"/>
+      <c r="L1" s="96"/>
+      <c r="M1" s="96"/>
+      <c r="N1" s="96"/>
+      <c r="O1" s="96"/>
+      <c r="P1" s="96"/>
+      <c r="Q1" s="96"/>
+      <c r="R1" s="96"/>
+      <c r="S1" s="96"/>
+      <c r="T1" s="97"/>
+      <c r="V1" s="98" t="s">
         <v>60</v>
       </c>
-      <c r="W1" s="94"/>
+      <c r="W1" s="97"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1">
       <c r="A2" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="99" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="93"/>
-      <c r="D2" s="93"/>
-      <c r="E2" s="93"/>
-      <c r="F2" s="93"/>
-      <c r="G2" s="93"/>
-      <c r="H2" s="94"/>
+      <c r="C2" s="96"/>
+      <c r="D2" s="96"/>
+      <c r="E2" s="96"/>
+      <c r="F2" s="96"/>
+      <c r="G2" s="96"/>
+      <c r="H2" s="97"/>
       <c r="J2" s="41" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Finished the in class, made a few other changes to formating.
</commit_message>
<xml_diff>
--- a/docs/unit1/2_lookup_match_if/(Starter-Workbook)-HW-Lookups-Match-IF.xlsx
+++ b/docs/unit1/2_lookup_match_if/(Starter-Workbook)-HW-Lookups-Match-IF.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\CCE270\Starter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\CCE270\content\docs\unit1\2_lookup_match_if\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15D79F5-89BF-478A-8386-1B21DDAD0F6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE97372-1F33-4C61-A897-5947626F00E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydrometer Analysis" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,6 @@
     <definedName name="GravelCosts">Tables!$V$1:$W$6</definedName>
     <definedName name="PricePerTest">Tables!$J$1:$T$9</definedName>
     <definedName name="StokesLaw">Tables!$A$1:$H$17</definedName>
-    <definedName name="ws">'Hydrometer Analysis'!$E$3</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="87">
   <si>
     <t>Hydrometer Analysis</t>
   </si>
@@ -302,9 +301,6 @@
   </si>
   <si>
     <t>Median:</t>
-  </si>
-  <si>
-    <t>Median2</t>
   </si>
 </sst>
 </file>
@@ -994,6 +990,12 @@
     <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1046,35 +1048,11 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <name val="Arial"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="5">
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -1123,9 +1101,9 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="Soil Services-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="5"/>
-      <tableStyleElement type="firstRowStripe" dxfId="4"/>
-      <tableStyleElement type="secondRowStripe" dxfId="3"/>
+      <tableStyleElement type="headerRow" dxfId="4"/>
+      <tableStyleElement type="firstRowStripe" dxfId="3"/>
+      <tableStyleElement type="secondRowStripe" dxfId="2"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1221,16 +1199,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:H31">
-  <tableColumns count="8">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:G31">
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Customer ID number"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Soil Service"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Test Quantities"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Price per Test"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Total Price"/>
-    <tableColumn id="6" xr3:uid="{E1FBCE2D-3A17-45F8-8CDE-14190854D098}" name="Average" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{7D474FD2-944C-44F2-B763-DB4A11808F26}" name="Median" dataDxfId="1"/>
-    <tableColumn id="8" xr3:uid="{1611D9D7-110E-4D92-A43F-A2E57908C929}" name="Median2" dataDxfId="0"/>
+    <tableColumn id="6" xr3:uid="{E1FBCE2D-3A17-45F8-8CDE-14190854D098}" name="Average" dataDxfId="1"/>
+    <tableColumn id="7" xr3:uid="{7D474FD2-944C-44F2-B763-DB4A11808F26}" name="Median" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Soil Services-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1439,8 +1416,8 @@
   </sheetPr>
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1452,12 +1429,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="26.25">
-      <c r="A1" s="74" t="s">
+      <c r="A1" s="76" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
       <c r="G1" s="1"/>
       <c r="H1" s="2"/>
       <c r="I1" s="2"/>
@@ -1467,11 +1444,11 @@
       <c r="M1" s="2"/>
     </row>
     <row r="2" spans="1:13" ht="15">
-      <c r="A2" s="76" t="s">
+      <c r="A2" s="78" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
+      <c r="B2" s="77"/>
+      <c r="C2" s="77"/>
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
@@ -1484,11 +1461,11 @@
       <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:13" ht="15">
-      <c r="A3" s="77" t="s">
+      <c r="A3" s="79" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="78"/>
-      <c r="C3" s="79"/>
+      <c r="B3" s="80"/>
+      <c r="C3" s="81"/>
       <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
@@ -1501,11 +1478,11 @@
       <c r="G3" s="8"/>
     </row>
     <row r="4" spans="1:13" ht="15">
-      <c r="A4" s="80" t="s">
+      <c r="A4" s="82" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="81"/>
-      <c r="C4" s="82"/>
+      <c r="B4" s="83"/>
+      <c r="C4" s="84"/>
       <c r="D4" s="9" t="s">
         <v>9</v>
       </c>
@@ -1516,11 +1493,11 @@
       <c r="G4" s="11"/>
     </row>
     <row r="5" spans="1:13" ht="15">
-      <c r="A5" s="83" t="s">
+      <c r="A5" s="85" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="84"/>
-      <c r="C5" s="85"/>
+      <c r="B5" s="86"/>
+      <c r="C5" s="87"/>
       <c r="D5" s="6" t="s">
         <v>11</v>
       </c>
@@ -1533,9 +1510,9 @@
       <c r="G5" s="12"/>
     </row>
     <row r="6" spans="1:13" ht="15">
-      <c r="A6" s="86"/>
-      <c r="B6" s="87"/>
-      <c r="C6" s="88"/>
+      <c r="A6" s="88"/>
+      <c r="B6" s="89"/>
+      <c r="C6" s="90"/>
       <c r="D6" s="9" t="s">
         <v>13</v>
       </c>
@@ -1546,11 +1523,11 @@
       <c r="G6" s="8"/>
     </row>
     <row r="7" spans="1:13" ht="15">
-      <c r="A7" s="77" t="s">
+      <c r="A7" s="79" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="78"/>
-      <c r="C7" s="79"/>
+      <c r="B7" s="80"/>
+      <c r="C7" s="81"/>
       <c r="D7" s="6" t="s">
         <v>16</v>
       </c>
@@ -1561,11 +1538,11 @@
       <c r="G7" s="11"/>
     </row>
     <row r="8" spans="1:13" ht="15">
-      <c r="A8" s="80" t="s">
+      <c r="A8" s="82" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="81"/>
-      <c r="C8" s="82"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="84"/>
       <c r="D8" s="9" t="s">
         <v>18</v>
       </c>
@@ -1576,11 +1553,11 @@
       <c r="G8" s="11"/>
     </row>
     <row r="9" spans="1:13" ht="15">
-      <c r="A9" s="77" t="s">
+      <c r="A9" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="78"/>
-      <c r="C9" s="79"/>
+      <c r="B9" s="80"/>
+      <c r="C9" s="81"/>
       <c r="D9" s="6" t="s">
         <v>20</v>
       </c>
@@ -1590,11 +1567,11 @@
       <c r="I9" s="17"/>
     </row>
     <row r="10" spans="1:13" ht="15">
-      <c r="A10" s="80" t="s">
+      <c r="A10" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="81"/>
-      <c r="C10" s="82"/>
+      <c r="B10" s="83"/>
+      <c r="C10" s="84"/>
       <c r="D10" s="9" t="s">
         <v>22</v>
       </c>
@@ -1603,11 +1580,11 @@
       <c r="G10" s="19"/>
     </row>
     <row r="11" spans="1:13" ht="15">
-      <c r="A11" s="77" t="s">
+      <c r="A11" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="78"/>
-      <c r="C11" s="79"/>
+      <c r="B11" s="80"/>
+      <c r="C11" s="81"/>
       <c r="D11" s="6" t="s">
         <v>24</v>
       </c>
@@ -1619,25 +1596,25 @@
     </row>
     <row r="12" spans="1:13" ht="18.75" customHeight="1"/>
     <row r="13" spans="1:13" ht="24.75" customHeight="1">
-      <c r="A13" s="89" t="s">
+      <c r="A13" s="91" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="89" t="s">
+      <c r="B13" s="91" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="89" t="s">
+      <c r="C13" s="91" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="89" t="s">
+      <c r="D13" s="91" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="89" t="s">
+      <c r="E13" s="91" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="89" t="s">
+      <c r="F13" s="91" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="89" t="s">
+      <c r="G13" s="91" t="s">
         <v>31</v>
       </c>
       <c r="H13" s="2"/>
@@ -1648,13 +1625,13 @@
       <c r="M13" s="2"/>
     </row>
     <row r="14" spans="1:13" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A14" s="90"/>
-      <c r="B14" s="90"/>
-      <c r="C14" s="90"/>
-      <c r="D14" s="90"/>
-      <c r="E14" s="90"/>
-      <c r="F14" s="90"/>
-      <c r="G14" s="90"/>
+      <c r="A14" s="92"/>
+      <c r="B14" s="92"/>
+      <c r="C14" s="92"/>
+      <c r="D14" s="92"/>
+      <c r="E14" s="92"/>
+      <c r="F14" s="92"/>
+      <c r="G14" s="92"/>
       <c r="H14" s="2"/>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -1884,10 +1861,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H35"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
@@ -1900,7 +1877,7 @@
     <col min="6" max="6" width="13.28515625" style="55" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.75">
+    <row r="1" spans="1:7" ht="12.75">
       <c r="A1" s="26" t="s">
         <v>32</v>
       </c>
@@ -1922,11 +1899,8 @@
       <c r="G1" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="H1" s="72" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" ht="12.75">
+    </row>
+    <row r="2" spans="1:7" ht="12.75">
       <c r="A2" s="28">
         <v>1124</v>
       </c>
@@ -1938,11 +1912,10 @@
       </c>
       <c r="D2" s="28"/>
       <c r="E2" s="28"/>
-      <c r="F2" s="100"/>
-      <c r="G2" s="101"/>
-      <c r="H2" s="101"/>
-    </row>
-    <row r="3" spans="1:8" ht="12.75">
+      <c r="F2" s="74"/>
+      <c r="G2" s="75"/>
+    </row>
+    <row r="3" spans="1:7" ht="12.75">
       <c r="A3" s="28">
         <v>1107</v>
       </c>
@@ -1954,11 +1927,10 @@
       </c>
       <c r="D3" s="28"/>
       <c r="E3" s="28"/>
-      <c r="F3" s="100"/>
-      <c r="G3" s="100"/>
-      <c r="H3" s="101"/>
-    </row>
-    <row r="4" spans="1:8" ht="12.75">
+      <c r="F3" s="74"/>
+      <c r="G3" s="74"/>
+    </row>
+    <row r="4" spans="1:7" ht="12.75">
       <c r="A4" s="28">
         <v>1163</v>
       </c>
@@ -1970,11 +1942,10 @@
       </c>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
-      <c r="F4" s="100"/>
-      <c r="G4" s="100"/>
-      <c r="H4" s="101"/>
-    </row>
-    <row r="5" spans="1:8" ht="12.75">
+      <c r="F4" s="74"/>
+      <c r="G4" s="74"/>
+    </row>
+    <row r="5" spans="1:7" ht="12.75">
       <c r="A5" s="28">
         <v>1182</v>
       </c>
@@ -1986,11 +1957,10 @@
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="28"/>
-      <c r="F5" s="100"/>
-      <c r="G5" s="100"/>
-      <c r="H5" s="101"/>
-    </row>
-    <row r="6" spans="1:8" ht="12.75">
+      <c r="F5" s="74"/>
+      <c r="G5" s="74"/>
+    </row>
+    <row r="6" spans="1:7" ht="12.75">
       <c r="A6" s="28">
         <v>1175</v>
       </c>
@@ -2002,11 +1972,10 @@
       </c>
       <c r="D6" s="28"/>
       <c r="E6" s="28"/>
-      <c r="F6" s="100"/>
-      <c r="G6" s="101"/>
-      <c r="H6" s="101"/>
-    </row>
-    <row r="7" spans="1:8" ht="12.75">
+      <c r="F6" s="74"/>
+      <c r="G6" s="75"/>
+    </row>
+    <row r="7" spans="1:7" ht="12.75">
       <c r="A7" s="28">
         <v>1049</v>
       </c>
@@ -2018,11 +1987,10 @@
       </c>
       <c r="D7" s="28"/>
       <c r="E7" s="28"/>
-      <c r="F7" s="100"/>
-      <c r="G7" s="101"/>
-      <c r="H7" s="101"/>
-    </row>
-    <row r="8" spans="1:8" ht="12.75">
+      <c r="F7" s="74"/>
+      <c r="G7" s="75"/>
+    </row>
+    <row r="8" spans="1:7" ht="12.75">
       <c r="A8" s="28">
         <v>1006</v>
       </c>
@@ -2034,11 +2002,10 @@
       </c>
       <c r="D8" s="28"/>
       <c r="E8" s="28"/>
-      <c r="F8" s="100"/>
-      <c r="G8" s="101"/>
-      <c r="H8" s="101"/>
-    </row>
-    <row r="9" spans="1:8" ht="12.75">
+      <c r="F8" s="74"/>
+      <c r="G8" s="75"/>
+    </row>
+    <row r="9" spans="1:7" ht="12.75">
       <c r="A9" s="28">
         <v>1129</v>
       </c>
@@ -2050,11 +2017,10 @@
       </c>
       <c r="D9" s="28"/>
       <c r="E9" s="28"/>
-      <c r="F9" s="100"/>
-      <c r="G9" s="101"/>
-      <c r="H9" s="101"/>
-    </row>
-    <row r="10" spans="1:8" ht="12.75">
+      <c r="F9" s="74"/>
+      <c r="G9" s="75"/>
+    </row>
+    <row r="10" spans="1:7" ht="12.75">
       <c r="A10" s="28">
         <v>1236</v>
       </c>
@@ -2066,11 +2032,10 @@
       </c>
       <c r="D10" s="28"/>
       <c r="E10" s="28"/>
-      <c r="F10" s="100"/>
-      <c r="G10" s="101"/>
-      <c r="H10" s="101"/>
-    </row>
-    <row r="11" spans="1:8" ht="12.75">
+      <c r="F10" s="74"/>
+      <c r="G10" s="75"/>
+    </row>
+    <row r="11" spans="1:7" ht="12.75">
       <c r="A11" s="28">
         <v>1041</v>
       </c>
@@ -2082,11 +2047,10 @@
       </c>
       <c r="D11" s="28"/>
       <c r="E11" s="28"/>
-      <c r="F11" s="100"/>
-      <c r="G11" s="101"/>
-      <c r="H11" s="101"/>
-    </row>
-    <row r="12" spans="1:8" ht="12.75">
+      <c r="F11" s="74"/>
+      <c r="G11" s="75"/>
+    </row>
+    <row r="12" spans="1:7" ht="12.75">
       <c r="A12" s="28">
         <v>1016</v>
       </c>
@@ -2098,11 +2062,10 @@
       </c>
       <c r="D12" s="28"/>
       <c r="E12" s="28"/>
-      <c r="F12" s="100"/>
-      <c r="G12" s="101"/>
-      <c r="H12" s="101"/>
-    </row>
-    <row r="13" spans="1:8" ht="12.75">
+      <c r="F12" s="74"/>
+      <c r="G12" s="75"/>
+    </row>
+    <row r="13" spans="1:7" ht="12.75">
       <c r="A13" s="28">
         <v>1195</v>
       </c>
@@ -2114,11 +2077,10 @@
       </c>
       <c r="D13" s="28"/>
       <c r="E13" s="28"/>
-      <c r="F13" s="100"/>
-      <c r="G13" s="101"/>
-      <c r="H13" s="101"/>
-    </row>
-    <row r="14" spans="1:8" ht="12.75">
+      <c r="F13" s="74"/>
+      <c r="G13" s="75"/>
+    </row>
+    <row r="14" spans="1:7" ht="12.75">
       <c r="A14" s="28">
         <v>1072</v>
       </c>
@@ -2130,11 +2092,10 @@
       </c>
       <c r="D14" s="28"/>
       <c r="E14" s="28"/>
-      <c r="F14" s="100"/>
-      <c r="G14" s="101"/>
-      <c r="H14" s="101"/>
-    </row>
-    <row r="15" spans="1:8" ht="12.75">
+      <c r="F14" s="74"/>
+      <c r="G14" s="75"/>
+    </row>
+    <row r="15" spans="1:7" ht="12.75">
       <c r="A15" s="28">
         <v>1073</v>
       </c>
@@ -2146,11 +2107,10 @@
       </c>
       <c r="D15" s="28"/>
       <c r="E15" s="28"/>
-      <c r="F15" s="100"/>
-      <c r="G15" s="101"/>
-      <c r="H15" s="101"/>
-    </row>
-    <row r="16" spans="1:8" ht="12.75">
+      <c r="F15" s="74"/>
+      <c r="G15" s="75"/>
+    </row>
+    <row r="16" spans="1:7" ht="12.75">
       <c r="A16" s="28">
         <v>1101</v>
       </c>
@@ -2162,11 +2122,10 @@
       </c>
       <c r="D16" s="28"/>
       <c r="E16" s="28"/>
-      <c r="F16" s="100"/>
-      <c r="G16" s="101"/>
-      <c r="H16" s="101"/>
-    </row>
-    <row r="17" spans="1:8" ht="12.75">
+      <c r="F16" s="74"/>
+      <c r="G16" s="75"/>
+    </row>
+    <row r="17" spans="1:7" ht="12.75">
       <c r="A17" s="28">
         <v>1026</v>
       </c>
@@ -2178,11 +2137,10 @@
       </c>
       <c r="D17" s="28"/>
       <c r="E17" s="28"/>
-      <c r="F17" s="100"/>
-      <c r="G17" s="101"/>
-      <c r="H17" s="101"/>
-    </row>
-    <row r="18" spans="1:8" ht="12.75">
+      <c r="F17" s="74"/>
+      <c r="G17" s="75"/>
+    </row>
+    <row r="18" spans="1:7" ht="12.75">
       <c r="A18" s="28">
         <v>1040</v>
       </c>
@@ -2194,11 +2152,10 @@
       </c>
       <c r="D18" s="28"/>
       <c r="E18" s="28"/>
-      <c r="F18" s="100"/>
-      <c r="G18" s="101"/>
-      <c r="H18" s="101"/>
-    </row>
-    <row r="19" spans="1:8" ht="12.75">
+      <c r="F18" s="74"/>
+      <c r="G18" s="75"/>
+    </row>
+    <row r="19" spans="1:7" ht="12.75">
       <c r="A19" s="28">
         <v>1126</v>
       </c>
@@ -2210,11 +2167,10 @@
       </c>
       <c r="D19" s="28"/>
       <c r="E19" s="28"/>
-      <c r="F19" s="100"/>
-      <c r="G19" s="101"/>
-      <c r="H19" s="101"/>
-    </row>
-    <row r="20" spans="1:8" ht="12.75">
+      <c r="F19" s="74"/>
+      <c r="G19" s="75"/>
+    </row>
+    <row r="20" spans="1:7" ht="12.75">
       <c r="A20" s="28">
         <v>1181</v>
       </c>
@@ -2226,11 +2182,10 @@
       </c>
       <c r="D20" s="28"/>
       <c r="E20" s="28"/>
-      <c r="F20" s="100"/>
-      <c r="G20" s="101"/>
-      <c r="H20" s="101"/>
-    </row>
-    <row r="21" spans="1:8" ht="12.75">
+      <c r="F20" s="74"/>
+      <c r="G20" s="75"/>
+    </row>
+    <row r="21" spans="1:7" ht="12.75">
       <c r="A21" s="28">
         <v>1002</v>
       </c>
@@ -2242,11 +2197,10 @@
       </c>
       <c r="D21" s="28"/>
       <c r="E21" s="28"/>
-      <c r="F21" s="100"/>
-      <c r="G21" s="101"/>
-      <c r="H21" s="101"/>
-    </row>
-    <row r="22" spans="1:8" ht="12.75">
+      <c r="F21" s="74"/>
+      <c r="G21" s="75"/>
+    </row>
+    <row r="22" spans="1:7" ht="12.75">
       <c r="A22" s="28">
         <v>1166</v>
       </c>
@@ -2258,11 +2212,10 @@
       </c>
       <c r="D22" s="28"/>
       <c r="E22" s="28"/>
-      <c r="F22" s="100"/>
-      <c r="G22" s="101"/>
-      <c r="H22" s="101"/>
-    </row>
-    <row r="23" spans="1:8" ht="12.75">
+      <c r="F22" s="74"/>
+      <c r="G22" s="75"/>
+    </row>
+    <row r="23" spans="1:7" ht="12.75">
       <c r="A23" s="28">
         <v>1248</v>
       </c>
@@ -2274,11 +2227,10 @@
       </c>
       <c r="D23" s="28"/>
       <c r="E23" s="28"/>
-      <c r="F23" s="100"/>
-      <c r="G23" s="101"/>
-      <c r="H23" s="101"/>
-    </row>
-    <row r="24" spans="1:8" ht="12.75">
+      <c r="F23" s="74"/>
+      <c r="G23" s="75"/>
+    </row>
+    <row r="24" spans="1:7" ht="12.75">
       <c r="A24" s="28">
         <v>1138</v>
       </c>
@@ -2290,11 +2242,10 @@
       </c>
       <c r="D24" s="28"/>
       <c r="E24" s="28"/>
-      <c r="F24" s="100"/>
-      <c r="G24" s="101"/>
-      <c r="H24" s="101"/>
-    </row>
-    <row r="25" spans="1:8" ht="12.75">
+      <c r="F24" s="74"/>
+      <c r="G24" s="75"/>
+    </row>
+    <row r="25" spans="1:7" ht="12.75">
       <c r="A25" s="28">
         <v>1256</v>
       </c>
@@ -2306,11 +2257,10 @@
       </c>
       <c r="D25" s="28"/>
       <c r="E25" s="28"/>
-      <c r="F25" s="100"/>
-      <c r="G25" s="101"/>
-      <c r="H25" s="101"/>
-    </row>
-    <row r="26" spans="1:8" ht="12.75">
+      <c r="F25" s="74"/>
+      <c r="G25" s="75"/>
+    </row>
+    <row r="26" spans="1:7" ht="12.75">
       <c r="A26" s="28">
         <v>1011</v>
       </c>
@@ -2322,11 +2272,10 @@
       </c>
       <c r="D26" s="28"/>
       <c r="E26" s="28"/>
-      <c r="F26" s="100"/>
-      <c r="G26" s="101"/>
-      <c r="H26" s="101"/>
-    </row>
-    <row r="27" spans="1:8" ht="12.75">
+      <c r="F26" s="74"/>
+      <c r="G26" s="75"/>
+    </row>
+    <row r="27" spans="1:7" ht="12.75">
       <c r="A27" s="28">
         <v>1163</v>
       </c>
@@ -2338,11 +2287,10 @@
       </c>
       <c r="D27" s="28"/>
       <c r="E27" s="28"/>
-      <c r="F27" s="100"/>
-      <c r="G27" s="101"/>
-      <c r="H27" s="101"/>
-    </row>
-    <row r="28" spans="1:8" ht="12.75">
+      <c r="F27" s="74"/>
+      <c r="G27" s="75"/>
+    </row>
+    <row r="28" spans="1:7" ht="12.75">
       <c r="A28" s="28">
         <v>1002</v>
       </c>
@@ -2354,11 +2302,10 @@
       </c>
       <c r="D28" s="28"/>
       <c r="E28" s="28"/>
-      <c r="F28" s="100"/>
-      <c r="G28" s="101"/>
-      <c r="H28" s="101"/>
-    </row>
-    <row r="29" spans="1:8" ht="12.75">
+      <c r="F28" s="74"/>
+      <c r="G28" s="75"/>
+    </row>
+    <row r="29" spans="1:7" ht="12.75">
       <c r="A29" s="28">
         <v>1078</v>
       </c>
@@ -2370,11 +2317,10 @@
       </c>
       <c r="D29" s="28"/>
       <c r="E29" s="28"/>
-      <c r="F29" s="100"/>
-      <c r="G29" s="101"/>
-      <c r="H29" s="101"/>
-    </row>
-    <row r="30" spans="1:8" ht="12.75">
+      <c r="F29" s="74"/>
+      <c r="G29" s="75"/>
+    </row>
+    <row r="30" spans="1:7" ht="12.75">
       <c r="A30" s="28">
         <v>1058</v>
       </c>
@@ -2386,11 +2332,10 @@
       </c>
       <c r="D30" s="28"/>
       <c r="E30" s="28"/>
-      <c r="F30" s="100"/>
-      <c r="G30" s="101"/>
-      <c r="H30" s="101"/>
-    </row>
-    <row r="31" spans="1:8" ht="12.75">
+      <c r="F30" s="74"/>
+      <c r="G30" s="75"/>
+    </row>
+    <row r="31" spans="1:7" ht="12.75">
       <c r="A31" s="28">
         <v>1135</v>
       </c>
@@ -2402,9 +2347,8 @@
       </c>
       <c r="D31" s="28"/>
       <c r="E31" s="28"/>
-      <c r="F31" s="100"/>
-      <c r="G31" s="101"/>
-      <c r="H31" s="101"/>
+      <c r="F31" s="74"/>
+      <c r="G31" s="75"/>
     </row>
     <row r="33" spans="4:6" ht="12.75">
       <c r="D33" s="73" t="s">
@@ -2468,18 +2412,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="91" t="s">
+      <c r="A1" s="93" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
     </row>
     <row r="2" spans="1:3">
       <c r="A2" s="32" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="92"/>
-      <c r="C2" s="79"/>
+      <c r="B2" s="94"/>
+      <c r="C2" s="81"/>
     </row>
     <row r="3" spans="1:3">
       <c r="A3" s="33" t="s">
@@ -2530,8 +2474,8 @@
       <c r="A8" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="93"/>
-      <c r="C8" s="79"/>
+      <c r="B8" s="95"/>
+      <c r="C8" s="81"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -3013,47 +2957,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="12.75">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="96" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="75"/>
-      <c r="C1" s="75"/>
-      <c r="D1" s="75"/>
-      <c r="E1" s="75"/>
-      <c r="F1" s="75"/>
-      <c r="G1" s="75"/>
-      <c r="H1" s="75"/>
-      <c r="J1" s="95" t="s">
+      <c r="B1" s="77"/>
+      <c r="C1" s="77"/>
+      <c r="D1" s="77"/>
+      <c r="E1" s="77"/>
+      <c r="F1" s="77"/>
+      <c r="G1" s="77"/>
+      <c r="H1" s="77"/>
+      <c r="J1" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="96"/>
-      <c r="O1" s="96"/>
-      <c r="P1" s="96"/>
-      <c r="Q1" s="96"/>
-      <c r="R1" s="96"/>
-      <c r="S1" s="96"/>
-      <c r="T1" s="97"/>
-      <c r="V1" s="98" t="s">
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="98"/>
+      <c r="N1" s="98"/>
+      <c r="O1" s="98"/>
+      <c r="P1" s="98"/>
+      <c r="Q1" s="98"/>
+      <c r="R1" s="98"/>
+      <c r="S1" s="98"/>
+      <c r="T1" s="99"/>
+      <c r="V1" s="100" t="s">
         <v>60</v>
       </c>
-      <c r="W1" s="97"/>
+      <c r="W1" s="99"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1">
       <c r="A2" s="40" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="99" t="s">
+      <c r="B2" s="101" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="96"/>
-      <c r="D2" s="96"/>
-      <c r="E2" s="96"/>
-      <c r="F2" s="96"/>
-      <c r="G2" s="96"/>
-      <c r="H2" s="97"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
+      <c r="E2" s="98"/>
+      <c r="F2" s="98"/>
+      <c r="G2" s="98"/>
+      <c r="H2" s="99"/>
       <c r="J2" s="41" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
reformatted homework starter sheet for unit 1 - lecture 01.
</commit_message>
<xml_diff>
--- a/docs/unit1/2_lookup_match_if/(Starter-Workbook)-HW-Lookups-Match-IF.xlsx
+++ b/docs/unit1/2_lookup_match_if/(Starter-Workbook)-HW-Lookups-Match-IF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\CCE270\content\docs\unit1\2_lookup_match_if\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/PycharmProjects/content/docs/unit1/2_lookup_match_if/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AE97372-1F33-4C61-A897-5947626F00E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31485A32-0D4B-1341-954C-088C603BE32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="24020" yWindow="2680" windowWidth="33860" windowHeight="24420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydrometer Analysis" sheetId="1" r:id="rId1"/>
@@ -307,11 +307,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="27">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -323,18 +324,21 @@
       <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -343,56 +347,66 @@
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -400,18 +414,21 @@
       <sz val="10"/>
       <color theme="0"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FFFFFFFF"/>
       <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -424,6 +441,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="9"/>
@@ -435,6 +453,7 @@
       <sz val="20"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
@@ -450,8 +469,31 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Arial (Body)"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial (Body)"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="25">
+  <fills count="27">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -462,18 +504,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFFFFF"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF26A69A"/>
-        <bgColor rgb="FF26A69A"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDDF2F0"/>
-        <bgColor rgb="FFDDF2F0"/>
       </patternFill>
     </fill>
     <fill>
@@ -490,26 +520,8 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFC6A679"/>
-        <bgColor rgb="FFC6A679"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFF7F2EB"/>
         <bgColor rgb="FFF7F2EB"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF46524"/>
-        <bgColor rgb="FFF46524"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFE6DD"/>
-        <bgColor rgb="FFFFE6DD"/>
       </patternFill>
     </fill>
     <fill>
@@ -596,8 +608,50 @@
         <bgColor rgb="FFFDE9D9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="-0.499984740745262"/>
+        <bgColor rgb="FFC6A679"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor rgb="FFF46524"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor rgb="FF26A69A"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="-0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="19">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -817,64 +871,44 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top style="thin">
+        <color theme="1"/>
+      </top>
+      <bottom style="thin">
+        <color theme="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="102">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="89">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -886,89 +920,66 @@
     <xf numFmtId="10" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="9" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="15" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="2" fontId="3" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="3" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="3" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="3" fontId="15" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="165" fontId="3" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="3" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="20" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="21" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="3" fillId="13" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="15" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="17" fillId="22" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="17" fillId="17" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="10" fontId="17" fillId="22" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="10" fontId="17" fillId="17" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="2" fontId="16" fillId="23" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="16" fillId="18" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -979,101 +990,145 @@
     <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="21" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="22" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="3" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="24" fillId="20" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="24" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="20" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
+  <dxfs count="3">
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -1101,9 +1156,9 @@
   </dxfs>
   <tableStyles count="1">
     <tableStyle name="Soil Services-style" pivot="0" count="3" xr9:uid="{00000000-0011-0000-FFFF-FFFF00000000}">
-      <tableStyleElement type="headerRow" dxfId="4"/>
-      <tableStyleElement type="firstRowStripe" dxfId="3"/>
-      <tableStyleElement type="secondRowStripe" dxfId="2"/>
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
   <extLst>
@@ -1196,21 +1251,6 @@
     <xdr:clientData fLocksWithSheet="0"/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
-</file>
-
-<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A1:G31">
-  <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Customer ID number"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Soil Service"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Test Quantities"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Price per Test"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Total Price"/>
-    <tableColumn id="6" xr3:uid="{E1FBCE2D-3A17-45F8-8CDE-14190854D098}" name="Average" dataDxfId="1"/>
-    <tableColumn id="7" xr3:uid="{7D474FD2-944C-44F2-B763-DB4A11808F26}" name="Median" dataDxfId="0"/>
-  </tableColumns>
-  <tableStyleInfo name="Soil Services-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
-</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1416,420 +1456,420 @@
   </sheetPr>
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" customWidth="1"/>
     <col min="3" max="6" width="11" customWidth="1"/>
-    <col min="7" max="13" width="14.5703125" customWidth="1"/>
+    <col min="7" max="13" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="26.25">
-      <c r="A1" s="76" t="s">
+    <row r="1" spans="1:13" s="55" customFormat="1" ht="32" customHeight="1">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2"/>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="57"/>
+      <c r="I1" s="57"/>
+      <c r="J1" s="57"/>
+      <c r="K1" s="57"/>
+      <c r="L1" s="57"/>
+      <c r="M1" s="57"/>
     </row>
     <row r="2" spans="1:13" ht="15">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="77"/>
-      <c r="C2" s="77"/>
-      <c r="D2" s="3" t="s">
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
+      <c r="D2" s="53" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="54" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="5"/>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:13" ht="15">
-      <c r="A3" s="79" t="s">
+      <c r="A3" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="80"/>
-      <c r="C3" s="81"/>
-      <c r="D3" s="6" t="s">
+      <c r="B3" s="69"/>
+      <c r="C3" s="70"/>
+      <c r="D3" s="50" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="50">
         <v>50</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="F3" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="8"/>
+      <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:13" ht="15">
-      <c r="A4" s="82" t="s">
+      <c r="A4" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="83"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="9" t="s">
+      <c r="B4" s="69"/>
+      <c r="C4" s="70"/>
+      <c r="D4" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="50">
         <v>2.6</v>
       </c>
-      <c r="F4" s="10"/>
-      <c r="G4" s="11"/>
+      <c r="F4" s="52"/>
+      <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:13" ht="15">
-      <c r="A5" s="85" t="s">
+      <c r="A5" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="86"/>
-      <c r="C5" s="87"/>
-      <c r="D5" s="6" t="s">
+      <c r="B5" s="72"/>
+      <c r="C5" s="73"/>
+      <c r="D5" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="50">
         <v>76</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="G5" s="12"/>
+      <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:13" ht="15">
-      <c r="A6" s="88"/>
-      <c r="B6" s="89"/>
-      <c r="C6" s="90"/>
-      <c r="D6" s="9" t="s">
+      <c r="A6" s="74"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="76"/>
+      <c r="D6" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="E6" s="13"/>
-      <c r="F6" s="14" t="s">
+      <c r="E6" s="50"/>
+      <c r="F6" s="51" t="s">
         <v>14</v>
       </c>
-      <c r="G6" s="8"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:13" ht="15">
-      <c r="A7" s="79" t="s">
+      <c r="A7" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="80"/>
-      <c r="C7" s="81"/>
-      <c r="D7" s="6" t="s">
+      <c r="B7" s="69"/>
+      <c r="C7" s="70"/>
+      <c r="D7" s="50" t="s">
         <v>16</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="50">
         <v>1</v>
       </c>
-      <c r="F7" s="15"/>
-      <c r="G7" s="11"/>
+      <c r="F7" s="52"/>
+      <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:13" ht="15">
-      <c r="A8" s="82" t="s">
+      <c r="A8" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="83"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="9" t="s">
+      <c r="B8" s="69"/>
+      <c r="C8" s="70"/>
+      <c r="D8" s="50" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="50">
         <v>3</v>
       </c>
-      <c r="F8" s="10"/>
-      <c r="G8" s="11"/>
+      <c r="F8" s="52"/>
+      <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:13" ht="15">
-      <c r="A9" s="79" t="s">
+      <c r="A9" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="80"/>
-      <c r="C9" s="81"/>
-      <c r="D9" s="6" t="s">
+      <c r="B9" s="69"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="50" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="16"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="11"/>
-      <c r="I9" s="17"/>
+      <c r="E9" s="50"/>
+      <c r="F9" s="52"/>
+      <c r="G9" s="4"/>
+      <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:13" ht="15">
-      <c r="A10" s="82" t="s">
+      <c r="A10" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="83"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="9" t="s">
+      <c r="B10" s="69"/>
+      <c r="C10" s="70"/>
+      <c r="D10" s="50" t="s">
         <v>22</v>
       </c>
-      <c r="E10" s="13"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="19"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:13" ht="15">
-      <c r="A11" s="79" t="s">
+      <c r="A11" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="80"/>
-      <c r="C11" s="81"/>
-      <c r="D11" s="6" t="s">
+      <c r="B11" s="69"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="50" t="s">
         <v>24</v>
       </c>
-      <c r="E11" s="6">
+      <c r="E11" s="50">
         <v>1.01</v>
       </c>
-      <c r="F11" s="15"/>
-      <c r="G11" s="20"/>
-    </row>
-    <row r="12" spans="1:13" ht="18.75" customHeight="1"/>
-    <row r="13" spans="1:13" ht="24.75" customHeight="1">
-      <c r="A13" s="91" t="s">
+      <c r="F11" s="52"/>
+      <c r="G11" s="5"/>
+    </row>
+    <row r="12" spans="1:13" ht="18" customHeight="1"/>
+    <row r="13" spans="1:13" ht="26" customHeight="1">
+      <c r="A13" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="91" t="s">
+      <c r="B13" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="91" t="s">
+      <c r="C13" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="91" t="s">
+      <c r="D13" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="91" t="s">
+      <c r="E13" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="91" t="s">
+      <c r="F13" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="91" t="s">
+      <c r="G13" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" ht="24.75" customHeight="1" thickBot="1">
-      <c r="A14" s="92"/>
-      <c r="B14" s="92"/>
-      <c r="C14" s="92"/>
-      <c r="D14" s="92"/>
-      <c r="E14" s="92"/>
-      <c r="F14" s="92"/>
-      <c r="G14" s="92"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-    </row>
-    <row r="15" spans="1:13" thickBot="1">
-      <c r="A15" s="21">
+      <c r="H13" s="1"/>
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+    </row>
+    <row r="14" spans="1:13" ht="7" customHeight="1" thickBot="1">
+      <c r="A14" s="78"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="78"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1"/>
+      <c r="M14" s="1"/>
+    </row>
+    <row r="15" spans="1:13" ht="16" thickBot="1">
+      <c r="A15" s="6">
         <v>0.25</v>
       </c>
-      <c r="B15" s="22">
+      <c r="B15" s="7">
         <v>32</v>
       </c>
-      <c r="C15" s="56"/>
-      <c r="D15" s="57"/>
-      <c r="E15" s="58"/>
-      <c r="F15" s="22">
+      <c r="C15" s="25"/>
+      <c r="D15" s="26"/>
+      <c r="E15" s="27"/>
+      <c r="F15" s="7">
         <v>10.9</v>
       </c>
-      <c r="G15" s="56"/>
-    </row>
-    <row r="16" spans="1:13" thickBot="1">
-      <c r="A16" s="21">
+      <c r="G15" s="25"/>
+    </row>
+    <row r="16" spans="1:13" ht="16" thickBot="1">
+      <c r="A16" s="6">
         <v>0.5</v>
       </c>
-      <c r="B16" s="22">
+      <c r="B16" s="7">
         <v>30</v>
       </c>
-      <c r="C16" s="59"/>
-      <c r="D16" s="60"/>
-      <c r="E16" s="61"/>
-      <c r="F16" s="22">
+      <c r="C16" s="28"/>
+      <c r="D16" s="29"/>
+      <c r="E16" s="30"/>
+      <c r="F16" s="7">
         <v>11.2</v>
       </c>
-      <c r="G16" s="59"/>
-    </row>
-    <row r="17" spans="1:7" thickBot="1">
-      <c r="A17" s="21">
+      <c r="G16" s="28"/>
+    </row>
+    <row r="17" spans="1:7" ht="16" thickBot="1">
+      <c r="A17" s="6">
         <v>1</v>
       </c>
-      <c r="B17" s="22">
+      <c r="B17" s="7">
         <v>27</v>
       </c>
-      <c r="C17" s="59"/>
-      <c r="D17" s="60"/>
-      <c r="E17" s="61"/>
-      <c r="F17" s="22">
+      <c r="C17" s="28"/>
+      <c r="D17" s="29"/>
+      <c r="E17" s="30"/>
+      <c r="F17" s="7">
         <v>11.7</v>
       </c>
-      <c r="G17" s="59"/>
-    </row>
-    <row r="18" spans="1:7" thickBot="1">
-      <c r="A18" s="21">
+      <c r="G17" s="28"/>
+    </row>
+    <row r="18" spans="1:7" ht="16" thickBot="1">
+      <c r="A18" s="6">
         <v>2</v>
       </c>
-      <c r="B18" s="22">
+      <c r="B18" s="7">
         <v>24</v>
       </c>
-      <c r="C18" s="59"/>
-      <c r="D18" s="60"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="22">
+      <c r="C18" s="28"/>
+      <c r="D18" s="29"/>
+      <c r="E18" s="30"/>
+      <c r="F18" s="7">
         <v>12.2</v>
       </c>
-      <c r="G18" s="59"/>
-    </row>
-    <row r="19" spans="1:7" thickBot="1">
-      <c r="A19" s="21">
+      <c r="G18" s="28"/>
+    </row>
+    <row r="19" spans="1:7" ht="16" thickBot="1">
+      <c r="A19" s="6">
         <v>4</v>
       </c>
-      <c r="B19" s="22">
+      <c r="B19" s="7">
         <v>22</v>
       </c>
-      <c r="C19" s="59"/>
-      <c r="D19" s="60"/>
-      <c r="E19" s="61"/>
-      <c r="F19" s="22">
+      <c r="C19" s="28"/>
+      <c r="D19" s="29"/>
+      <c r="E19" s="30"/>
+      <c r="F19" s="7">
         <v>12.5</v>
       </c>
-      <c r="G19" s="59"/>
-    </row>
-    <row r="20" spans="1:7" thickBot="1">
-      <c r="A20" s="21">
+      <c r="G19" s="28"/>
+    </row>
+    <row r="20" spans="1:7" ht="16" thickBot="1">
+      <c r="A20" s="6">
         <v>8</v>
       </c>
-      <c r="B20" s="22">
+      <c r="B20" s="7">
         <v>20</v>
       </c>
-      <c r="C20" s="59"/>
-      <c r="D20" s="60"/>
-      <c r="E20" s="61"/>
-      <c r="F20" s="22">
+      <c r="C20" s="28"/>
+      <c r="D20" s="29"/>
+      <c r="E20" s="30"/>
+      <c r="F20" s="7">
         <v>12.9</v>
       </c>
-      <c r="G20" s="59"/>
-    </row>
-    <row r="21" spans="1:7" thickBot="1">
-      <c r="A21" s="21">
+      <c r="G20" s="28"/>
+    </row>
+    <row r="21" spans="1:7" ht="16" thickBot="1">
+      <c r="A21" s="6">
         <v>15</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="7">
         <v>17</v>
       </c>
-      <c r="C21" s="59"/>
-      <c r="D21" s="60"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="22">
+      <c r="C21" s="28"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="7">
         <v>13.3</v>
       </c>
-      <c r="G21" s="59"/>
-    </row>
-    <row r="22" spans="1:7" thickBot="1">
-      <c r="A22" s="21">
+      <c r="G21" s="28"/>
+    </row>
+    <row r="22" spans="1:7" ht="16" thickBot="1">
+      <c r="A22" s="6">
         <v>30</v>
       </c>
-      <c r="B22" s="22">
+      <c r="B22" s="7">
         <v>15</v>
       </c>
-      <c r="C22" s="59"/>
-      <c r="D22" s="60"/>
-      <c r="E22" s="61"/>
-      <c r="F22" s="22">
+      <c r="C22" s="28"/>
+      <c r="D22" s="29"/>
+      <c r="E22" s="30"/>
+      <c r="F22" s="7">
         <v>13.7</v>
       </c>
-      <c r="G22" s="59"/>
-    </row>
-    <row r="23" spans="1:7" thickBot="1">
-      <c r="A23" s="21">
+      <c r="G22" s="28"/>
+    </row>
+    <row r="23" spans="1:7" ht="16" thickBot="1">
+      <c r="A23" s="6">
         <v>60</v>
       </c>
-      <c r="B23" s="22">
+      <c r="B23" s="7">
         <v>13</v>
       </c>
-      <c r="C23" s="59"/>
-      <c r="D23" s="60"/>
-      <c r="E23" s="61"/>
-      <c r="F23" s="22">
+      <c r="C23" s="28"/>
+      <c r="D23" s="29"/>
+      <c r="E23" s="30"/>
+      <c r="F23" s="7">
         <v>14</v>
       </c>
-      <c r="G23" s="59"/>
-    </row>
-    <row r="24" spans="1:7" thickBot="1">
-      <c r="A24" s="21">
+      <c r="G23" s="28"/>
+    </row>
+    <row r="24" spans="1:7" ht="16" thickBot="1">
+      <c r="A24" s="6">
         <v>787</v>
       </c>
-      <c r="B24" s="22">
+      <c r="B24" s="7">
         <v>9</v>
       </c>
-      <c r="C24" s="59"/>
-      <c r="D24" s="60"/>
-      <c r="E24" s="61"/>
-      <c r="F24" s="22">
+      <c r="C24" s="28"/>
+      <c r="D24" s="29"/>
+      <c r="E24" s="30"/>
+      <c r="F24" s="7">
         <v>14.7</v>
       </c>
-      <c r="G24" s="59"/>
-    </row>
-    <row r="25" spans="1:7" thickBot="1">
-      <c r="A25" s="21">
+      <c r="G24" s="28"/>
+    </row>
+    <row r="25" spans="1:7" ht="16" thickBot="1">
+      <c r="A25" s="6">
         <v>1459</v>
       </c>
-      <c r="B25" s="22">
+      <c r="B25" s="7">
         <v>8</v>
       </c>
-      <c r="C25" s="59"/>
-      <c r="D25" s="60"/>
-      <c r="E25" s="61"/>
-      <c r="F25" s="22">
+      <c r="C25" s="28"/>
+      <c r="D25" s="29"/>
+      <c r="E25" s="30"/>
+      <c r="F25" s="7">
         <v>14.8</v>
       </c>
-      <c r="G25" s="59"/>
+      <c r="G25" s="28"/>
     </row>
     <row r="26" spans="1:7" ht="15">
-      <c r="A26" s="23"/>
-      <c r="B26" s="23"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="25"/>
-      <c r="E26" s="24"/>
-      <c r="F26" s="23"/>
-      <c r="G26" s="24"/>
+      <c r="A26" s="8"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="9"/>
+      <c r="F26" s="8"/>
+      <c r="G26" s="9"/>
     </row>
     <row r="27" spans="1:7" ht="15">
-      <c r="A27" s="23"/>
-      <c r="B27" s="23"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="25"/>
-      <c r="E27" s="24"/>
-      <c r="F27" s="23"/>
-      <c r="G27" s="24"/>
+      <c r="A27" s="8"/>
+      <c r="B27" s="8"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="10"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="9"/>
     </row>
     <row r="28" spans="1:7" ht="15">
-      <c r="A28" s="23"/>
-      <c r="B28" s="23"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="24"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="24"/>
+      <c r="A28" s="8"/>
+      <c r="B28" s="8"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="10"/>
+      <c r="E28" s="9"/>
+      <c r="F28" s="8"/>
+      <c r="G28" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="17">
@@ -1863,521 +1903,515 @@
   </sheetPr>
   <dimension ref="A1:G35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" customWidth="1"/>
-    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" style="55" customWidth="1"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="39" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="39" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="12.75">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:7" ht="17" customHeight="1">
+      <c r="A1" s="42" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="43" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="42" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="26" t="s">
+      <c r="D1" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="26" t="s">
+      <c r="E1" s="43" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="72" t="s">
+      <c r="F1" s="43" t="s">
         <v>83</v>
       </c>
-      <c r="G1" s="72" t="s">
+      <c r="G1" s="43" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="12.75">
-      <c r="A2" s="28">
+    <row r="2" spans="1:7" ht="13">
+      <c r="A2" s="40">
         <v>1124</v>
       </c>
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="28">
+      <c r="C2" s="40">
         <v>7</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="74"/>
-      <c r="G2" s="75"/>
-    </row>
-    <row r="3" spans="1:7" ht="12.75">
-      <c r="A3" s="28">
+      <c r="D2" s="47"/>
+      <c r="E2" s="47"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="41"/>
+    </row>
+    <row r="3" spans="1:7" ht="13">
+      <c r="A3" s="40">
         <v>1107</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="B3" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="28">
+      <c r="C3" s="40">
         <v>5</v>
       </c>
-      <c r="D3" s="28"/>
-      <c r="E3" s="28"/>
-      <c r="F3" s="74"/>
-      <c r="G3" s="74"/>
-    </row>
-    <row r="4" spans="1:7" ht="12.75">
-      <c r="A4" s="28">
+      <c r="D3" s="47"/>
+      <c r="E3" s="47"/>
+      <c r="F3" s="40"/>
+      <c r="G3" s="40"/>
+    </row>
+    <row r="4" spans="1:7" ht="13">
+      <c r="A4" s="40">
         <v>1163</v>
       </c>
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="40">
         <v>7</v>
       </c>
-      <c r="D4" s="28"/>
-      <c r="E4" s="28"/>
-      <c r="F4" s="74"/>
-      <c r="G4" s="74"/>
-    </row>
-    <row r="5" spans="1:7" ht="12.75">
-      <c r="A5" s="28">
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="40"/>
+      <c r="G4" s="40"/>
+    </row>
+    <row r="5" spans="1:7" ht="13">
+      <c r="A5" s="40">
         <v>1182</v>
       </c>
-      <c r="B5" s="29" t="s">
+      <c r="B5" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="28">
+      <c r="C5" s="40">
         <v>3</v>
       </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="28"/>
-      <c r="F5" s="74"/>
-      <c r="G5" s="74"/>
-    </row>
-    <row r="6" spans="1:7" ht="12.75">
-      <c r="A6" s="28">
+      <c r="D5" s="47"/>
+      <c r="E5" s="47"/>
+      <c r="F5" s="40"/>
+      <c r="G5" s="40"/>
+    </row>
+    <row r="6" spans="1:7" ht="13">
+      <c r="A6" s="40">
         <v>1175</v>
       </c>
-      <c r="B6" s="29" t="s">
+      <c r="B6" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C6" s="40">
         <v>15</v>
       </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="28"/>
-      <c r="F6" s="74"/>
-      <c r="G6" s="75"/>
-    </row>
-    <row r="7" spans="1:7" ht="12.75">
-      <c r="A7" s="28">
+      <c r="D6" s="47"/>
+      <c r="E6" s="47"/>
+      <c r="F6" s="40"/>
+      <c r="G6" s="41"/>
+    </row>
+    <row r="7" spans="1:7" ht="13">
+      <c r="A7" s="40">
         <v>1049</v>
       </c>
-      <c r="B7" s="29" t="s">
+      <c r="B7" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C7" s="28">
+      <c r="C7" s="40">
         <v>8</v>
       </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="28"/>
-      <c r="F7" s="74"/>
-      <c r="G7" s="75"/>
-    </row>
-    <row r="8" spans="1:7" ht="12.75">
-      <c r="A8" s="28">
+      <c r="D7" s="47"/>
+      <c r="E7" s="47"/>
+      <c r="F7" s="40"/>
+      <c r="G7" s="41"/>
+    </row>
+    <row r="8" spans="1:7" ht="13">
+      <c r="A8" s="40">
         <v>1006</v>
       </c>
-      <c r="B8" s="29" t="s">
+      <c r="B8" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C8" s="28">
+      <c r="C8" s="40">
         <v>9</v>
       </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="74"/>
-      <c r="G8" s="75"/>
-    </row>
-    <row r="9" spans="1:7" ht="12.75">
-      <c r="A9" s="28">
+      <c r="D8" s="47"/>
+      <c r="E8" s="47"/>
+      <c r="F8" s="40"/>
+      <c r="G8" s="41"/>
+    </row>
+    <row r="9" spans="1:7" ht="13">
+      <c r="A9" s="40">
         <v>1129</v>
       </c>
-      <c r="B9" s="29" t="s">
+      <c r="B9" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="28">
+      <c r="C9" s="40">
         <v>1</v>
       </c>
-      <c r="D9" s="28"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="74"/>
-      <c r="G9" s="75"/>
-    </row>
-    <row r="10" spans="1:7" ht="12.75">
-      <c r="A10" s="28">
+      <c r="D9" s="47"/>
+      <c r="E9" s="47"/>
+      <c r="F9" s="40"/>
+      <c r="G9" s="41"/>
+    </row>
+    <row r="10" spans="1:7" ht="13">
+      <c r="A10" s="40">
         <v>1236</v>
       </c>
-      <c r="B10" s="29" t="s">
+      <c r="B10" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="40">
         <v>2</v>
       </c>
-      <c r="D10" s="28"/>
-      <c r="E10" s="28"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="75"/>
-    </row>
-    <row r="11" spans="1:7" ht="12.75">
-      <c r="A11" s="28">
+      <c r="D10" s="47"/>
+      <c r="E10" s="47"/>
+      <c r="F10" s="40"/>
+      <c r="G10" s="41"/>
+    </row>
+    <row r="11" spans="1:7" ht="13">
+      <c r="A11" s="40">
         <v>1041</v>
       </c>
-      <c r="B11" s="29" t="s">
+      <c r="B11" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C11" s="28">
+      <c r="C11" s="40">
         <v>20</v>
       </c>
-      <c r="D11" s="28"/>
-      <c r="E11" s="28"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="75"/>
-    </row>
-    <row r="12" spans="1:7" ht="12.75">
-      <c r="A12" s="28">
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="40"/>
+      <c r="G11" s="41"/>
+    </row>
+    <row r="12" spans="1:7" ht="13">
+      <c r="A12" s="40">
         <v>1016</v>
       </c>
-      <c r="B12" s="29" t="s">
+      <c r="B12" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C12" s="28">
+      <c r="C12" s="40">
         <v>1</v>
       </c>
-      <c r="D12" s="28"/>
-      <c r="E12" s="28"/>
-      <c r="F12" s="74"/>
-      <c r="G12" s="75"/>
-    </row>
-    <row r="13" spans="1:7" ht="12.75">
-      <c r="A13" s="28">
+      <c r="D12" s="47"/>
+      <c r="E12" s="47"/>
+      <c r="F12" s="40"/>
+      <c r="G12" s="41"/>
+    </row>
+    <row r="13" spans="1:7" ht="13">
+      <c r="A13" s="40">
         <v>1195</v>
       </c>
-      <c r="B13" s="29" t="s">
+      <c r="B13" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="28">
+      <c r="C13" s="40">
         <v>1</v>
       </c>
-      <c r="D13" s="28"/>
-      <c r="E13" s="28"/>
-      <c r="F13" s="74"/>
-      <c r="G13" s="75"/>
-    </row>
-    <row r="14" spans="1:7" ht="12.75">
-      <c r="A14" s="28">
+      <c r="D13" s="47"/>
+      <c r="E13" s="47"/>
+      <c r="F13" s="40"/>
+      <c r="G13" s="41"/>
+    </row>
+    <row r="14" spans="1:7" ht="13">
+      <c r="A14" s="40">
         <v>1072</v>
       </c>
-      <c r="B14" s="29" t="s">
+      <c r="B14" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="28">
+      <c r="C14" s="40">
         <v>1</v>
       </c>
-      <c r="D14" s="28"/>
-      <c r="E14" s="28"/>
-      <c r="F14" s="74"/>
-      <c r="G14" s="75"/>
-    </row>
-    <row r="15" spans="1:7" ht="12.75">
-      <c r="A15" s="28">
+      <c r="D14" s="47"/>
+      <c r="E14" s="47"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="41"/>
+    </row>
+    <row r="15" spans="1:7" ht="13">
+      <c r="A15" s="40">
         <v>1073</v>
       </c>
-      <c r="B15" s="29" t="s">
+      <c r="B15" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C15" s="28">
+      <c r="C15" s="40">
         <v>2</v>
       </c>
-      <c r="D15" s="28"/>
-      <c r="E15" s="28"/>
-      <c r="F15" s="74"/>
-      <c r="G15" s="75"/>
-    </row>
-    <row r="16" spans="1:7" ht="12.75">
-      <c r="A16" s="28">
+      <c r="D15" s="47"/>
+      <c r="E15" s="47"/>
+      <c r="F15" s="40"/>
+      <c r="G15" s="41"/>
+    </row>
+    <row r="16" spans="1:7" ht="13">
+      <c r="A16" s="40">
         <v>1101</v>
       </c>
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="C16" s="28">
+      <c r="C16" s="40">
         <v>10</v>
       </c>
-      <c r="D16" s="28"/>
-      <c r="E16" s="28"/>
-      <c r="F16" s="74"/>
-      <c r="G16" s="75"/>
-    </row>
-    <row r="17" spans="1:7" ht="12.75">
-      <c r="A17" s="28">
+      <c r="D16" s="47"/>
+      <c r="E16" s="47"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="41"/>
+    </row>
+    <row r="17" spans="1:7" ht="13">
+      <c r="A17" s="40">
         <v>1026</v>
       </c>
-      <c r="B17" s="29" t="s">
+      <c r="B17" s="40" t="s">
         <v>42</v>
       </c>
-      <c r="C17" s="28">
+      <c r="C17" s="40">
         <v>5</v>
       </c>
-      <c r="D17" s="28"/>
-      <c r="E17" s="28"/>
-      <c r="F17" s="74"/>
-      <c r="G17" s="75"/>
-    </row>
-    <row r="18" spans="1:7" ht="12.75">
-      <c r="A18" s="28">
+      <c r="D17" s="47"/>
+      <c r="E17" s="47"/>
+      <c r="F17" s="40"/>
+      <c r="G17" s="41"/>
+    </row>
+    <row r="18" spans="1:7" ht="13">
+      <c r="A18" s="40">
         <v>1040</v>
       </c>
-      <c r="B18" s="29" t="s">
+      <c r="B18" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="28">
+      <c r="C18" s="40">
         <v>15</v>
       </c>
-      <c r="D18" s="28"/>
-      <c r="E18" s="28"/>
-      <c r="F18" s="74"/>
-      <c r="G18" s="75"/>
-    </row>
-    <row r="19" spans="1:7" ht="12.75">
-      <c r="A19" s="28">
+      <c r="D18" s="47"/>
+      <c r="E18" s="47"/>
+      <c r="F18" s="40"/>
+      <c r="G18" s="41"/>
+    </row>
+    <row r="19" spans="1:7" ht="13">
+      <c r="A19" s="40">
         <v>1126</v>
       </c>
-      <c r="B19" s="29" t="s">
+      <c r="B19" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="28">
+      <c r="C19" s="40">
         <v>8</v>
       </c>
-      <c r="D19" s="28"/>
-      <c r="E19" s="28"/>
-      <c r="F19" s="74"/>
-      <c r="G19" s="75"/>
-    </row>
-    <row r="20" spans="1:7" ht="12.75">
-      <c r="A20" s="28">
+      <c r="D19" s="47"/>
+      <c r="E19" s="47"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="41"/>
+    </row>
+    <row r="20" spans="1:7" ht="13">
+      <c r="A20" s="40">
         <v>1181</v>
       </c>
-      <c r="B20" s="29" t="s">
+      <c r="B20" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="28">
+      <c r="C20" s="40">
         <v>11</v>
       </c>
-      <c r="D20" s="28"/>
-      <c r="E20" s="28"/>
-      <c r="F20" s="74"/>
-      <c r="G20" s="75"/>
-    </row>
-    <row r="21" spans="1:7" ht="12.75">
-      <c r="A21" s="28">
+      <c r="D20" s="47"/>
+      <c r="E20" s="47"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="41"/>
+    </row>
+    <row r="21" spans="1:7" ht="13">
+      <c r="A21" s="40">
         <v>1002</v>
       </c>
-      <c r="B21" s="29" t="s">
+      <c r="B21" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="28">
+      <c r="C21" s="40">
         <v>2</v>
       </c>
-      <c r="D21" s="28"/>
-      <c r="E21" s="28"/>
-      <c r="F21" s="74"/>
-      <c r="G21" s="75"/>
-    </row>
-    <row r="22" spans="1:7" ht="12.75">
-      <c r="A22" s="28">
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="41"/>
+    </row>
+    <row r="22" spans="1:7" ht="13">
+      <c r="A22" s="40">
         <v>1166</v>
       </c>
-      <c r="B22" s="29" t="s">
+      <c r="B22" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C22" s="28">
+      <c r="C22" s="40">
         <v>10</v>
       </c>
-      <c r="D22" s="28"/>
-      <c r="E22" s="28"/>
-      <c r="F22" s="74"/>
-      <c r="G22" s="75"/>
-    </row>
-    <row r="23" spans="1:7" ht="12.75">
-      <c r="A23" s="28">
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="40"/>
+      <c r="G22" s="41"/>
+    </row>
+    <row r="23" spans="1:7" ht="13">
+      <c r="A23" s="40">
         <v>1248</v>
       </c>
-      <c r="B23" s="29" t="s">
+      <c r="B23" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="C23" s="28">
+      <c r="C23" s="40">
         <v>10</v>
       </c>
-      <c r="D23" s="28"/>
-      <c r="E23" s="28"/>
-      <c r="F23" s="74"/>
-      <c r="G23" s="75"/>
-    </row>
-    <row r="24" spans="1:7" ht="12.75">
-      <c r="A24" s="28">
+      <c r="D23" s="47"/>
+      <c r="E23" s="47"/>
+      <c r="F23" s="40"/>
+      <c r="G23" s="41"/>
+    </row>
+    <row r="24" spans="1:7" ht="13">
+      <c r="A24" s="40">
         <v>1138</v>
       </c>
-      <c r="B24" s="29" t="s">
+      <c r="B24" s="40" t="s">
         <v>43</v>
       </c>
-      <c r="C24" s="28">
+      <c r="C24" s="40">
         <v>1</v>
       </c>
-      <c r="D24" s="28"/>
-      <c r="E24" s="28"/>
-      <c r="F24" s="74"/>
-      <c r="G24" s="75"/>
-    </row>
-    <row r="25" spans="1:7" ht="12.75">
-      <c r="A25" s="28">
+      <c r="D24" s="47"/>
+      <c r="E24" s="47"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="41"/>
+    </row>
+    <row r="25" spans="1:7" ht="13">
+      <c r="A25" s="40">
         <v>1256</v>
       </c>
-      <c r="B25" s="29" t="s">
+      <c r="B25" s="40" t="s">
         <v>37</v>
       </c>
-      <c r="C25" s="28">
+      <c r="C25" s="40">
         <v>1</v>
       </c>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="74"/>
-      <c r="G25" s="75"/>
-    </row>
-    <row r="26" spans="1:7" ht="12.75">
-      <c r="A26" s="28">
+      <c r="D25" s="47"/>
+      <c r="E25" s="47"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="41"/>
+    </row>
+    <row r="26" spans="1:7" ht="13">
+      <c r="A26" s="40">
         <v>1011</v>
       </c>
-      <c r="B26" s="29" t="s">
+      <c r="B26" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C26" s="28">
+      <c r="C26" s="40">
         <v>2</v>
       </c>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="74"/>
-      <c r="G26" s="75"/>
-    </row>
-    <row r="27" spans="1:7" ht="12.75">
-      <c r="A27" s="28">
+      <c r="D26" s="47"/>
+      <c r="E26" s="47"/>
+      <c r="F26" s="40"/>
+      <c r="G26" s="41"/>
+    </row>
+    <row r="27" spans="1:7" ht="13">
+      <c r="A27" s="40">
         <v>1163</v>
       </c>
-      <c r="B27" s="29" t="s">
+      <c r="B27" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C27" s="28">
+      <c r="C27" s="40">
         <v>11</v>
       </c>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="74"/>
-      <c r="G27" s="75"/>
-    </row>
-    <row r="28" spans="1:7" ht="12.75">
-      <c r="A28" s="28">
+      <c r="D27" s="47"/>
+      <c r="E27" s="47"/>
+      <c r="F27" s="40"/>
+      <c r="G27" s="41"/>
+    </row>
+    <row r="28" spans="1:7" ht="13">
+      <c r="A28" s="40">
         <v>1002</v>
       </c>
-      <c r="B28" s="29" t="s">
+      <c r="B28" s="40" t="s">
         <v>40</v>
       </c>
-      <c r="C28" s="28">
+      <c r="C28" s="40">
         <v>15</v>
       </c>
-      <c r="D28" s="28"/>
-      <c r="E28" s="28"/>
-      <c r="F28" s="74"/>
-      <c r="G28" s="75"/>
-    </row>
-    <row r="29" spans="1:7" ht="12.75">
-      <c r="A29" s="28">
+      <c r="D28" s="47"/>
+      <c r="E28" s="47"/>
+      <c r="F28" s="40"/>
+      <c r="G28" s="41"/>
+    </row>
+    <row r="29" spans="1:7" ht="13">
+      <c r="A29" s="40">
         <v>1078</v>
       </c>
-      <c r="B29" s="29" t="s">
+      <c r="B29" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="C29" s="28">
+      <c r="C29" s="40">
         <v>4</v>
       </c>
-      <c r="D29" s="28"/>
-      <c r="E29" s="28"/>
-      <c r="F29" s="74"/>
-      <c r="G29" s="75"/>
-    </row>
-    <row r="30" spans="1:7" ht="12.75">
-      <c r="A30" s="28">
+      <c r="D29" s="47"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="40"/>
+      <c r="G29" s="41"/>
+    </row>
+    <row r="30" spans="1:7" ht="13">
+      <c r="A30" s="40">
         <v>1058</v>
       </c>
-      <c r="B30" s="29" t="s">
+      <c r="B30" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C30" s="28">
+      <c r="C30" s="40">
         <v>3</v>
       </c>
-      <c r="D30" s="28"/>
-      <c r="E30" s="28"/>
-      <c r="F30" s="74"/>
-      <c r="G30" s="75"/>
-    </row>
-    <row r="31" spans="1:7" ht="12.75">
-      <c r="A31" s="28">
+      <c r="D30" s="47"/>
+      <c r="E30" s="47"/>
+      <c r="F30" s="40"/>
+      <c r="G30" s="41"/>
+    </row>
+    <row r="31" spans="1:7" ht="13">
+      <c r="A31" s="40">
         <v>1135</v>
       </c>
-      <c r="B31" s="29" t="s">
+      <c r="B31" s="40" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="28">
+      <c r="C31" s="40">
         <v>3</v>
       </c>
-      <c r="D31" s="28"/>
-      <c r="E31" s="28"/>
-      <c r="F31" s="74"/>
-      <c r="G31" s="75"/>
-    </row>
-    <row r="33" spans="4:6" ht="12.75">
-      <c r="D33" s="73" t="s">
+      <c r="D31" s="47"/>
+      <c r="E31" s="47"/>
+      <c r="F31" s="40"/>
+      <c r="G31" s="41"/>
+    </row>
+    <row r="33" spans="4:5" ht="13">
+      <c r="D33" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="E33" s="31"/>
-      <c r="F33" s="71"/>
-    </row>
-    <row r="34" spans="4:6" ht="15.75" customHeight="1">
-      <c r="D34" s="73" t="s">
+      <c r="E33" s="45"/>
+    </row>
+    <row r="34" spans="4:5" ht="15.75" customHeight="1">
+      <c r="D34" s="44" t="s">
         <v>86</v>
       </c>
-      <c r="E34" s="31"/>
-      <c r="F34" s="71"/>
-    </row>
-    <row r="35" spans="4:6" ht="15.75" customHeight="1">
-      <c r="D35" s="30" t="s">
+      <c r="E34" s="45"/>
+    </row>
+    <row r="35" spans="4:5" ht="15.75" customHeight="1">
+      <c r="D35" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="E35" s="31"/>
-      <c r="F35" s="71"/>
+      <c r="E35" s="45"/>
     </row>
   </sheetData>
   <phoneticPr fontId="22" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
-  <tableParts count="1">
-    <tablePart r:id="rId2"/>
-  </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
@@ -2400,82 +2434,82 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView showGridLines="0" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
-      <c r="A1" s="93" t="s">
+    <row r="1" spans="1:3" ht="17" customHeight="1">
+      <c r="A1" s="79" t="s">
         <v>45</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" s="32" t="s">
+      <c r="B1" s="80"/>
+      <c r="C1" s="80"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A2" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="94"/>
-      <c r="C2" s="81"/>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" s="33" t="s">
+      <c r="B2" s="81"/>
+      <c r="C2" s="82"/>
+    </row>
+    <row r="3" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A3" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34" t="s">
+      <c r="B3" s="59"/>
+      <c r="C3" s="48" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
-      <c r="A4" s="32" t="s">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A4" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="C4" s="35" t="s">
+      <c r="B4" s="60"/>
+      <c r="C4" s="58" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
-      <c r="A5" s="33" t="s">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A5" s="48" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="36"/>
-      <c r="C5" s="34" t="s">
+      <c r="B5" s="61"/>
+      <c r="C5" s="48" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="32" t="s">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A6" s="58" t="s">
         <v>53</v>
       </c>
-      <c r="B6" s="37"/>
-      <c r="C6" s="35" t="s">
+      <c r="B6" s="62"/>
+      <c r="C6" s="58" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="33" t="s">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A7" s="48" t="s">
         <v>55</v>
       </c>
-      <c r="B7" s="38"/>
-      <c r="C7" s="39" t="s">
+      <c r="B7" s="63"/>
+      <c r="C7" s="49" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="32" t="s">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1">
+      <c r="A8" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="95"/>
-      <c r="C8" s="81"/>
+      <c r="B8" s="83"/>
+      <c r="C8" s="82"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2491,436 +2525,434 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{606274E6-D00F-4C5B-960E-02503400C7A7}">
   <dimension ref="A1:G40"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
+    <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="62" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" style="62" customWidth="1"/>
-    <col min="3" max="6" width="8" style="62" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" style="62" customWidth="1"/>
-    <col min="8" max="16384" width="12.5703125" style="62"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="3" max="6" width="8" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1">
-      <c r="A1" s="70" t="s">
+      <c r="A1" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="B1" s="63"/>
-      <c r="C1" s="63"/>
-      <c r="D1" s="63"/>
-      <c r="E1" s="63"/>
-      <c r="F1" s="63"/>
-      <c r="G1" s="63"/>
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="E1" s="31"/>
+      <c r="F1" s="31"/>
+      <c r="G1" s="31"/>
     </row>
     <row r="2" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A2" s="66"/>
-      <c r="B2" s="63"/>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="31"/>
+      <c r="C2" s="31"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
+      <c r="G2" s="31"/>
     </row>
     <row r="3" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A3" s="63"/>
-      <c r="B3" s="63"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
+      <c r="A3" s="31"/>
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A4" s="65" t="s">
+      <c r="A4" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="B4" s="69">
+      <c r="B4" s="37">
         <v>5000</v>
       </c>
-      <c r="C4" s="63" t="s">
+      <c r="C4" s="31" t="s">
         <v>80</v>
       </c>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="69">
+      <c r="B5" s="37">
         <f>10*10^6</f>
         <v>10000000</v>
       </c>
-      <c r="C5" s="63" t="s">
+      <c r="C5" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A6" s="65" t="s">
+      <c r="A6" s="33" t="s">
         <v>78</v>
       </c>
-      <c r="B6" s="69">
+      <c r="B6" s="37">
         <v>144</v>
       </c>
-      <c r="C6" s="63" t="s">
+      <c r="C6" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="31"/>
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A7" s="65" t="s">
+      <c r="A7" s="33" t="s">
         <v>77</v>
       </c>
-      <c r="B7" s="69">
+      <c r="B7" s="37">
         <v>48</v>
       </c>
-      <c r="C7" s="63" t="s">
+      <c r="C7" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="63"/>
-      <c r="E7" s="63"/>
-      <c r="F7" s="63"/>
-      <c r="G7" s="63"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
+      <c r="G7" s="31"/>
     </row>
     <row r="8" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="33" t="s">
         <v>76</v>
       </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="63"/>
-      <c r="D8" s="63"/>
-      <c r="E8" s="63"/>
-      <c r="F8" s="63"/>
-      <c r="G8" s="63"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="31"/>
+      <c r="D8" s="31"/>
+      <c r="E8" s="31"/>
+      <c r="F8" s="31"/>
+      <c r="G8" s="31"/>
     </row>
     <row r="9" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A9" s="65" t="s">
+      <c r="A9" s="33" t="s">
         <v>75</v>
       </c>
-      <c r="B9" s="69">
+      <c r="B9" s="37">
         <v>2</v>
       </c>
-      <c r="C9" s="63" t="s">
+      <c r="C9" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="63"/>
-      <c r="E9" s="63"/>
-      <c r="F9" s="63"/>
-      <c r="G9" s="63"/>
+      <c r="D9" s="31"/>
+      <c r="E9" s="31"/>
+      <c r="F9" s="31"/>
+      <c r="G9" s="31"/>
     </row>
     <row r="10" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="B10" s="69">
+      <c r="B10" s="37">
         <v>4</v>
       </c>
-      <c r="C10" s="63" t="s">
+      <c r="C10" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="D10" s="63"/>
-      <c r="E10" s="63"/>
-      <c r="F10" s="63"/>
-      <c r="G10" s="63"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A11" s="65" t="s">
+      <c r="A11" s="33" t="s">
         <v>73</v>
       </c>
-      <c r="B11" s="64"/>
-      <c r="C11" s="63" t="s">
+      <c r="B11" s="32"/>
+      <c r="C11" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="D11" s="63"/>
-      <c r="E11" s="63"/>
-      <c r="F11" s="63"/>
-      <c r="G11" s="63"/>
+      <c r="D11" s="31"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="31"/>
     </row>
     <row r="12" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A12" s="63"/>
-      <c r="B12" s="63"/>
-      <c r="C12" s="63"/>
-      <c r="D12" s="63"/>
-      <c r="E12" s="63"/>
-      <c r="F12" s="63"/>
-      <c r="G12" s="63"/>
+      <c r="A12" s="31"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="31"/>
+      <c r="D12" s="31"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="31"/>
     </row>
     <row r="13" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A13" s="65" t="s">
+      <c r="A13" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="B13" s="64"/>
-      <c r="C13" s="63" t="s">
+      <c r="B13" s="32"/>
+      <c r="C13" s="31" t="s">
         <v>71</v>
       </c>
-      <c r="D13" s="63"/>
-      <c r="E13" s="63"/>
-      <c r="F13" s="63"/>
-      <c r="G13" s="63"/>
+      <c r="D13" s="31"/>
+      <c r="E13" s="31"/>
+      <c r="F13" s="31"/>
+      <c r="G13" s="31"/>
     </row>
     <row r="14" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A14" s="65" t="s">
+      <c r="A14" s="33" t="s">
         <v>70</v>
       </c>
-      <c r="B14" s="64"/>
-      <c r="C14" s="63"/>
-      <c r="D14" s="63"/>
-      <c r="E14" s="63"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="63"/>
+      <c r="B14" s="32"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="31"/>
+      <c r="F14" s="36"/>
+      <c r="G14" s="31"/>
     </row>
     <row r="15" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A15" s="65" t="s">
+      <c r="A15" s="33" t="s">
         <v>69</v>
       </c>
-      <c r="B15" s="64"/>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="67"/>
-      <c r="G15" s="63"/>
+      <c r="B15" s="32"/>
+      <c r="C15" s="31"/>
+      <c r="D15" s="31"/>
+      <c r="E15" s="31"/>
+      <c r="F15" s="35"/>
+      <c r="G15" s="31"/>
     </row>
     <row r="16" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A16" s="65" t="s">
+      <c r="A16" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="B16" s="64"/>
-      <c r="C16" s="63" t="s">
+      <c r="B16" s="32"/>
+      <c r="C16" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="D16" s="63"/>
-      <c r="E16" s="63"/>
-      <c r="F16" s="63"/>
-      <c r="G16" s="63"/>
+      <c r="D16" s="31"/>
+      <c r="E16" s="31"/>
+      <c r="F16" s="31"/>
+      <c r="G16" s="31"/>
     </row>
     <row r="17" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A17" s="63"/>
-      <c r="B17" s="63"/>
-      <c r="C17" s="63"/>
-      <c r="D17" s="63"/>
-      <c r="E17" s="63"/>
-      <c r="F17" s="63"/>
-      <c r="G17" s="63"/>
+      <c r="A17" s="31"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="31"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="31"/>
+      <c r="G17" s="31"/>
     </row>
     <row r="18" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A18" s="63"/>
-      <c r="B18" s="63"/>
-      <c r="C18" s="63"/>
-      <c r="D18" s="63"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="63"/>
-      <c r="G18" s="63"/>
+      <c r="A18" s="31"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
     </row>
     <row r="19" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A19" s="63"/>
-      <c r="B19" s="63"/>
-      <c r="C19" s="63"/>
-      <c r="D19" s="63"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="63"/>
-      <c r="G19" s="63"/>
+      <c r="A19" s="31"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="31"/>
+      <c r="E19" s="31"/>
+      <c r="F19" s="31"/>
+      <c r="G19" s="31"/>
     </row>
     <row r="20" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A20" s="63"/>
-      <c r="B20" s="63"/>
-      <c r="C20" s="63"/>
-      <c r="D20" s="63"/>
-      <c r="E20" s="63"/>
-      <c r="F20" s="63"/>
-      <c r="G20" s="63"/>
+      <c r="A20" s="31"/>
+      <c r="B20" s="31"/>
+      <c r="C20" s="31"/>
+      <c r="D20" s="31"/>
+      <c r="E20" s="31"/>
+      <c r="F20" s="31"/>
+      <c r="G20" s="31"/>
     </row>
     <row r="21" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A21" s="63"/>
-      <c r="B21" s="63"/>
-      <c r="C21" s="63"/>
-      <c r="D21" s="63"/>
-      <c r="E21" s="63"/>
-      <c r="F21" s="63"/>
-      <c r="G21" s="63"/>
+      <c r="A21" s="31"/>
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
     </row>
     <row r="22" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A22" s="63"/>
-      <c r="B22" s="63"/>
-      <c r="C22" s="63"/>
-      <c r="D22" s="63"/>
-      <c r="E22" s="63"/>
-      <c r="F22" s="63"/>
-      <c r="G22" s="63"/>
+      <c r="A22" s="31"/>
+      <c r="B22" s="31"/>
+      <c r="C22" s="31"/>
+      <c r="D22" s="31"/>
+      <c r="E22" s="31"/>
+      <c r="F22" s="31"/>
+      <c r="G22" s="31"/>
     </row>
     <row r="23" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A23" s="63"/>
-      <c r="B23" s="63"/>
-      <c r="C23" s="63"/>
-      <c r="D23" s="63"/>
-      <c r="E23" s="63"/>
-      <c r="F23" s="63"/>
-      <c r="G23" s="63"/>
+      <c r="A23" s="31"/>
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
     </row>
     <row r="24" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A24" s="63"/>
-      <c r="B24" s="63"/>
-      <c r="C24" s="63"/>
-      <c r="D24" s="63"/>
-      <c r="E24" s="63"/>
-      <c r="F24" s="63"/>
-      <c r="G24" s="63"/>
+      <c r="A24" s="31"/>
+      <c r="B24" s="31"/>
+      <c r="C24" s="31"/>
+      <c r="D24" s="31"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
     </row>
     <row r="25" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A25" s="63"/>
-      <c r="B25" s="63"/>
-      <c r="C25" s="63"/>
-      <c r="D25" s="63"/>
-      <c r="E25" s="63"/>
-      <c r="F25" s="63"/>
-      <c r="G25" s="63"/>
+      <c r="A25" s="31"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="31"/>
+      <c r="D25" s="31"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="31"/>
+      <c r="G25" s="31"/>
     </row>
     <row r="26" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A26" s="63"/>
-      <c r="B26" s="63"/>
-      <c r="C26" s="63"/>
-      <c r="D26" s="63"/>
-      <c r="E26" s="63"/>
-      <c r="F26" s="63"/>
-      <c r="G26" s="63"/>
+      <c r="A26" s="31"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="31"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="31"/>
+      <c r="G26" s="31"/>
     </row>
     <row r="27" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A27" s="63"/>
-      <c r="B27" s="63"/>
-      <c r="C27" s="63"/>
-      <c r="D27" s="63"/>
-      <c r="E27" s="63"/>
-      <c r="F27" s="63"/>
-      <c r="G27" s="63"/>
+      <c r="A27" s="31"/>
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
     </row>
     <row r="28" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A28" s="63"/>
-      <c r="B28" s="63"/>
-      <c r="C28" s="63"/>
-      <c r="D28" s="63"/>
-      <c r="E28" s="63"/>
-      <c r="F28" s="63"/>
-      <c r="G28" s="63"/>
+      <c r="A28" s="31"/>
+      <c r="B28" s="31"/>
+      <c r="C28" s="31"/>
+      <c r="D28" s="31"/>
+      <c r="E28" s="31"/>
+      <c r="F28" s="31"/>
+      <c r="G28" s="31"/>
     </row>
     <row r="29" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A29" s="63"/>
-      <c r="B29" s="63"/>
-      <c r="C29" s="63"/>
-      <c r="D29" s="63"/>
-      <c r="E29" s="63"/>
-      <c r="F29" s="63"/>
-      <c r="G29" s="63"/>
+      <c r="A29" s="31"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="31"/>
+      <c r="D29" s="31"/>
+      <c r="E29" s="31"/>
+      <c r="F29" s="31"/>
+      <c r="G29" s="31"/>
     </row>
     <row r="30" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A30" s="63"/>
-      <c r="B30" s="63"/>
-      <c r="C30" s="63"/>
-      <c r="D30" s="63"/>
-      <c r="E30" s="63"/>
-      <c r="F30" s="63"/>
-      <c r="G30" s="63"/>
+      <c r="A30" s="31"/>
+      <c r="B30" s="31"/>
+      <c r="C30" s="31"/>
+      <c r="D30" s="31"/>
+      <c r="E30" s="31"/>
+      <c r="F30" s="31"/>
+      <c r="G30" s="31"/>
     </row>
     <row r="31" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A31" s="63"/>
-      <c r="B31" s="63"/>
-      <c r="C31" s="63"/>
-      <c r="D31" s="63"/>
-      <c r="E31" s="63"/>
-      <c r="F31" s="63"/>
-      <c r="G31" s="63"/>
+      <c r="A31" s="31"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="31"/>
+      <c r="D31" s="31"/>
+      <c r="E31" s="31"/>
+      <c r="F31" s="31"/>
+      <c r="G31" s="31"/>
     </row>
     <row r="32" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A32" s="63"/>
-      <c r="B32" s="63"/>
-      <c r="C32" s="63"/>
-      <c r="D32" s="63"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="63"/>
-      <c r="G32" s="63"/>
+      <c r="A32" s="31"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
     </row>
     <row r="33" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A33" s="63"/>
-      <c r="B33" s="63"/>
-      <c r="C33" s="63"/>
-      <c r="D33" s="63"/>
-      <c r="E33" s="63"/>
-      <c r="F33" s="63"/>
-      <c r="G33" s="63"/>
+      <c r="A33" s="31"/>
+      <c r="B33" s="31"/>
+      <c r="C33" s="31"/>
+      <c r="D33" s="31"/>
+      <c r="E33" s="31"/>
+      <c r="F33" s="31"/>
+      <c r="G33" s="31"/>
     </row>
     <row r="34" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A34" s="63"/>
-      <c r="B34" s="63"/>
-      <c r="C34" s="63"/>
-      <c r="D34" s="63"/>
-      <c r="E34" s="63"/>
-      <c r="F34" s="63"/>
-      <c r="G34" s="63"/>
+      <c r="A34" s="31"/>
+      <c r="B34" s="31"/>
+      <c r="C34" s="31"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
+      <c r="F34" s="31"/>
+      <c r="G34" s="31"/>
     </row>
     <row r="35" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A35" s="63"/>
-      <c r="B35" s="63"/>
-      <c r="C35" s="63"/>
-      <c r="D35" s="63"/>
-      <c r="E35" s="63"/>
-      <c r="F35" s="63"/>
-      <c r="G35" s="63"/>
+      <c r="A35" s="31"/>
+      <c r="B35" s="31"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="31"/>
+      <c r="G35" s="31"/>
     </row>
     <row r="36" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A36" s="63"/>
-      <c r="B36" s="63"/>
-      <c r="C36" s="63"/>
-      <c r="D36" s="63"/>
-      <c r="E36" s="63"/>
-      <c r="F36" s="63"/>
-      <c r="G36" s="63"/>
+      <c r="A36" s="31"/>
+      <c r="B36" s="31"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="31"/>
+      <c r="G36" s="31"/>
     </row>
     <row r="37" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A37" s="63"/>
-      <c r="B37" s="63"/>
-      <c r="C37" s="63"/>
-      <c r="D37" s="63"/>
-      <c r="E37" s="63"/>
-      <c r="F37" s="63"/>
-      <c r="G37" s="63"/>
+      <c r="A37" s="31"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
     </row>
     <row r="38" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A38" s="63"/>
-      <c r="B38" s="63"/>
-      <c r="C38" s="63"/>
-      <c r="D38" s="63"/>
-      <c r="E38" s="63"/>
-      <c r="F38" s="63"/>
-      <c r="G38" s="63"/>
+      <c r="A38" s="31"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="31"/>
+      <c r="G38" s="31"/>
     </row>
     <row r="39" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A39" s="63"/>
-      <c r="B39" s="63"/>
-      <c r="C39" s="63"/>
-      <c r="D39" s="63"/>
-      <c r="E39" s="63"/>
-      <c r="F39" s="63"/>
-      <c r="G39" s="63"/>
+      <c r="A39" s="31"/>
+      <c r="B39" s="31"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="31"/>
+      <c r="G39" s="31"/>
     </row>
     <row r="40" spans="1:7" ht="14.25" customHeight="1">
-      <c r="A40" s="63"/>
-      <c r="B40" s="63"/>
-      <c r="C40" s="63"/>
-      <c r="D40" s="63"/>
-      <c r="E40" s="63"/>
-      <c r="F40" s="63"/>
-      <c r="G40" s="63"/>
+      <c r="A40" s="31"/>
+      <c r="B40" s="31"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="31"/>
+      <c r="G40" s="31"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -2942,805 +2974,805 @@
   </sheetPr>
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H17"/>
+    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="9" width="6.28515625" customWidth="1"/>
-    <col min="10" max="10" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="21" width="6.28515625" customWidth="1"/>
-    <col min="22" max="22" width="14.85546875" customWidth="1"/>
-    <col min="23" max="23" width="8.5703125" customWidth="1"/>
-    <col min="24" max="26" width="6.28515625" customWidth="1"/>
+    <col min="1" max="9" width="6.33203125" customWidth="1"/>
+    <col min="10" max="10" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="21" width="6.33203125" customWidth="1"/>
+    <col min="22" max="22" width="14.83203125" customWidth="1"/>
+    <col min="23" max="23" width="8.5" customWidth="1"/>
+    <col min="24" max="26" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="12.75">
-      <c r="A1" s="96" t="s">
+    <row r="1" spans="1:23" ht="13">
+      <c r="A1" s="84" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="J1" s="97" t="s">
+      <c r="B1" s="85"/>
+      <c r="C1" s="85"/>
+      <c r="D1" s="85"/>
+      <c r="E1" s="85"/>
+      <c r="F1" s="85"/>
+      <c r="G1" s="85"/>
+      <c r="H1" s="85"/>
+      <c r="J1" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="K1" s="98"/>
-      <c r="L1" s="98"/>
-      <c r="M1" s="98"/>
-      <c r="N1" s="98"/>
-      <c r="O1" s="98"/>
-      <c r="P1" s="98"/>
-      <c r="Q1" s="98"/>
-      <c r="R1" s="98"/>
-      <c r="S1" s="98"/>
-      <c r="T1" s="99"/>
-      <c r="V1" s="100" t="s">
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69"/>
+      <c r="S1" s="69"/>
+      <c r="T1" s="70"/>
+      <c r="V1" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="W1" s="99"/>
+      <c r="W1" s="70"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="98"/>
-      <c r="D2" s="98"/>
-      <c r="E2" s="98"/>
-      <c r="F2" s="98"/>
-      <c r="G2" s="98"/>
-      <c r="H2" s="99"/>
-      <c r="J2" s="41" t="s">
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="70"/>
+      <c r="J2" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="K2" s="42">
+      <c r="K2" s="13">
         <v>1</v>
       </c>
-      <c r="L2" s="42">
+      <c r="L2" s="13">
         <v>2</v>
       </c>
-      <c r="M2" s="42">
+      <c r="M2" s="13">
         <v>3</v>
       </c>
-      <c r="N2" s="42">
+      <c r="N2" s="13">
         <v>4</v>
       </c>
-      <c r="O2" s="42">
+      <c r="O2" s="13">
         <v>5</v>
       </c>
-      <c r="P2" s="42">
+      <c r="P2" s="13">
         <v>6</v>
       </c>
-      <c r="Q2" s="42">
+      <c r="Q2" s="13">
         <v>7</v>
       </c>
-      <c r="R2" s="42">
+      <c r="R2" s="13">
         <v>8</v>
       </c>
-      <c r="S2" s="42">
+      <c r="S2" s="13">
         <v>9</v>
       </c>
-      <c r="T2" s="42">
+      <c r="T2" s="13">
         <v>10</v>
       </c>
-      <c r="V2" s="43" t="s">
+      <c r="V2" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="W2" s="43" t="s">
+      <c r="W2" s="14" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A3" s="44"/>
-      <c r="B3" s="45">
+      <c r="A3" s="15"/>
+      <c r="B3" s="16">
         <v>2.5</v>
       </c>
-      <c r="C3" s="45">
+      <c r="C3" s="16">
         <v>2.5499999999999998</v>
       </c>
-      <c r="D3" s="45">
+      <c r="D3" s="16">
         <v>2.6</v>
       </c>
-      <c r="E3" s="45">
+      <c r="E3" s="16">
         <v>2.65</v>
       </c>
-      <c r="F3" s="45">
+      <c r="F3" s="16">
         <v>2.7</v>
       </c>
-      <c r="G3" s="45">
+      <c r="G3" s="16">
         <v>2.75</v>
       </c>
-      <c r="H3" s="45">
+      <c r="H3" s="16">
         <v>2.8</v>
       </c>
-      <c r="J3" s="46" t="s">
+      <c r="J3" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="K3" s="47">
+      <c r="K3" s="18">
         <v>100</v>
       </c>
-      <c r="L3" s="48">
+      <c r="L3" s="18">
         <f t="shared" ref="L3:P3" si="0">K3-5</f>
         <v>95</v>
       </c>
-      <c r="M3" s="48">
+      <c r="M3" s="18">
         <f t="shared" si="0"/>
         <v>90</v>
       </c>
-      <c r="N3" s="48">
+      <c r="N3" s="18">
         <f t="shared" si="0"/>
         <v>85</v>
       </c>
-      <c r="O3" s="48">
+      <c r="O3" s="18">
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="P3" s="48">
+      <c r="P3" s="18">
         <f t="shared" si="0"/>
         <v>75</v>
       </c>
-      <c r="Q3" s="48">
+      <c r="Q3" s="18">
         <f t="shared" ref="Q3:S3" si="1">P3-2</f>
         <v>73</v>
       </c>
-      <c r="R3" s="48">
+      <c r="R3" s="18">
         <f t="shared" si="1"/>
         <v>71</v>
       </c>
-      <c r="S3" s="48">
+      <c r="S3" s="18">
         <f t="shared" si="1"/>
         <v>69</v>
       </c>
-      <c r="T3" s="48">
+      <c r="T3" s="18">
         <f t="shared" ref="T3:T9" si="2">S3-4</f>
         <v>65</v>
       </c>
-      <c r="V3" s="49" t="s">
+      <c r="V3" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="W3" s="50">
+      <c r="W3" s="20">
         <v>70</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A4" s="51">
+      <c r="A4" s="21">
         <v>17</v>
       </c>
-      <c r="B4" s="52">
+      <c r="B4" s="22">
         <v>1.49E-2</v>
       </c>
-      <c r="C4" s="52">
+      <c r="C4" s="22">
         <v>1.46E-2</v>
       </c>
-      <c r="D4" s="52">
+      <c r="D4" s="22">
         <v>1.44E-2</v>
       </c>
-      <c r="E4" s="52">
+      <c r="E4" s="22">
         <v>1.4200000000000001E-2</v>
       </c>
-      <c r="F4" s="52">
+      <c r="F4" s="22">
         <v>1.4E-2</v>
       </c>
-      <c r="G4" s="52">
+      <c r="G4" s="22">
         <v>1.38E-2</v>
       </c>
-      <c r="H4" s="52">
+      <c r="H4" s="22">
         <v>1.3599999999999999E-2</v>
       </c>
-      <c r="J4" s="46" t="s">
+      <c r="J4" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="47">
+      <c r="K4" s="18">
         <v>120</v>
       </c>
-      <c r="L4" s="48">
+      <c r="L4" s="18">
         <f t="shared" ref="L4:P4" si="3">K4-5</f>
         <v>115</v>
       </c>
-      <c r="M4" s="48">
+      <c r="M4" s="18">
         <f t="shared" si="3"/>
         <v>110</v>
       </c>
-      <c r="N4" s="48">
+      <c r="N4" s="18">
         <f t="shared" si="3"/>
         <v>105</v>
       </c>
-      <c r="O4" s="48">
+      <c r="O4" s="18">
         <f t="shared" si="3"/>
         <v>100</v>
       </c>
-      <c r="P4" s="48">
+      <c r="P4" s="18">
         <f t="shared" si="3"/>
         <v>95</v>
       </c>
-      <c r="Q4" s="48">
+      <c r="Q4" s="18">
         <f t="shared" ref="Q4:S4" si="4">P4-2</f>
         <v>93</v>
       </c>
-      <c r="R4" s="48">
+      <c r="R4" s="18">
         <f t="shared" si="4"/>
         <v>91</v>
       </c>
-      <c r="S4" s="48">
+      <c r="S4" s="18">
         <f t="shared" si="4"/>
         <v>89</v>
       </c>
-      <c r="T4" s="48">
+      <c r="T4" s="18">
         <f t="shared" si="2"/>
         <v>85</v>
       </c>
-      <c r="V4" s="49" t="s">
+      <c r="V4" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="W4" s="50">
+      <c r="W4" s="20">
         <v>72</v>
       </c>
     </row>
     <row r="5" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A5" s="51">
+      <c r="A5" s="21">
         <v>18</v>
       </c>
-      <c r="B5" s="52">
+      <c r="B5" s="22">
         <v>1.47E-2</v>
       </c>
-      <c r="C5" s="52">
+      <c r="C5" s="22">
         <v>1.44E-2</v>
       </c>
-      <c r="D5" s="52">
+      <c r="D5" s="22">
         <v>1.4200000000000001E-2</v>
       </c>
-      <c r="E5" s="52">
+      <c r="E5" s="22">
         <v>1.4E-2</v>
       </c>
-      <c r="F5" s="52">
+      <c r="F5" s="22">
         <v>1.38E-2</v>
       </c>
-      <c r="G5" s="52">
+      <c r="G5" s="22">
         <v>1.3599999999999999E-2</v>
       </c>
-      <c r="H5" s="52">
+      <c r="H5" s="22">
         <v>1.34E-2</v>
       </c>
-      <c r="J5" s="46" t="s">
+      <c r="J5" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="K5" s="47">
+      <c r="K5" s="18">
         <v>150</v>
       </c>
-      <c r="L5" s="48">
+      <c r="L5" s="18">
         <f t="shared" ref="L5:P5" si="5">K5-5</f>
         <v>145</v>
       </c>
-      <c r="M5" s="48">
+      <c r="M5" s="18">
         <f t="shared" si="5"/>
         <v>140</v>
       </c>
-      <c r="N5" s="48">
+      <c r="N5" s="18">
         <f t="shared" si="5"/>
         <v>135</v>
       </c>
-      <c r="O5" s="48">
+      <c r="O5" s="18">
         <f t="shared" si="5"/>
         <v>130</v>
       </c>
-      <c r="P5" s="48">
+      <c r="P5" s="18">
         <f t="shared" si="5"/>
         <v>125</v>
       </c>
-      <c r="Q5" s="48">
+      <c r="Q5" s="18">
         <f t="shared" ref="Q5:S5" si="6">P5-2</f>
         <v>123</v>
       </c>
-      <c r="R5" s="48">
+      <c r="R5" s="18">
         <f t="shared" si="6"/>
         <v>121</v>
       </c>
-      <c r="S5" s="48">
+      <c r="S5" s="18">
         <f t="shared" si="6"/>
         <v>119</v>
       </c>
-      <c r="T5" s="48">
+      <c r="T5" s="18">
         <f t="shared" si="2"/>
         <v>115</v>
       </c>
-      <c r="V5" s="49" t="s">
+      <c r="V5" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="W5" s="50">
+      <c r="W5" s="20">
         <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A6" s="51">
+      <c r="A6" s="21">
         <v>19</v>
       </c>
-      <c r="B6" s="52">
+      <c r="B6" s="22">
         <v>1.4500000000000001E-2</v>
       </c>
-      <c r="C6" s="52">
+      <c r="C6" s="22">
         <v>1.43E-2</v>
       </c>
-      <c r="D6" s="52">
+      <c r="D6" s="22">
         <v>1.4E-2</v>
       </c>
-      <c r="E6" s="52">
+      <c r="E6" s="22">
         <v>1.38E-2</v>
       </c>
-      <c r="F6" s="52">
+      <c r="F6" s="22">
         <v>1.3599999999999999E-2</v>
       </c>
-      <c r="G6" s="52">
+      <c r="G6" s="22">
         <v>1.34E-2</v>
       </c>
-      <c r="H6" s="52">
+      <c r="H6" s="22">
         <v>1.32E-2</v>
       </c>
-      <c r="J6" s="46" t="s">
+      <c r="J6" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="K6" s="47">
+      <c r="K6" s="18">
         <v>100</v>
       </c>
-      <c r="L6" s="48">
+      <c r="L6" s="18">
         <f t="shared" ref="L6:P6" si="7">K6-5</f>
         <v>95</v>
       </c>
-      <c r="M6" s="48">
+      <c r="M6" s="18">
         <f t="shared" si="7"/>
         <v>90</v>
       </c>
-      <c r="N6" s="48">
+      <c r="N6" s="18">
         <f t="shared" si="7"/>
         <v>85</v>
       </c>
-      <c r="O6" s="48">
+      <c r="O6" s="18">
         <f t="shared" si="7"/>
         <v>80</v>
       </c>
-      <c r="P6" s="48">
+      <c r="P6" s="18">
         <f t="shared" si="7"/>
         <v>75</v>
       </c>
-      <c r="Q6" s="48">
+      <c r="Q6" s="18">
         <f t="shared" ref="Q6:S6" si="8">P6-2</f>
         <v>73</v>
       </c>
-      <c r="R6" s="48">
+      <c r="R6" s="18">
         <f t="shared" si="8"/>
         <v>71</v>
       </c>
-      <c r="S6" s="48">
+      <c r="S6" s="18">
         <f t="shared" si="8"/>
         <v>69</v>
       </c>
-      <c r="T6" s="48">
+      <c r="T6" s="18">
         <f t="shared" si="2"/>
         <v>65</v>
       </c>
-      <c r="V6" s="49" t="s">
+      <c r="V6" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="W6" s="50">
+      <c r="W6" s="20">
         <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A7" s="51">
+      <c r="A7" s="21">
         <v>20</v>
       </c>
-      <c r="B7" s="52">
+      <c r="B7" s="22">
         <v>1.43E-2</v>
       </c>
-      <c r="C7" s="52">
+      <c r="C7" s="22">
         <v>1.41E-2</v>
       </c>
-      <c r="D7" s="52">
+      <c r="D7" s="22">
         <v>1.3899999999999999E-2</v>
       </c>
-      <c r="E7" s="52">
+      <c r="E7" s="22">
         <v>1.37E-2</v>
       </c>
-      <c r="F7" s="52">
+      <c r="F7" s="22">
         <v>1.34E-2</v>
       </c>
-      <c r="G7" s="52">
+      <c r="G7" s="22">
         <v>1.3299999999999999E-2</v>
       </c>
-      <c r="H7" s="52">
+      <c r="H7" s="22">
         <v>1.3100000000000001E-2</v>
       </c>
-      <c r="J7" s="46" t="s">
+      <c r="J7" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="K7" s="47">
+      <c r="K7" s="18">
         <v>70</v>
       </c>
-      <c r="L7" s="48">
+      <c r="L7" s="18">
         <f t="shared" ref="L7:P7" si="9">K7-5</f>
         <v>65</v>
       </c>
-      <c r="M7" s="48">
+      <c r="M7" s="18">
         <f t="shared" si="9"/>
         <v>60</v>
       </c>
-      <c r="N7" s="48">
+      <c r="N7" s="18">
         <f t="shared" si="9"/>
         <v>55</v>
       </c>
-      <c r="O7" s="48">
+      <c r="O7" s="18">
         <f t="shared" si="9"/>
         <v>50</v>
       </c>
-      <c r="P7" s="48">
+      <c r="P7" s="18">
         <f t="shared" si="9"/>
         <v>45</v>
       </c>
-      <c r="Q7" s="48">
+      <c r="Q7" s="18">
         <f t="shared" ref="Q7:S7" si="10">P7-2</f>
         <v>43</v>
       </c>
-      <c r="R7" s="48">
+      <c r="R7" s="18">
         <f t="shared" si="10"/>
         <v>41</v>
       </c>
-      <c r="S7" s="48">
+      <c r="S7" s="18">
         <f t="shared" si="10"/>
         <v>39</v>
       </c>
-      <c r="T7" s="48">
+      <c r="T7" s="18">
         <f t="shared" si="2"/>
         <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A8" s="51">
+      <c r="A8" s="21">
         <v>21</v>
       </c>
-      <c r="B8" s="52">
+      <c r="B8" s="22">
         <v>1.41E-2</v>
       </c>
-      <c r="C8" s="52">
+      <c r="C8" s="22">
         <v>1.3899999999999999E-2</v>
       </c>
-      <c r="D8" s="52">
+      <c r="D8" s="22">
         <v>1.37E-2</v>
       </c>
-      <c r="E8" s="52">
+      <c r="E8" s="22">
         <v>1.35E-2</v>
       </c>
-      <c r="F8" s="52">
+      <c r="F8" s="22">
         <v>1.3299999999999999E-2</v>
       </c>
-      <c r="G8" s="52">
+      <c r="G8" s="22">
         <v>1.3100000000000001E-2</v>
       </c>
-      <c r="H8" s="52">
+      <c r="H8" s="22">
         <v>1.29E-2</v>
       </c>
-      <c r="J8" s="46" t="s">
+      <c r="J8" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="K8" s="47">
+      <c r="K8" s="18">
         <v>80</v>
       </c>
-      <c r="L8" s="48">
+      <c r="L8" s="18">
         <f t="shared" ref="L8:P8" si="11">K8-5</f>
         <v>75</v>
       </c>
-      <c r="M8" s="48">
+      <c r="M8" s="18">
         <f t="shared" si="11"/>
         <v>70</v>
       </c>
-      <c r="N8" s="48">
+      <c r="N8" s="18">
         <f t="shared" si="11"/>
         <v>65</v>
       </c>
-      <c r="O8" s="48">
+      <c r="O8" s="18">
         <f t="shared" si="11"/>
         <v>60</v>
       </c>
-      <c r="P8" s="48">
+      <c r="P8" s="18">
         <f t="shared" si="11"/>
         <v>55</v>
       </c>
-      <c r="Q8" s="48">
+      <c r="Q8" s="18">
         <f t="shared" ref="Q8:S8" si="12">P8-2</f>
         <v>53</v>
       </c>
-      <c r="R8" s="48">
+      <c r="R8" s="18">
         <f t="shared" si="12"/>
         <v>51</v>
       </c>
-      <c r="S8" s="48">
+      <c r="S8" s="18">
         <f t="shared" si="12"/>
         <v>49</v>
       </c>
-      <c r="T8" s="48">
+      <c r="T8" s="18">
         <f t="shared" si="2"/>
         <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A9" s="51">
+      <c r="A9" s="21">
         <v>22</v>
       </c>
-      <c r="B9" s="52">
+      <c r="B9" s="22">
         <v>1.4E-2</v>
       </c>
-      <c r="C9" s="52">
+      <c r="C9" s="22">
         <v>1.37E-2</v>
       </c>
-      <c r="D9" s="52">
+      <c r="D9" s="22">
         <v>1.35E-2</v>
       </c>
-      <c r="E9" s="52">
+      <c r="E9" s="22">
         <v>1.3299999999999999E-2</v>
       </c>
-      <c r="F9" s="52">
+      <c r="F9" s="22">
         <v>1.3100000000000001E-2</v>
       </c>
-      <c r="G9" s="52">
+      <c r="G9" s="22">
         <v>1.29E-2</v>
       </c>
-      <c r="H9" s="52">
+      <c r="H9" s="22">
         <v>1.2800000000000001E-2</v>
       </c>
-      <c r="J9" s="46" t="s">
+      <c r="J9" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="K9" s="47">
+      <c r="K9" s="18">
         <v>150</v>
       </c>
-      <c r="L9" s="48">
+      <c r="L9" s="18">
         <f t="shared" ref="L9:P9" si="13">K9-5</f>
         <v>145</v>
       </c>
-      <c r="M9" s="48">
+      <c r="M9" s="18">
         <f t="shared" si="13"/>
         <v>140</v>
       </c>
-      <c r="N9" s="48">
+      <c r="N9" s="18">
         <f t="shared" si="13"/>
         <v>135</v>
       </c>
-      <c r="O9" s="48">
+      <c r="O9" s="18">
         <f t="shared" si="13"/>
         <v>130</v>
       </c>
-      <c r="P9" s="48">
+      <c r="P9" s="18">
         <f t="shared" si="13"/>
         <v>125</v>
       </c>
-      <c r="Q9" s="48">
+      <c r="Q9" s="18">
         <f t="shared" ref="Q9:S9" si="14">P9-2</f>
         <v>123</v>
       </c>
-      <c r="R9" s="48">
+      <c r="R9" s="18">
         <f t="shared" si="14"/>
         <v>121</v>
       </c>
-      <c r="S9" s="48">
+      <c r="S9" s="18">
         <f t="shared" si="14"/>
         <v>119</v>
       </c>
-      <c r="T9" s="48">
+      <c r="T9" s="18">
         <f t="shared" si="2"/>
         <v>115</v>
       </c>
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A10" s="51">
+      <c r="A10" s="21">
         <v>23</v>
       </c>
-      <c r="B10" s="52">
+      <c r="B10" s="22">
         <v>1.38E-2</v>
       </c>
-      <c r="C10" s="52">
+      <c r="C10" s="22">
         <v>1.3599999999999999E-2</v>
       </c>
-      <c r="D10" s="52">
+      <c r="D10" s="22">
         <v>1.34E-2</v>
       </c>
-      <c r="E10" s="52">
+      <c r="E10" s="22">
         <v>1.32E-2</v>
       </c>
-      <c r="F10" s="52">
+      <c r="F10" s="22">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="G10" s="52">
+      <c r="G10" s="22">
         <v>1.2800000000000001E-2</v>
       </c>
-      <c r="H10" s="52">
+      <c r="H10" s="22">
         <v>1.26E-2</v>
       </c>
     </row>
     <row r="11" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A11" s="51">
+      <c r="A11" s="21">
         <v>24</v>
       </c>
-      <c r="B11" s="52">
+      <c r="B11" s="22">
         <v>1.37E-2</v>
       </c>
-      <c r="C11" s="52">
+      <c r="C11" s="22">
         <v>1.34E-2</v>
       </c>
-      <c r="D11" s="52">
+      <c r="D11" s="22">
         <v>1.32E-2</v>
       </c>
-      <c r="E11" s="52">
+      <c r="E11" s="22">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="F11" s="52">
+      <c r="F11" s="22">
         <v>1.2800000000000001E-2</v>
       </c>
-      <c r="G11" s="52">
+      <c r="G11" s="22">
         <v>1.26E-2</v>
       </c>
-      <c r="H11" s="52">
+      <c r="H11" s="22">
         <v>1.2500000000000001E-2</v>
       </c>
     </row>
     <row r="12" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A12" s="51">
+      <c r="A12" s="21">
         <v>25</v>
       </c>
-      <c r="B12" s="52">
+      <c r="B12" s="22">
         <v>1.35E-2</v>
       </c>
-      <c r="C12" s="52">
+      <c r="C12" s="22">
         <v>1.3299999999999999E-2</v>
       </c>
-      <c r="D12" s="52">
+      <c r="D12" s="22">
         <v>1.3100000000000001E-2</v>
       </c>
-      <c r="E12" s="52">
+      <c r="E12" s="22">
         <v>1.29E-2</v>
       </c>
-      <c r="F12" s="52">
+      <c r="F12" s="22">
         <v>1.2699999999999999E-2</v>
       </c>
-      <c r="G12" s="52">
+      <c r="G12" s="22">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="H12" s="52">
+      <c r="H12" s="22">
         <v>1.23E-2</v>
       </c>
     </row>
     <row r="13" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A13" s="51">
+      <c r="A13" s="21">
         <v>26</v>
       </c>
-      <c r="B13" s="52">
+      <c r="B13" s="22">
         <v>1.3299999999999999E-2</v>
       </c>
-      <c r="C13" s="52">
+      <c r="C13" s="22">
         <v>1.3100000000000001E-2</v>
       </c>
-      <c r="D13" s="52">
+      <c r="D13" s="22">
         <v>1.29E-2</v>
       </c>
-      <c r="E13" s="52">
+      <c r="E13" s="22">
         <v>1.2699999999999999E-2</v>
       </c>
-      <c r="F13" s="52">
+      <c r="F13" s="22">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="G13" s="52">
+      <c r="G13" s="22">
         <v>1.24E-2</v>
       </c>
-      <c r="H13" s="52">
+      <c r="H13" s="22">
         <v>1.2200000000000001E-2</v>
       </c>
     </row>
     <row r="14" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A14" s="51">
+      <c r="A14" s="21">
         <v>27</v>
       </c>
-      <c r="B14" s="52">
+      <c r="B14" s="22">
         <v>1.32E-2</v>
       </c>
-      <c r="C14" s="52">
+      <c r="C14" s="22">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="D14" s="52">
+      <c r="D14" s="22">
         <v>1.2800000000000001E-2</v>
       </c>
-      <c r="E14" s="52">
+      <c r="E14" s="22">
         <v>1.26E-2</v>
       </c>
-      <c r="F14" s="52">
+      <c r="F14" s="22">
         <v>1.24E-2</v>
       </c>
-      <c r="G14" s="52">
+      <c r="G14" s="22">
         <v>1.2200000000000001E-2</v>
       </c>
-      <c r="H14" s="52">
+      <c r="H14" s="22">
         <v>1.2E-2</v>
       </c>
     </row>
     <row r="15" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A15" s="51">
+      <c r="A15" s="21">
         <v>28</v>
       </c>
-      <c r="B15" s="52">
+      <c r="B15" s="22">
         <v>1.2999999999999999E-2</v>
       </c>
-      <c r="C15" s="52">
+      <c r="C15" s="22">
         <v>1.2800000000000001E-2</v>
       </c>
-      <c r="D15" s="52">
+      <c r="D15" s="22">
         <v>1.26E-2</v>
       </c>
-      <c r="E15" s="52">
+      <c r="E15" s="22">
         <v>1.24E-2</v>
       </c>
-      <c r="F15" s="52">
+      <c r="F15" s="22">
         <v>1.23E-2</v>
       </c>
-      <c r="G15" s="52">
+      <c r="G15" s="22">
         <v>1.21E-2</v>
       </c>
-      <c r="H15" s="52">
+      <c r="H15" s="22">
         <v>1.1900000000000001E-2</v>
       </c>
     </row>
     <row r="16" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A16" s="51">
+      <c r="A16" s="21">
         <v>29</v>
       </c>
-      <c r="B16" s="52">
+      <c r="B16" s="22">
         <v>1.29E-2</v>
       </c>
-      <c r="C16" s="52">
+      <c r="C16" s="22">
         <v>1.2699999999999999E-2</v>
       </c>
-      <c r="D16" s="52">
+      <c r="D16" s="22">
         <v>1.2500000000000001E-2</v>
       </c>
-      <c r="E16" s="52">
+      <c r="E16" s="22">
         <v>1.23E-2</v>
       </c>
-      <c r="F16" s="52">
+      <c r="F16" s="22">
         <v>1.3100000000000001E-2</v>
       </c>
-      <c r="G16" s="52">
+      <c r="G16" s="22">
         <v>1.2E-2</v>
       </c>
-      <c r="H16" s="52">
+      <c r="H16" s="22">
         <v>1.18E-2</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A17" s="53">
+      <c r="A17" s="23">
         <v>30</v>
       </c>
-      <c r="B17" s="54">
+      <c r="B17" s="24">
         <v>1.2800000000000001E-2</v>
       </c>
-      <c r="C17" s="54">
+      <c r="C17" s="24">
         <v>1.26E-2</v>
       </c>
-      <c r="D17" s="54">
+      <c r="D17" s="24">
         <v>1.24E-2</v>
       </c>
-      <c r="E17" s="54">
+      <c r="E17" s="24">
         <v>1.2200000000000001E-2</v>
       </c>
-      <c r="F17" s="54">
+      <c r="F17" s="24">
         <v>1.2E-2</v>
       </c>
-      <c r="G17" s="54">
+      <c r="G17" s="24">
         <v>1.18E-2</v>
       </c>
-      <c r="H17" s="54">
+      <c r="H17" s="24">
         <v>1.17E-2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Fixed the data validation in the hw
</commit_message>
<xml_diff>
--- a/docs/unit1/2_lookup_match_if/(Starter-Workbook)-HW-Lookups-Match-IF.xlsx
+++ b/docs/unit1/2_lookup_match_if/(Starter-Workbook)-HW-Lookups-Match-IF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/njones/PycharmProjects/content/docs/unit1/2_lookup_match_if/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\CCE270\content\docs\unit1\2_lookup_match_if\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31485A32-0D4B-1341-954C-088C603BE32D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF320F51-9C6F-44C8-9D69-E2F9630463F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="24020" yWindow="2680" windowWidth="33860" windowHeight="24420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydrometer Analysis" sheetId="1" r:id="rId1"/>
@@ -35,8 +35,33 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1067,6 +1092,17 @@
     <xf numFmtId="164" fontId="24" fillId="20" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1077,11 +1113,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1090,12 +1121,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1456,25 +1481,25 @@
   </sheetPr>
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
       <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="11.83203125" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="3" max="6" width="11" customWidth="1"/>
-    <col min="7" max="13" width="14.5" customWidth="1"/>
+    <col min="7" max="13" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="55" customFormat="1" ht="32" customHeight="1">
-      <c r="A1" s="64" t="s">
+    <row r="1" spans="1:13" s="55" customFormat="1" ht="32.1" customHeight="1">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
       <c r="G1" s="56"/>
       <c r="H1" s="57"/>
       <c r="I1" s="57"/>
@@ -1484,11 +1509,11 @@
       <c r="M1" s="57"/>
     </row>
     <row r="2" spans="1:13" ht="15">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
       <c r="D2" s="53" t="s">
         <v>2</v>
       </c>
@@ -1501,11 +1526,11 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:13" ht="15">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="70"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="66"/>
       <c r="D3" s="50" t="s">
         <v>6</v>
       </c>
@@ -1518,11 +1543,11 @@
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:13" ht="15">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="70"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="66"/>
       <c r="D4" s="50" t="s">
         <v>9</v>
       </c>
@@ -1533,11 +1558,11 @@
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:13" ht="15">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="73"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="75"/>
       <c r="D5" s="50" t="s">
         <v>11</v>
       </c>
@@ -1550,9 +1575,9 @@
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:13" ht="15">
-      <c r="A6" s="74"/>
-      <c r="B6" s="75"/>
-      <c r="C6" s="76"/>
+      <c r="A6" s="76"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="78"/>
       <c r="D6" s="50" t="s">
         <v>13</v>
       </c>
@@ -1563,11 +1588,11 @@
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:13" ht="15">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="70"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="66"/>
       <c r="D7" s="50" t="s">
         <v>16</v>
       </c>
@@ -1578,11 +1603,11 @@
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:13" ht="15">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="70"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="66"/>
       <c r="D8" s="50" t="s">
         <v>18</v>
       </c>
@@ -1593,11 +1618,11 @@
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:13" ht="15">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="70"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="66"/>
       <c r="D9" s="50" t="s">
         <v>20</v>
       </c>
@@ -1607,11 +1632,11 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:13" ht="15">
-      <c r="A10" s="68" t="s">
+      <c r="A10" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="69"/>
-      <c r="C10" s="70"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="66"/>
       <c r="D10" s="50" t="s">
         <v>22</v>
       </c>
@@ -1620,11 +1645,11 @@
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:13" ht="15">
-      <c r="A11" s="68" t="s">
+      <c r="A11" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="69"/>
-      <c r="C11" s="70"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="66"/>
       <c r="D11" s="50" t="s">
         <v>24</v>
       </c>
@@ -1635,26 +1660,26 @@
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:13" ht="18" customHeight="1"/>
-    <row r="13" spans="1:13" ht="26" customHeight="1">
-      <c r="A13" s="77" t="s">
+    <row r="13" spans="1:13" ht="26.1" customHeight="1">
+      <c r="A13" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="77" t="s">
+      <c r="B13" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="77" t="s">
+      <c r="C13" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="77" t="s">
+      <c r="D13" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="77" t="s">
+      <c r="E13" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="77" t="s">
+      <c r="F13" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="77" t="s">
+      <c r="G13" s="67" t="s">
         <v>31</v>
       </c>
       <c r="H13" s="1"/>
@@ -1664,14 +1689,14 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" ht="7" customHeight="1" thickBot="1">
-      <c r="A14" s="78"/>
-      <c r="B14" s="78"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
+    <row r="14" spans="1:13" ht="6.95" customHeight="1" thickBot="1">
+      <c r="A14" s="68"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="68"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1679,7 +1704,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" ht="16" thickBot="1">
+    <row r="15" spans="1:13" thickBot="1">
       <c r="A15" s="6">
         <v>0.25</v>
       </c>
@@ -1694,7 +1719,7 @@
       </c>
       <c r="G15" s="25"/>
     </row>
-    <row r="16" spans="1:13" ht="16" thickBot="1">
+    <row r="16" spans="1:13" thickBot="1">
       <c r="A16" s="6">
         <v>0.5</v>
       </c>
@@ -1709,7 +1734,7 @@
       </c>
       <c r="G16" s="28"/>
     </row>
-    <row r="17" spans="1:7" ht="16" thickBot="1">
+    <row r="17" spans="1:7" thickBot="1">
       <c r="A17" s="6">
         <v>1</v>
       </c>
@@ -1724,7 +1749,7 @@
       </c>
       <c r="G17" s="28"/>
     </row>
-    <row r="18" spans="1:7" ht="16" thickBot="1">
+    <row r="18" spans="1:7" thickBot="1">
       <c r="A18" s="6">
         <v>2</v>
       </c>
@@ -1739,7 +1764,7 @@
       </c>
       <c r="G18" s="28"/>
     </row>
-    <row r="19" spans="1:7" ht="16" thickBot="1">
+    <row r="19" spans="1:7" thickBot="1">
       <c r="A19" s="6">
         <v>4</v>
       </c>
@@ -1754,7 +1779,7 @@
       </c>
       <c r="G19" s="28"/>
     </row>
-    <row r="20" spans="1:7" ht="16" thickBot="1">
+    <row r="20" spans="1:7" thickBot="1">
       <c r="A20" s="6">
         <v>8</v>
       </c>
@@ -1769,7 +1794,7 @@
       </c>
       <c r="G20" s="28"/>
     </row>
-    <row r="21" spans="1:7" ht="16" thickBot="1">
+    <row r="21" spans="1:7" thickBot="1">
       <c r="A21" s="6">
         <v>15</v>
       </c>
@@ -1784,7 +1809,7 @@
       </c>
       <c r="G21" s="28"/>
     </row>
-    <row r="22" spans="1:7" ht="16" thickBot="1">
+    <row r="22" spans="1:7" thickBot="1">
       <c r="A22" s="6">
         <v>30</v>
       </c>
@@ -1799,7 +1824,7 @@
       </c>
       <c r="G22" s="28"/>
     </row>
-    <row r="23" spans="1:7" ht="16" thickBot="1">
+    <row r="23" spans="1:7" thickBot="1">
       <c r="A23" s="6">
         <v>60</v>
       </c>
@@ -1814,7 +1839,7 @@
       </c>
       <c r="G23" s="28"/>
     </row>
-    <row r="24" spans="1:7" ht="16" thickBot="1">
+    <row r="24" spans="1:7" thickBot="1">
       <c r="A24" s="6">
         <v>787</v>
       </c>
@@ -1829,7 +1854,7 @@
       </c>
       <c r="G24" s="28"/>
     </row>
-    <row r="25" spans="1:7" ht="16" thickBot="1">
+    <row r="25" spans="1:7" thickBot="1">
       <c r="A25" s="6">
         <v>1459</v>
       </c>
@@ -1873,6 +1898,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C6"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="E13:E14"/>
@@ -1885,11 +1915,6 @@
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1907,17 +1932,17 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="39" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.1640625" style="39" customWidth="1"/>
-    <col min="6" max="6" width="13.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.85546875" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.140625" style="39" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17" customHeight="1">
+    <row r="1" spans="1:7" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="42" t="s">
         <v>32</v>
       </c>
@@ -1940,7 +1965,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="13">
+    <row r="2" spans="1:7" ht="12.75">
       <c r="A2" s="40">
         <v>1124</v>
       </c>
@@ -1955,7 +1980,7 @@
       <c r="F2" s="40"/>
       <c r="G2" s="41"/>
     </row>
-    <row r="3" spans="1:7" ht="13">
+    <row r="3" spans="1:7" ht="12.75">
       <c r="A3" s="40">
         <v>1107</v>
       </c>
@@ -1970,7 +1995,7 @@
       <c r="F3" s="40"/>
       <c r="G3" s="40"/>
     </row>
-    <row r="4" spans="1:7" ht="13">
+    <row r="4" spans="1:7" ht="12.75">
       <c r="A4" s="40">
         <v>1163</v>
       </c>
@@ -1985,7 +2010,7 @@
       <c r="F4" s="40"/>
       <c r="G4" s="40"/>
     </row>
-    <row r="5" spans="1:7" ht="13">
+    <row r="5" spans="1:7" ht="12.75">
       <c r="A5" s="40">
         <v>1182</v>
       </c>
@@ -2000,7 +2025,7 @@
       <c r="F5" s="40"/>
       <c r="G5" s="40"/>
     </row>
-    <row r="6" spans="1:7" ht="13">
+    <row r="6" spans="1:7" ht="12.75">
       <c r="A6" s="40">
         <v>1175</v>
       </c>
@@ -2015,7 +2040,7 @@
       <c r="F6" s="40"/>
       <c r="G6" s="41"/>
     </row>
-    <row r="7" spans="1:7" ht="13">
+    <row r="7" spans="1:7" ht="12.75">
       <c r="A7" s="40">
         <v>1049</v>
       </c>
@@ -2030,7 +2055,7 @@
       <c r="F7" s="40"/>
       <c r="G7" s="41"/>
     </row>
-    <row r="8" spans="1:7" ht="13">
+    <row r="8" spans="1:7" ht="12.75">
       <c r="A8" s="40">
         <v>1006</v>
       </c>
@@ -2045,7 +2070,7 @@
       <c r="F8" s="40"/>
       <c r="G8" s="41"/>
     </row>
-    <row r="9" spans="1:7" ht="13">
+    <row r="9" spans="1:7" ht="12.75">
       <c r="A9" s="40">
         <v>1129</v>
       </c>
@@ -2060,7 +2085,7 @@
       <c r="F9" s="40"/>
       <c r="G9" s="41"/>
     </row>
-    <row r="10" spans="1:7" ht="13">
+    <row r="10" spans="1:7" ht="12.75">
       <c r="A10" s="40">
         <v>1236</v>
       </c>
@@ -2075,7 +2100,7 @@
       <c r="F10" s="40"/>
       <c r="G10" s="41"/>
     </row>
-    <row r="11" spans="1:7" ht="13">
+    <row r="11" spans="1:7" ht="12.75">
       <c r="A11" s="40">
         <v>1041</v>
       </c>
@@ -2090,7 +2115,7 @@
       <c r="F11" s="40"/>
       <c r="G11" s="41"/>
     </row>
-    <row r="12" spans="1:7" ht="13">
+    <row r="12" spans="1:7" ht="12.75">
       <c r="A12" s="40">
         <v>1016</v>
       </c>
@@ -2105,7 +2130,7 @@
       <c r="F12" s="40"/>
       <c r="G12" s="41"/>
     </row>
-    <row r="13" spans="1:7" ht="13">
+    <row r="13" spans="1:7" ht="12.75">
       <c r="A13" s="40">
         <v>1195</v>
       </c>
@@ -2120,7 +2145,7 @@
       <c r="F13" s="40"/>
       <c r="G13" s="41"/>
     </row>
-    <row r="14" spans="1:7" ht="13">
+    <row r="14" spans="1:7" ht="12.75">
       <c r="A14" s="40">
         <v>1072</v>
       </c>
@@ -2135,7 +2160,7 @@
       <c r="F14" s="40"/>
       <c r="G14" s="41"/>
     </row>
-    <row r="15" spans="1:7" ht="13">
+    <row r="15" spans="1:7" ht="12.75">
       <c r="A15" s="40">
         <v>1073</v>
       </c>
@@ -2150,7 +2175,7 @@
       <c r="F15" s="40"/>
       <c r="G15" s="41"/>
     </row>
-    <row r="16" spans="1:7" ht="13">
+    <row r="16" spans="1:7" ht="12.75">
       <c r="A16" s="40">
         <v>1101</v>
       </c>
@@ -2165,7 +2190,7 @@
       <c r="F16" s="40"/>
       <c r="G16" s="41"/>
     </row>
-    <row r="17" spans="1:7" ht="13">
+    <row r="17" spans="1:7" ht="12.75">
       <c r="A17" s="40">
         <v>1026</v>
       </c>
@@ -2180,7 +2205,7 @@
       <c r="F17" s="40"/>
       <c r="G17" s="41"/>
     </row>
-    <row r="18" spans="1:7" ht="13">
+    <row r="18" spans="1:7" ht="12.75">
       <c r="A18" s="40">
         <v>1040</v>
       </c>
@@ -2195,7 +2220,7 @@
       <c r="F18" s="40"/>
       <c r="G18" s="41"/>
     </row>
-    <row r="19" spans="1:7" ht="13">
+    <row r="19" spans="1:7" ht="12.75">
       <c r="A19" s="40">
         <v>1126</v>
       </c>
@@ -2210,7 +2235,7 @@
       <c r="F19" s="40"/>
       <c r="G19" s="41"/>
     </row>
-    <row r="20" spans="1:7" ht="13">
+    <row r="20" spans="1:7" ht="12.75">
       <c r="A20" s="40">
         <v>1181</v>
       </c>
@@ -2225,7 +2250,7 @@
       <c r="F20" s="40"/>
       <c r="G20" s="41"/>
     </row>
-    <row r="21" spans="1:7" ht="13">
+    <row r="21" spans="1:7" ht="12.75">
       <c r="A21" s="40">
         <v>1002</v>
       </c>
@@ -2240,7 +2265,7 @@
       <c r="F21" s="40"/>
       <c r="G21" s="41"/>
     </row>
-    <row r="22" spans="1:7" ht="13">
+    <row r="22" spans="1:7" ht="12.75">
       <c r="A22" s="40">
         <v>1166</v>
       </c>
@@ -2255,7 +2280,7 @@
       <c r="F22" s="40"/>
       <c r="G22" s="41"/>
     </row>
-    <row r="23" spans="1:7" ht="13">
+    <row r="23" spans="1:7" ht="12.75">
       <c r="A23" s="40">
         <v>1248</v>
       </c>
@@ -2270,7 +2295,7 @@
       <c r="F23" s="40"/>
       <c r="G23" s="41"/>
     </row>
-    <row r="24" spans="1:7" ht="13">
+    <row r="24" spans="1:7" ht="12.75">
       <c r="A24" s="40">
         <v>1138</v>
       </c>
@@ -2285,7 +2310,7 @@
       <c r="F24" s="40"/>
       <c r="G24" s="41"/>
     </row>
-    <row r="25" spans="1:7" ht="13">
+    <row r="25" spans="1:7" ht="12.75">
       <c r="A25" s="40">
         <v>1256</v>
       </c>
@@ -2300,7 +2325,7 @@
       <c r="F25" s="40"/>
       <c r="G25" s="41"/>
     </row>
-    <row r="26" spans="1:7" ht="13">
+    <row r="26" spans="1:7" ht="12.75">
       <c r="A26" s="40">
         <v>1011</v>
       </c>
@@ -2315,7 +2340,7 @@
       <c r="F26" s="40"/>
       <c r="G26" s="41"/>
     </row>
-    <row r="27" spans="1:7" ht="13">
+    <row r="27" spans="1:7" ht="12.75">
       <c r="A27" s="40">
         <v>1163</v>
       </c>
@@ -2330,7 +2355,7 @@
       <c r="F27" s="40"/>
       <c r="G27" s="41"/>
     </row>
-    <row r="28" spans="1:7" ht="13">
+    <row r="28" spans="1:7" ht="12.75">
       <c r="A28" s="40">
         <v>1002</v>
       </c>
@@ -2345,7 +2370,7 @@
       <c r="F28" s="40"/>
       <c r="G28" s="41"/>
     </row>
-    <row r="29" spans="1:7" ht="13">
+    <row r="29" spans="1:7" ht="12.75">
       <c r="A29" s="40">
         <v>1078</v>
       </c>
@@ -2360,7 +2385,7 @@
       <c r="F29" s="40"/>
       <c r="G29" s="41"/>
     </row>
-    <row r="30" spans="1:7" ht="13">
+    <row r="30" spans="1:7" ht="12.75">
       <c r="A30" s="40">
         <v>1058</v>
       </c>
@@ -2375,7 +2400,7 @@
       <c r="F30" s="40"/>
       <c r="G30" s="41"/>
     </row>
-    <row r="31" spans="1:7" ht="13">
+    <row r="31" spans="1:7" ht="12.75">
       <c r="A31" s="40">
         <v>1135</v>
       </c>
@@ -2390,7 +2415,7 @@
       <c r="F31" s="40"/>
       <c r="G31" s="41"/>
     </row>
-    <row r="33" spans="4:5" ht="13">
+    <row r="33" spans="4:5" ht="12.75">
       <c r="D33" s="44" t="s">
         <v>85</v>
       </c>
@@ -2434,18 +2459,18 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.6640625" customWidth="1"/>
-    <col min="3" max="3" width="15.33203125" customWidth="1"/>
+    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" customWidth="1"/>
+    <col min="3" max="3" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17" customHeight="1">
+    <row r="1" spans="1:3" ht="17.100000000000001" customHeight="1">
       <c r="A1" s="79" t="s">
         <v>45</v>
       </c>
@@ -2518,6 +2543,18 @@
     <mergeCell ref="B8:C8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{593AA9FD-DD17-4D57-8A6C-E07B0A3E9DF9}">
+          <x14:formula1>
+            <xm:f>Tables!$V$3:$V$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>B2:C2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2526,15 +2563,15 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="K32" sqref="K32"/>
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="25.33203125" customWidth="1"/>
-    <col min="2" max="2" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="25.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
     <col min="3" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="20.1640625" customWidth="1"/>
+    <col min="7" max="7" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1">
@@ -2763,7 +2800,10 @@
       <c r="D19" s="31"/>
       <c r="E19" s="31"/>
       <c r="F19" s="31"/>
-      <c r="G19" s="31"/>
+      <c r="G19" s="31" t="e" cm="1">
+        <f t="array" ref="G19">mod</f>
+        <v>#NAME?</v>
+      </c>
     </row>
     <row r="20" spans="1:7" ht="14.25" customHeight="1">
       <c r="A20" s="31"/>
@@ -2978,17 +3018,17 @@
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="9" width="6.33203125" customWidth="1"/>
-    <col min="10" max="10" width="20.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="21" width="6.33203125" customWidth="1"/>
-    <col min="22" max="22" width="14.83203125" customWidth="1"/>
-    <col min="23" max="23" width="8.5" customWidth="1"/>
-    <col min="24" max="26" width="6.33203125" customWidth="1"/>
+    <col min="1" max="9" width="6.28515625" customWidth="1"/>
+    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="21" width="6.28515625" customWidth="1"/>
+    <col min="22" max="22" width="14.85546875" customWidth="1"/>
+    <col min="23" max="23" width="8.42578125" customWidth="1"/>
+    <col min="24" max="26" width="6.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="13">
+    <row r="1" spans="1:23" ht="12.75">
       <c r="A1" s="84" t="s">
         <v>58</v>
       </c>
@@ -3002,20 +3042,20 @@
       <c r="J1" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
-      <c r="S1" s="69"/>
-      <c r="T1" s="70"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="66"/>
       <c r="V1" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="W1" s="70"/>
+      <c r="W1" s="66"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1">
       <c r="A2" s="11" t="s">
@@ -3024,12 +3064,12 @@
       <c r="B2" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="70"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="66"/>
       <c r="J2" s="12" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
fixed random content on last sheet of lookup hw
</commit_message>
<xml_diff>
--- a/docs/unit1/2_lookup_match_if/(Starter-Workbook)-HW-Lookups-Match-IF.xlsx
+++ b/docs/unit1/2_lookup_match_if/(Starter-Workbook)-HW-Lookups-Match-IF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\CCE270\content\docs\unit1\2_lookup_match_if\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jones/PycharmProjects/content/docs/unit1/2_lookup_match_if/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF320F51-9C6F-44C8-9D69-E2F9630463F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D67114-760E-1245-95CD-F874892297CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydrometer Analysis" sheetId="1" r:id="rId1"/>
@@ -35,33 +35,8 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
-    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
-      <xlwcv:version setVersion="1"/>
-    </ext>
   </extLst>
 </workbook>
-</file>
-
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1092,27 +1067,21 @@
     <xf numFmtId="164" fontId="24" fillId="20" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1121,6 +1090,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1481,25 +1456,25 @@
   </sheetPr>
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="11" customWidth="1"/>
-    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.83203125" customWidth="1"/>
     <col min="3" max="6" width="11" customWidth="1"/>
-    <col min="7" max="13" width="14.42578125" customWidth="1"/>
+    <col min="7" max="13" width="14.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" s="55" customFormat="1" ht="32.1" customHeight="1">
-      <c r="A1" s="69" t="s">
+    <row r="1" spans="1:13" s="55" customFormat="1" ht="32" customHeight="1">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
       <c r="G1" s="56"/>
       <c r="H1" s="57"/>
       <c r="I1" s="57"/>
@@ -1509,11 +1484,11 @@
       <c r="M1" s="57"/>
     </row>
     <row r="2" spans="1:13" ht="15">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
       <c r="D2" s="53" t="s">
         <v>2</v>
       </c>
@@ -1526,11 +1501,11 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:13" ht="15">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="66"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="70"/>
       <c r="D3" s="50" t="s">
         <v>6</v>
       </c>
@@ -1543,11 +1518,11 @@
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:13" ht="15">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="66"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="70"/>
       <c r="D4" s="50" t="s">
         <v>9</v>
       </c>
@@ -1558,11 +1533,11 @@
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:13" ht="15">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="74"/>
-      <c r="C5" s="75"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="73"/>
       <c r="D5" s="50" t="s">
         <v>11</v>
       </c>
@@ -1575,9 +1550,9 @@
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:13" ht="15">
-      <c r="A6" s="76"/>
-      <c r="B6" s="77"/>
-      <c r="C6" s="78"/>
+      <c r="A6" s="74"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="76"/>
       <c r="D6" s="50" t="s">
         <v>13</v>
       </c>
@@ -1588,11 +1563,11 @@
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:13" ht="15">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="65"/>
-      <c r="C7" s="66"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="70"/>
       <c r="D7" s="50" t="s">
         <v>16</v>
       </c>
@@ -1603,11 +1578,11 @@
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:13" ht="15">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="65"/>
-      <c r="C8" s="66"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="70"/>
       <c r="D8" s="50" t="s">
         <v>18</v>
       </c>
@@ -1618,11 +1593,11 @@
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:13" ht="15">
-      <c r="A9" s="64" t="s">
+      <c r="A9" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="65"/>
-      <c r="C9" s="66"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="70"/>
       <c r="D9" s="50" t="s">
         <v>20</v>
       </c>
@@ -1632,11 +1607,11 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:13" ht="15">
-      <c r="A10" s="64" t="s">
+      <c r="A10" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="65"/>
-      <c r="C10" s="66"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="50" t="s">
         <v>22</v>
       </c>
@@ -1645,11 +1620,11 @@
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:13" ht="15">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="66"/>
+      <c r="B11" s="69"/>
+      <c r="C11" s="70"/>
       <c r="D11" s="50" t="s">
         <v>24</v>
       </c>
@@ -1660,26 +1635,26 @@
       <c r="G11" s="5"/>
     </row>
     <row r="12" spans="1:13" ht="18" customHeight="1"/>
-    <row r="13" spans="1:13" ht="26.1" customHeight="1">
-      <c r="A13" s="67" t="s">
+    <row r="13" spans="1:13" ht="26" customHeight="1">
+      <c r="A13" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="67" t="s">
+      <c r="B13" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="67" t="s">
+      <c r="C13" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="67" t="s">
+      <c r="D13" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="67" t="s">
+      <c r="E13" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="67" t="s">
+      <c r="F13" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="67" t="s">
+      <c r="G13" s="77" t="s">
         <v>31</v>
       </c>
       <c r="H13" s="1"/>
@@ -1689,14 +1664,14 @@
       <c r="L13" s="1"/>
       <c r="M13" s="1"/>
     </row>
-    <row r="14" spans="1:13" ht="6.95" customHeight="1" thickBot="1">
-      <c r="A14" s="68"/>
-      <c r="B14" s="68"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="68"/>
+    <row r="14" spans="1:13" ht="7" customHeight="1" thickBot="1">
+      <c r="A14" s="78"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="78"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1704,7 +1679,7 @@
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
     </row>
-    <row r="15" spans="1:13" thickBot="1">
+    <row r="15" spans="1:13" ht="16" thickBot="1">
       <c r="A15" s="6">
         <v>0.25</v>
       </c>
@@ -1719,7 +1694,7 @@
       </c>
       <c r="G15" s="25"/>
     </row>
-    <row r="16" spans="1:13" thickBot="1">
+    <row r="16" spans="1:13" ht="16" thickBot="1">
       <c r="A16" s="6">
         <v>0.5</v>
       </c>
@@ -1734,7 +1709,7 @@
       </c>
       <c r="G16" s="28"/>
     </row>
-    <row r="17" spans="1:7" thickBot="1">
+    <row r="17" spans="1:7" ht="16" thickBot="1">
       <c r="A17" s="6">
         <v>1</v>
       </c>
@@ -1749,7 +1724,7 @@
       </c>
       <c r="G17" s="28"/>
     </row>
-    <row r="18" spans="1:7" thickBot="1">
+    <row r="18" spans="1:7" ht="16" thickBot="1">
       <c r="A18" s="6">
         <v>2</v>
       </c>
@@ -1764,7 +1739,7 @@
       </c>
       <c r="G18" s="28"/>
     </row>
-    <row r="19" spans="1:7" thickBot="1">
+    <row r="19" spans="1:7" ht="16" thickBot="1">
       <c r="A19" s="6">
         <v>4</v>
       </c>
@@ -1779,7 +1754,7 @@
       </c>
       <c r="G19" s="28"/>
     </row>
-    <row r="20" spans="1:7" thickBot="1">
+    <row r="20" spans="1:7" ht="16" thickBot="1">
       <c r="A20" s="6">
         <v>8</v>
       </c>
@@ -1794,7 +1769,7 @@
       </c>
       <c r="G20" s="28"/>
     </row>
-    <row r="21" spans="1:7" thickBot="1">
+    <row r="21" spans="1:7" ht="16" thickBot="1">
       <c r="A21" s="6">
         <v>15</v>
       </c>
@@ -1809,7 +1784,7 @@
       </c>
       <c r="G21" s="28"/>
     </row>
-    <row r="22" spans="1:7" thickBot="1">
+    <row r="22" spans="1:7" ht="16" thickBot="1">
       <c r="A22" s="6">
         <v>30</v>
       </c>
@@ -1824,7 +1799,7 @@
       </c>
       <c r="G22" s="28"/>
     </row>
-    <row r="23" spans="1:7" thickBot="1">
+    <row r="23" spans="1:7" ht="16" thickBot="1">
       <c r="A23" s="6">
         <v>60</v>
       </c>
@@ -1839,7 +1814,7 @@
       </c>
       <c r="G23" s="28"/>
     </row>
-    <row r="24" spans="1:7" thickBot="1">
+    <row r="24" spans="1:7" ht="16" thickBot="1">
       <c r="A24" s="6">
         <v>787</v>
       </c>
@@ -1854,7 +1829,7 @@
       </c>
       <c r="G24" s="28"/>
     </row>
-    <row r="25" spans="1:7" thickBot="1">
+    <row r="25" spans="1:7" ht="16" thickBot="1">
       <c r="A25" s="6">
         <v>1459</v>
       </c>
@@ -1898,11 +1873,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C6"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="E13:E14"/>
@@ -1915,6 +1885,11 @@
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1932,17 +1907,17 @@
       <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="20.85546875" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.7109375" style="39" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" style="39" customWidth="1"/>
-    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="39" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.1640625" style="39" customWidth="1"/>
+    <col min="6" max="6" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="17.100000000000001" customHeight="1">
+    <row r="1" spans="1:7" ht="17" customHeight="1">
       <c r="A1" s="42" t="s">
         <v>32</v>
       </c>
@@ -1965,7 +1940,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="12.75">
+    <row r="2" spans="1:7" ht="13">
       <c r="A2" s="40">
         <v>1124</v>
       </c>
@@ -1980,7 +1955,7 @@
       <c r="F2" s="40"/>
       <c r="G2" s="41"/>
     </row>
-    <row r="3" spans="1:7" ht="12.75">
+    <row r="3" spans="1:7" ht="13">
       <c r="A3" s="40">
         <v>1107</v>
       </c>
@@ -1995,7 +1970,7 @@
       <c r="F3" s="40"/>
       <c r="G3" s="40"/>
     </row>
-    <row r="4" spans="1:7" ht="12.75">
+    <row r="4" spans="1:7" ht="13">
       <c r="A4" s="40">
         <v>1163</v>
       </c>
@@ -2010,7 +1985,7 @@
       <c r="F4" s="40"/>
       <c r="G4" s="40"/>
     </row>
-    <row r="5" spans="1:7" ht="12.75">
+    <row r="5" spans="1:7" ht="13">
       <c r="A5" s="40">
         <v>1182</v>
       </c>
@@ -2025,7 +2000,7 @@
       <c r="F5" s="40"/>
       <c r="G5" s="40"/>
     </row>
-    <row r="6" spans="1:7" ht="12.75">
+    <row r="6" spans="1:7" ht="13">
       <c r="A6" s="40">
         <v>1175</v>
       </c>
@@ -2040,7 +2015,7 @@
       <c r="F6" s="40"/>
       <c r="G6" s="41"/>
     </row>
-    <row r="7" spans="1:7" ht="12.75">
+    <row r="7" spans="1:7" ht="13">
       <c r="A7" s="40">
         <v>1049</v>
       </c>
@@ -2055,7 +2030,7 @@
       <c r="F7" s="40"/>
       <c r="G7" s="41"/>
     </row>
-    <row r="8" spans="1:7" ht="12.75">
+    <row r="8" spans="1:7" ht="13">
       <c r="A8" s="40">
         <v>1006</v>
       </c>
@@ -2070,7 +2045,7 @@
       <c r="F8" s="40"/>
       <c r="G8" s="41"/>
     </row>
-    <row r="9" spans="1:7" ht="12.75">
+    <row r="9" spans="1:7" ht="13">
       <c r="A9" s="40">
         <v>1129</v>
       </c>
@@ -2085,7 +2060,7 @@
       <c r="F9" s="40"/>
       <c r="G9" s="41"/>
     </row>
-    <row r="10" spans="1:7" ht="12.75">
+    <row r="10" spans="1:7" ht="13">
       <c r="A10" s="40">
         <v>1236</v>
       </c>
@@ -2100,7 +2075,7 @@
       <c r="F10" s="40"/>
       <c r="G10" s="41"/>
     </row>
-    <row r="11" spans="1:7" ht="12.75">
+    <row r="11" spans="1:7" ht="13">
       <c r="A11" s="40">
         <v>1041</v>
       </c>
@@ -2115,7 +2090,7 @@
       <c r="F11" s="40"/>
       <c r="G11" s="41"/>
     </row>
-    <row r="12" spans="1:7" ht="12.75">
+    <row r="12" spans="1:7" ht="13">
       <c r="A12" s="40">
         <v>1016</v>
       </c>
@@ -2130,7 +2105,7 @@
       <c r="F12" s="40"/>
       <c r="G12" s="41"/>
     </row>
-    <row r="13" spans="1:7" ht="12.75">
+    <row r="13" spans="1:7" ht="13">
       <c r="A13" s="40">
         <v>1195</v>
       </c>
@@ -2145,7 +2120,7 @@
       <c r="F13" s="40"/>
       <c r="G13" s="41"/>
     </row>
-    <row r="14" spans="1:7" ht="12.75">
+    <row r="14" spans="1:7" ht="13">
       <c r="A14" s="40">
         <v>1072</v>
       </c>
@@ -2160,7 +2135,7 @@
       <c r="F14" s="40"/>
       <c r="G14" s="41"/>
     </row>
-    <row r="15" spans="1:7" ht="12.75">
+    <row r="15" spans="1:7" ht="13">
       <c r="A15" s="40">
         <v>1073</v>
       </c>
@@ -2175,7 +2150,7 @@
       <c r="F15" s="40"/>
       <c r="G15" s="41"/>
     </row>
-    <row r="16" spans="1:7" ht="12.75">
+    <row r="16" spans="1:7" ht="13">
       <c r="A16" s="40">
         <v>1101</v>
       </c>
@@ -2190,7 +2165,7 @@
       <c r="F16" s="40"/>
       <c r="G16" s="41"/>
     </row>
-    <row r="17" spans="1:7" ht="12.75">
+    <row r="17" spans="1:7" ht="13">
       <c r="A17" s="40">
         <v>1026</v>
       </c>
@@ -2205,7 +2180,7 @@
       <c r="F17" s="40"/>
       <c r="G17" s="41"/>
     </row>
-    <row r="18" spans="1:7" ht="12.75">
+    <row r="18" spans="1:7" ht="13">
       <c r="A18" s="40">
         <v>1040</v>
       </c>
@@ -2220,7 +2195,7 @@
       <c r="F18" s="40"/>
       <c r="G18" s="41"/>
     </row>
-    <row r="19" spans="1:7" ht="12.75">
+    <row r="19" spans="1:7" ht="13">
       <c r="A19" s="40">
         <v>1126</v>
       </c>
@@ -2235,7 +2210,7 @@
       <c r="F19" s="40"/>
       <c r="G19" s="41"/>
     </row>
-    <row r="20" spans="1:7" ht="12.75">
+    <row r="20" spans="1:7" ht="13">
       <c r="A20" s="40">
         <v>1181</v>
       </c>
@@ -2250,7 +2225,7 @@
       <c r="F20" s="40"/>
       <c r="G20" s="41"/>
     </row>
-    <row r="21" spans="1:7" ht="12.75">
+    <row r="21" spans="1:7" ht="13">
       <c r="A21" s="40">
         <v>1002</v>
       </c>
@@ -2265,7 +2240,7 @@
       <c r="F21" s="40"/>
       <c r="G21" s="41"/>
     </row>
-    <row r="22" spans="1:7" ht="12.75">
+    <row r="22" spans="1:7" ht="13">
       <c r="A22" s="40">
         <v>1166</v>
       </c>
@@ -2280,7 +2255,7 @@
       <c r="F22" s="40"/>
       <c r="G22" s="41"/>
     </row>
-    <row r="23" spans="1:7" ht="12.75">
+    <row r="23" spans="1:7" ht="13">
       <c r="A23" s="40">
         <v>1248</v>
       </c>
@@ -2295,7 +2270,7 @@
       <c r="F23" s="40"/>
       <c r="G23" s="41"/>
     </row>
-    <row r="24" spans="1:7" ht="12.75">
+    <row r="24" spans="1:7" ht="13">
       <c r="A24" s="40">
         <v>1138</v>
       </c>
@@ -2310,7 +2285,7 @@
       <c r="F24" s="40"/>
       <c r="G24" s="41"/>
     </row>
-    <row r="25" spans="1:7" ht="12.75">
+    <row r="25" spans="1:7" ht="13">
       <c r="A25" s="40">
         <v>1256</v>
       </c>
@@ -2325,7 +2300,7 @@
       <c r="F25" s="40"/>
       <c r="G25" s="41"/>
     </row>
-    <row r="26" spans="1:7" ht="12.75">
+    <row r="26" spans="1:7" ht="13">
       <c r="A26" s="40">
         <v>1011</v>
       </c>
@@ -2340,7 +2315,7 @@
       <c r="F26" s="40"/>
       <c r="G26" s="41"/>
     </row>
-    <row r="27" spans="1:7" ht="12.75">
+    <row r="27" spans="1:7" ht="13">
       <c r="A27" s="40">
         <v>1163</v>
       </c>
@@ -2355,7 +2330,7 @@
       <c r="F27" s="40"/>
       <c r="G27" s="41"/>
     </row>
-    <row r="28" spans="1:7" ht="12.75">
+    <row r="28" spans="1:7" ht="13">
       <c r="A28" s="40">
         <v>1002</v>
       </c>
@@ -2370,7 +2345,7 @@
       <c r="F28" s="40"/>
       <c r="G28" s="41"/>
     </row>
-    <row r="29" spans="1:7" ht="12.75">
+    <row r="29" spans="1:7" ht="13">
       <c r="A29" s="40">
         <v>1078</v>
       </c>
@@ -2385,7 +2360,7 @@
       <c r="F29" s="40"/>
       <c r="G29" s="41"/>
     </row>
-    <row r="30" spans="1:7" ht="12.75">
+    <row r="30" spans="1:7" ht="13">
       <c r="A30" s="40">
         <v>1058</v>
       </c>
@@ -2400,7 +2375,7 @@
       <c r="F30" s="40"/>
       <c r="G30" s="41"/>
     </row>
-    <row r="31" spans="1:7" ht="12.75">
+    <row r="31" spans="1:7" ht="13">
       <c r="A31" s="40">
         <v>1135</v>
       </c>
@@ -2415,7 +2390,7 @@
       <c r="F31" s="40"/>
       <c r="G31" s="41"/>
     </row>
-    <row r="33" spans="4:5" ht="12.75">
+    <row r="33" spans="4:5" ht="13">
       <c r="D33" s="44" t="s">
         <v>85</v>
       </c>
@@ -2459,18 +2434,18 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.7109375" customWidth="1"/>
-    <col min="3" max="3" width="15.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" customWidth="1"/>
+    <col min="3" max="3" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="17.100000000000001" customHeight="1">
+    <row r="1" spans="1:3" ht="17" customHeight="1">
       <c r="A1" s="79" t="s">
         <v>45</v>
       </c>
@@ -2563,15 +2538,15 @@
   <dimension ref="A1:G40"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+    <col min="2" max="2" width="9.6640625" customWidth="1"/>
     <col min="3" max="6" width="8" customWidth="1"/>
-    <col min="7" max="7" width="20.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1">
@@ -2800,10 +2775,7 @@
       <c r="D19" s="31"/>
       <c r="E19" s="31"/>
       <c r="F19" s="31"/>
-      <c r="G19" s="31" t="e" cm="1">
-        <f t="array" ref="G19">mod</f>
-        <v>#NAME?</v>
-      </c>
+      <c r="G19" s="31"/>
     </row>
     <row r="20" spans="1:7" ht="14.25" customHeight="1">
       <c r="A20" s="31"/>
@@ -3018,17 +2990,17 @@
       <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="9" width="6.28515625" customWidth="1"/>
-    <col min="10" max="10" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="21" width="6.28515625" customWidth="1"/>
-    <col min="22" max="22" width="14.85546875" customWidth="1"/>
-    <col min="23" max="23" width="8.42578125" customWidth="1"/>
-    <col min="24" max="26" width="6.28515625" customWidth="1"/>
+    <col min="1" max="9" width="6.33203125" customWidth="1"/>
+    <col min="10" max="10" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="11" max="21" width="6.33203125" customWidth="1"/>
+    <col min="22" max="22" width="14.83203125" customWidth="1"/>
+    <col min="23" max="23" width="8.5" customWidth="1"/>
+    <col min="24" max="26" width="6.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="12.75">
+    <row r="1" spans="1:23" ht="13">
       <c r="A1" s="84" t="s">
         <v>58</v>
       </c>
@@ -3042,20 +3014,20 @@
       <c r="J1" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="66"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69"/>
+      <c r="S1" s="69"/>
+      <c r="T1" s="70"/>
       <c r="V1" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="W1" s="66"/>
+      <c r="W1" s="70"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1">
       <c r="A2" s="11" t="s">
@@ -3064,12 +3036,12 @@
       <c r="B2" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="66"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="70"/>
       <c r="J2" s="12" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Minor fixes to HW
</commit_message>
<xml_diff>
--- a/docs/unit1/2_lookup_match_if/(Starter-Workbook)-HW-Lookups-Match-IF.xlsx
+++ b/docs/unit1/2_lookup_match_if/(Starter-Workbook)-HW-Lookups-Match-IF.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jones/PycharmProjects/content/docs/unit1/2_lookup_match_if/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/griffinizu/PycharmProjects/content/docs/unit1/2_lookup_match_if/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19D67114-760E-1245-95CD-F874892297CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABE90C2-B350-B146-BE6C-3103518BA54B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydrometer Analysis" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="87">
   <si>
     <t>Hydrometer Analysis</t>
   </si>
@@ -1067,6 +1067,17 @@
     <xf numFmtId="164" fontId="24" fillId="20" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1077,11 +1088,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1090,12 +1096,6 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1456,7 +1456,7 @@
   </sheetPr>
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
       <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
@@ -1469,12 +1469,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="55" customFormat="1" ht="32" customHeight="1">
-      <c r="A1" s="64" t="s">
+      <c r="A1" s="69" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="65"/>
-      <c r="C1" s="65"/>
-      <c r="D1" s="65"/>
+      <c r="B1" s="70"/>
+      <c r="C1" s="70"/>
+      <c r="D1" s="70"/>
       <c r="G1" s="56"/>
       <c r="H1" s="57"/>
       <c r="I1" s="57"/>
@@ -1484,11 +1484,11 @@
       <c r="M1" s="57"/>
     </row>
     <row r="2" spans="1:13" ht="15">
-      <c r="A2" s="66" t="s">
+      <c r="A2" s="71" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="67"/>
-      <c r="C2" s="67"/>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
       <c r="D2" s="53" t="s">
         <v>2</v>
       </c>
@@ -1501,11 +1501,11 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:13" ht="15">
-      <c r="A3" s="68" t="s">
+      <c r="A3" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="69"/>
-      <c r="C3" s="70"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="66"/>
       <c r="D3" s="50" t="s">
         <v>6</v>
       </c>
@@ -1518,11 +1518,11 @@
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:13" ht="15">
-      <c r="A4" s="68" t="s">
+      <c r="A4" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="69"/>
-      <c r="C4" s="70"/>
+      <c r="B4" s="65"/>
+      <c r="C4" s="66"/>
       <c r="D4" s="50" t="s">
         <v>9</v>
       </c>
@@ -1533,11 +1533,11 @@
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:13" ht="15">
-      <c r="A5" s="71" t="s">
+      <c r="A5" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="72"/>
-      <c r="C5" s="73"/>
+      <c r="B5" s="74"/>
+      <c r="C5" s="75"/>
       <c r="D5" s="50" t="s">
         <v>11</v>
       </c>
@@ -1550,9 +1550,9 @@
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:13" ht="15">
-      <c r="A6" s="74"/>
-      <c r="B6" s="75"/>
-      <c r="C6" s="76"/>
+      <c r="A6" s="76"/>
+      <c r="B6" s="77"/>
+      <c r="C6" s="78"/>
       <c r="D6" s="50" t="s">
         <v>13</v>
       </c>
@@ -1563,11 +1563,11 @@
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:13" ht="15">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="64" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="69"/>
-      <c r="C7" s="70"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="66"/>
       <c r="D7" s="50" t="s">
         <v>16</v>
       </c>
@@ -1578,11 +1578,11 @@
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:13" ht="15">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="69"/>
-      <c r="C8" s="70"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="66"/>
       <c r="D8" s="50" t="s">
         <v>18</v>
       </c>
@@ -1593,11 +1593,11 @@
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:13" ht="15">
-      <c r="A9" s="68" t="s">
+      <c r="A9" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="69"/>
-      <c r="C9" s="70"/>
+      <c r="B9" s="65"/>
+      <c r="C9" s="66"/>
       <c r="D9" s="50" t="s">
         <v>20</v>
       </c>
@@ -1607,11 +1607,11 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:13" ht="15">
-      <c r="A10" s="68" t="s">
+      <c r="A10" s="64" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="69"/>
-      <c r="C10" s="70"/>
+      <c r="B10" s="65"/>
+      <c r="C10" s="66"/>
       <c r="D10" s="50" t="s">
         <v>22</v>
       </c>
@@ -1620,11 +1620,11 @@
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:13" ht="15">
-      <c r="A11" s="68" t="s">
+      <c r="A11" s="64" t="s">
         <v>23</v>
       </c>
-      <c r="B11" s="69"/>
-      <c r="C11" s="70"/>
+      <c r="B11" s="65"/>
+      <c r="C11" s="66"/>
       <c r="D11" s="50" t="s">
         <v>24</v>
       </c>
@@ -1636,25 +1636,25 @@
     </row>
     <row r="12" spans="1:13" ht="18" customHeight="1"/>
     <row r="13" spans="1:13" ht="26" customHeight="1">
-      <c r="A13" s="77" t="s">
+      <c r="A13" s="67" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="77" t="s">
+      <c r="B13" s="67" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="77" t="s">
+      <c r="C13" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="77" t="s">
+      <c r="D13" s="67" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="77" t="s">
+      <c r="E13" s="67" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="77" t="s">
+      <c r="F13" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="G13" s="77" t="s">
+      <c r="G13" s="67" t="s">
         <v>31</v>
       </c>
       <c r="H13" s="1"/>
@@ -1665,13 +1665,13 @@
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:13" ht="7" customHeight="1" thickBot="1">
-      <c r="A14" s="78"/>
-      <c r="B14" s="78"/>
-      <c r="C14" s="78"/>
-      <c r="D14" s="78"/>
-      <c r="E14" s="78"/>
-      <c r="F14" s="78"/>
-      <c r="G14" s="78"/>
+      <c r="A14" s="68"/>
+      <c r="B14" s="68"/>
+      <c r="C14" s="68"/>
+      <c r="D14" s="68"/>
+      <c r="E14" s="68"/>
+      <c r="F14" s="68"/>
+      <c r="G14" s="68"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1873,6 +1873,11 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C6"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="E13:E14"/>
@@ -1885,11 +1890,6 @@
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -2434,8 +2434,8 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -2456,14 +2456,18 @@
       <c r="A2" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="B2" s="81"/>
+      <c r="B2" s="81" t="s">
+        <v>63</v>
+      </c>
       <c r="C2" s="82"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="48" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="59"/>
+      <c r="B3" s="59">
+        <v>3</v>
+      </c>
       <c r="C3" s="48" t="s">
         <v>48</v>
       </c>
@@ -2472,7 +2476,9 @@
       <c r="A4" s="58" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="60"/>
+      <c r="B4" s="60">
+        <v>4400</v>
+      </c>
       <c r="C4" s="58" t="s">
         <v>50</v>
       </c>
@@ -3014,20 +3020,20 @@
       <c r="J1" s="86" t="s">
         <v>59</v>
       </c>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
-      <c r="S1" s="69"/>
-      <c r="T1" s="70"/>
+      <c r="K1" s="65"/>
+      <c r="L1" s="65"/>
+      <c r="M1" s="65"/>
+      <c r="N1" s="65"/>
+      <c r="O1" s="65"/>
+      <c r="P1" s="65"/>
+      <c r="Q1" s="65"/>
+      <c r="R1" s="65"/>
+      <c r="S1" s="65"/>
+      <c r="T1" s="66"/>
       <c r="V1" s="87" t="s">
         <v>60</v>
       </c>
-      <c r="W1" s="70"/>
+      <c r="W1" s="66"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1">
       <c r="A2" s="11" t="s">
@@ -3036,12 +3042,12 @@
       <c r="B2" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="69"/>
-      <c r="D2" s="69"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="70"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
+      <c r="F2" s="65"/>
+      <c r="G2" s="65"/>
+      <c r="H2" s="66"/>
       <c r="J2" s="12" t="s">
         <v>33</v>
       </c>

</xml_diff>

<commit_message>
Updated Stokes' Coefficient to be "K", updated rubric, updated some instructions/hints
</commit_message>
<xml_diff>
--- a/docs/unit1/2_lookup_match_if/(Starter-Workbook)-HW-Lookups-Match-IF.xlsx
+++ b/docs/unit1/2_lookup_match_if/(Starter-Workbook)-HW-Lookups-Match-IF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/griffinizu/PycharmProjects/content/docs/unit1/2_lookup_match_if/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EABE90C2-B350-B146-BE6C-3103518BA54B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C9C2122-A379-F544-BCFC-B5A8996D6D5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hydrometer Analysis" sheetId="1" r:id="rId1"/>
@@ -108,9 +108,6 @@
     <t>Stokes' law coefficient</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>Specific gravity correction factor</t>
   </si>
   <si>
@@ -301,6 +298,9 @@
   </si>
   <si>
     <t>Median:</t>
+  </si>
+  <si>
+    <t>K</t>
   </si>
 </sst>
 </file>
@@ -1067,27 +1067,21 @@
     <xf numFmtId="164" fontId="24" fillId="20" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="26" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="25" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="26" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
@@ -1096,6 +1090,12 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="26" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1456,8 +1456,8 @@
   </sheetPr>
   <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="124" zoomScaleNormal="124" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -1469,12 +1469,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" s="55" customFormat="1" ht="32" customHeight="1">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="70"/>
-      <c r="C1" s="70"/>
-      <c r="D1" s="70"/>
+      <c r="B1" s="65"/>
+      <c r="C1" s="65"/>
+      <c r="D1" s="65"/>
       <c r="G1" s="56"/>
       <c r="H1" s="57"/>
       <c r="I1" s="57"/>
@@ -1484,11 +1484,11 @@
       <c r="M1" s="57"/>
     </row>
     <row r="2" spans="1:13" ht="15">
-      <c r="A2" s="71" t="s">
+      <c r="A2" s="66" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
+      <c r="B2" s="67"/>
+      <c r="C2" s="67"/>
       <c r="D2" s="53" t="s">
         <v>2</v>
       </c>
@@ -1501,11 +1501,11 @@
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:13" ht="15">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="65"/>
-      <c r="C3" s="66"/>
+      <c r="B3" s="69"/>
+      <c r="C3" s="70"/>
       <c r="D3" s="50" t="s">
         <v>6</v>
       </c>
@@ -1518,11 +1518,11 @@
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:13" ht="15">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="65"/>
-      <c r="C4" s="66"/>
+      <c r="B4" s="69"/>
+      <c r="C4" s="70"/>
       <c r="D4" s="50" t="s">
         <v>9</v>
       </c>
@@ -1533,11 +1533,11 @@
       <c r="G4" s="4"/>
     </row>
     <row r="5" spans="1:13" ht="15">
-      <c r="A5" s="73" t="s">
+      <c r="A5" s="71" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="74"/>
-      <c r="C5" s="75"/>
+      <c r="B5" s="72"/>
+      <c r="C5" s="73"/>
       <c r="D5" s="50" t="s">
         <v>11</v>
       </c>
@@ -1550,9 +1550,9 @@
       <c r="G5" s="4"/>
     </row>
     <row r="6" spans="1:13" ht="15">
-      <c r="A6" s="76"/>
-      <c r="B6" s="77"/>
-      <c r="C6" s="78"/>
+      <c r="A6" s="74"/>
+      <c r="B6" s="75"/>
+      <c r="C6" s="76"/>
       <c r="D6" s="50" t="s">
         <v>13</v>
       </c>
@@ -1563,11 +1563,11 @@
       <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:13" ht="15">
-      <c r="A7" s="64" t="s">
+      <c r="A7" s="68" t="s">
         <v>15</v>
       </c>
-      <c r="B7" s="65"/>
-      <c r="C7" s="66"/>
+      <c r="B7" s="69"/>
+      <c r="C7" s="70"/>
       <c r="D7" s="50" t="s">
         <v>16</v>
       </c>
@@ -1578,11 +1578,11 @@
       <c r="G7" s="4"/>
     </row>
     <row r="8" spans="1:13" ht="15">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="68" t="s">
         <v>17</v>
       </c>
-      <c r="B8" s="65"/>
-      <c r="C8" s="66"/>
+      <c r="B8" s="69"/>
+      <c r="C8" s="70"/>
       <c r="D8" s="50" t="s">
         <v>18</v>
       </c>
@@ -1593,11 +1593,11 @@
       <c r="G8" s="4"/>
     </row>
     <row r="9" spans="1:13" ht="15">
-      <c r="A9" s="64" t="s">
+      <c r="A9" s="68" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="65"/>
-      <c r="C9" s="66"/>
+      <c r="B9" s="69"/>
+      <c r="C9" s="70"/>
       <c r="D9" s="50" t="s">
         <v>20</v>
       </c>
@@ -1607,26 +1607,26 @@
       <c r="I9" s="1"/>
     </row>
     <row r="10" spans="1:13" ht="15">
-      <c r="A10" s="64" t="s">
+      <c r="A10" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="65"/>
-      <c r="C10" s="66"/>
+      <c r="B10" s="69"/>
+      <c r="C10" s="70"/>
       <c r="D10" s="50" t="s">
-        <v>22</v>
+        <v>86</v>
       </c>
       <c r="E10" s="50"/>
       <c r="F10" s="52"/>
       <c r="G10" s="5"/>
     </row>
     <row r="11" spans="1:13" ht="15">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="68" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="69"/>
+      <c r="C11" s="70"/>
+      <c r="D11" s="50" t="s">
         <v>23</v>
-      </c>
-      <c r="B11" s="65"/>
-      <c r="C11" s="66"/>
-      <c r="D11" s="50" t="s">
-        <v>24</v>
       </c>
       <c r="E11" s="50">
         <v>1.01</v>
@@ -1636,26 +1636,26 @@
     </row>
     <row r="12" spans="1:13" ht="18" customHeight="1"/>
     <row r="13" spans="1:13" ht="26" customHeight="1">
-      <c r="A13" s="67" t="s">
+      <c r="A13" s="77" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="77" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="67" t="s">
+      <c r="C13" s="77" t="s">
         <v>26</v>
       </c>
-      <c r="C13" s="67" t="s">
+      <c r="D13" s="77" t="s">
         <v>27</v>
       </c>
-      <c r="D13" s="67" t="s">
+      <c r="E13" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="E13" s="67" t="s">
+      <c r="F13" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="F13" s="67" t="s">
+      <c r="G13" s="77" t="s">
         <v>30</v>
-      </c>
-      <c r="G13" s="67" t="s">
-        <v>31</v>
       </c>
       <c r="H13" s="1"/>
       <c r="I13" s="1"/>
@@ -1665,13 +1665,13 @@
       <c r="M13" s="1"/>
     </row>
     <row r="14" spans="1:13" ht="7" customHeight="1" thickBot="1">
-      <c r="A14" s="68"/>
-      <c r="B14" s="68"/>
-      <c r="C14" s="68"/>
-      <c r="D14" s="68"/>
-      <c r="E14" s="68"/>
-      <c r="F14" s="68"/>
-      <c r="G14" s="68"/>
+      <c r="A14" s="78"/>
+      <c r="B14" s="78"/>
+      <c r="C14" s="78"/>
+      <c r="D14" s="78"/>
+      <c r="E14" s="78"/>
+      <c r="F14" s="78"/>
+      <c r="G14" s="78"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -1873,11 +1873,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:C3"/>
-    <mergeCell ref="A4:C4"/>
-    <mergeCell ref="A5:C6"/>
     <mergeCell ref="A7:C7"/>
     <mergeCell ref="A8:C8"/>
     <mergeCell ref="E13:E14"/>
@@ -1890,6 +1885,11 @@
     <mergeCell ref="B13:B14"/>
     <mergeCell ref="C13:C14"/>
     <mergeCell ref="D13:D14"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A2:C2"/>
+    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="A4:C4"/>
+    <mergeCell ref="A5:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1919,25 +1919,25 @@
   <sheetData>
     <row r="1" spans="1:7" ht="17" customHeight="1">
       <c r="A1" s="42" t="s">
+        <v>31</v>
+      </c>
+      <c r="B1" s="43" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="43" t="s">
+      <c r="C1" s="42" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="D1" s="43" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="43" t="s">
+      <c r="E1" s="43" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="43" t="s">
-        <v>36</v>
-      </c>
       <c r="F1" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="G1" s="43" t="s">
         <v>83</v>
-      </c>
-      <c r="G1" s="43" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="13">
@@ -1945,7 +1945,7 @@
         <v>1124</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C2" s="40">
         <v>7</v>
@@ -1960,7 +1960,7 @@
         <v>1107</v>
       </c>
       <c r="B3" s="40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C3" s="40">
         <v>5</v>
@@ -1975,7 +1975,7 @@
         <v>1163</v>
       </c>
       <c r="B4" s="40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C4" s="40">
         <v>7</v>
@@ -1990,7 +1990,7 @@
         <v>1182</v>
       </c>
       <c r="B5" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="40">
         <v>3</v>
@@ -2005,7 +2005,7 @@
         <v>1175</v>
       </c>
       <c r="B6" s="40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C6" s="40">
         <v>15</v>
@@ -2020,7 +2020,7 @@
         <v>1049</v>
       </c>
       <c r="B7" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="40">
         <v>8</v>
@@ -2035,7 +2035,7 @@
         <v>1006</v>
       </c>
       <c r="B8" s="40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C8" s="40">
         <v>9</v>
@@ -2050,7 +2050,7 @@
         <v>1129</v>
       </c>
       <c r="B9" s="40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C9" s="40">
         <v>1</v>
@@ -2065,7 +2065,7 @@
         <v>1236</v>
       </c>
       <c r="B10" s="40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C10" s="40">
         <v>2</v>
@@ -2080,7 +2080,7 @@
         <v>1041</v>
       </c>
       <c r="B11" s="40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="40">
         <v>20</v>
@@ -2095,7 +2095,7 @@
         <v>1016</v>
       </c>
       <c r="B12" s="40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C12" s="40">
         <v>1</v>
@@ -2110,7 +2110,7 @@
         <v>1195</v>
       </c>
       <c r="B13" s="40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C13" s="40">
         <v>1</v>
@@ -2125,7 +2125,7 @@
         <v>1072</v>
       </c>
       <c r="B14" s="40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C14" s="40">
         <v>1</v>
@@ -2140,7 +2140,7 @@
         <v>1073</v>
       </c>
       <c r="B15" s="40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C15" s="40">
         <v>2</v>
@@ -2155,7 +2155,7 @@
         <v>1101</v>
       </c>
       <c r="B16" s="40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="40">
         <v>10</v>
@@ -2170,7 +2170,7 @@
         <v>1026</v>
       </c>
       <c r="B17" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C17" s="40">
         <v>5</v>
@@ -2185,7 +2185,7 @@
         <v>1040</v>
       </c>
       <c r="B18" s="40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C18" s="40">
         <v>15</v>
@@ -2200,7 +2200,7 @@
         <v>1126</v>
       </c>
       <c r="B19" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19" s="40">
         <v>8</v>
@@ -2215,7 +2215,7 @@
         <v>1181</v>
       </c>
       <c r="B20" s="40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C20" s="40">
         <v>11</v>
@@ -2230,7 +2230,7 @@
         <v>1002</v>
       </c>
       <c r="B21" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C21" s="40">
         <v>2</v>
@@ -2245,7 +2245,7 @@
         <v>1166</v>
       </c>
       <c r="B22" s="40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C22" s="40">
         <v>10</v>
@@ -2260,7 +2260,7 @@
         <v>1248</v>
       </c>
       <c r="B23" s="40" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" s="40">
         <v>10</v>
@@ -2275,7 +2275,7 @@
         <v>1138</v>
       </c>
       <c r="B24" s="40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" s="40">
         <v>1</v>
@@ -2290,7 +2290,7 @@
         <v>1256</v>
       </c>
       <c r="B25" s="40" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C25" s="40">
         <v>1</v>
@@ -2305,7 +2305,7 @@
         <v>1011</v>
       </c>
       <c r="B26" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" s="40">
         <v>2</v>
@@ -2320,7 +2320,7 @@
         <v>1163</v>
       </c>
       <c r="B27" s="40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C27" s="40">
         <v>11</v>
@@ -2335,7 +2335,7 @@
         <v>1002</v>
       </c>
       <c r="B28" s="40" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C28" s="40">
         <v>15</v>
@@ -2350,7 +2350,7 @@
         <v>1078</v>
       </c>
       <c r="B29" s="40" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29" s="40">
         <v>4</v>
@@ -2365,7 +2365,7 @@
         <v>1058</v>
       </c>
       <c r="B30" s="40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C30" s="40">
         <v>3</v>
@@ -2380,7 +2380,7 @@
         <v>1135</v>
       </c>
       <c r="B31" s="40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C31" s="40">
         <v>3</v>
@@ -2392,19 +2392,19 @@
     </row>
     <row r="33" spans="4:5" ht="13">
       <c r="D33" s="44" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E33" s="45"/>
     </row>
     <row r="34" spans="4:5" ht="15.75" customHeight="1">
       <c r="D34" s="44" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E34" s="45"/>
     </row>
     <row r="35" spans="4:5" ht="15.75" customHeight="1">
       <c r="D35" s="46" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E35" s="45"/>
     </row>
@@ -2434,7 +2434,7 @@
   </sheetPr>
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -2447,72 +2447,72 @@
   <sheetData>
     <row r="1" spans="1:3" ht="17" customHeight="1">
       <c r="A1" s="79" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="80"/>
       <c r="C1" s="80"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1">
       <c r="A2" s="58" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" s="81" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C2" s="82"/>
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1">
       <c r="A3" s="48" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B3" s="59">
         <v>3</v>
       </c>
       <c r="C3" s="48" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1">
       <c r="A4" s="58" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B4" s="60">
         <v>4400</v>
       </c>
       <c r="C4" s="58" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1">
       <c r="A5" s="48" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B5" s="61"/>
       <c r="C5" s="48" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1">
       <c r="A6" s="58" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B6" s="62"/>
       <c r="C6" s="58" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1">
       <c r="A7" s="48" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" s="63"/>
       <c r="C7" s="49" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1">
       <c r="A8" s="58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="83"/>
       <c r="C8" s="82"/>
@@ -2557,7 +2557,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="26.25" customHeight="1">
       <c r="A1" s="38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B1" s="31"/>
       <c r="C1" s="31"/>
@@ -2586,13 +2586,13 @@
     </row>
     <row r="4" spans="1:7" ht="14.25" customHeight="1">
       <c r="A4" s="33" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B4" s="37">
         <v>5000</v>
       </c>
       <c r="C4" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D4" s="31"/>
       <c r="E4" s="31"/>
@@ -2601,14 +2601,14 @@
     </row>
     <row r="5" spans="1:7" ht="14.25" customHeight="1">
       <c r="A5" s="33" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="37">
         <f>10*10^6</f>
         <v>10000000</v>
       </c>
       <c r="C5" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D5" s="31"/>
       <c r="E5" s="31"/>
@@ -2617,13 +2617,13 @@
     </row>
     <row r="6" spans="1:7" ht="14.25" customHeight="1">
       <c r="A6" s="33" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B6" s="37">
         <v>144</v>
       </c>
       <c r="C6" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D6" s="31"/>
       <c r="E6" s="31"/>
@@ -2632,13 +2632,13 @@
     </row>
     <row r="7" spans="1:7" ht="14.25" customHeight="1">
       <c r="A7" s="33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="37">
         <v>48</v>
       </c>
       <c r="C7" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D7" s="31"/>
       <c r="E7" s="31"/>
@@ -2647,7 +2647,7 @@
     </row>
     <row r="8" spans="1:7" ht="14.25" customHeight="1">
       <c r="A8" s="33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B8" s="37"/>
       <c r="C8" s="31"/>
@@ -2658,13 +2658,13 @@
     </row>
     <row r="9" spans="1:7" ht="14.25" customHeight="1">
       <c r="A9" s="33" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B9" s="37">
         <v>2</v>
       </c>
       <c r="C9" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D9" s="31"/>
       <c r="E9" s="31"/>
@@ -2673,13 +2673,13 @@
     </row>
     <row r="10" spans="1:7" ht="14.25" customHeight="1">
       <c r="A10" s="33" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B10" s="37">
         <v>4</v>
       </c>
       <c r="C10" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D10" s="31"/>
       <c r="E10" s="31"/>
@@ -2688,11 +2688,11 @@
     </row>
     <row r="11" spans="1:7" ht="14.25" customHeight="1">
       <c r="A11" s="33" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B11" s="32"/>
       <c r="C11" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D11" s="31"/>
       <c r="E11" s="31"/>
@@ -2710,11 +2710,11 @@
     </row>
     <row r="13" spans="1:7" ht="14.25" customHeight="1">
       <c r="A13" s="33" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B13" s="32"/>
       <c r="C13" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D13" s="31"/>
       <c r="E13" s="31"/>
@@ -2723,7 +2723,7 @@
     </row>
     <row r="14" spans="1:7" ht="14.25" customHeight="1">
       <c r="A14" s="33" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B14" s="32"/>
       <c r="C14" s="31"/>
@@ -2734,7 +2734,7 @@
     </row>
     <row r="15" spans="1:7" ht="14.25" customHeight="1">
       <c r="A15" s="33" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B15" s="32"/>
       <c r="C15" s="31"/>
@@ -2745,11 +2745,11 @@
     </row>
     <row r="16" spans="1:7" ht="14.25" customHeight="1">
       <c r="A16" s="33" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B16" s="32"/>
       <c r="C16" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D16" s="31"/>
       <c r="E16" s="31"/>
@@ -2992,8 +2992,8 @@
   </sheetPr>
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.5" defaultRowHeight="15.75" customHeight="1"/>
@@ -3008,7 +3008,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="13">
       <c r="A1" s="84" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B1" s="85"/>
       <c r="C1" s="85"/>
@@ -3018,38 +3018,38 @@
       <c r="G1" s="85"/>
       <c r="H1" s="85"/>
       <c r="J1" s="86" t="s">
+        <v>58</v>
+      </c>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69"/>
+      <c r="S1" s="69"/>
+      <c r="T1" s="70"/>
+      <c r="V1" s="87" t="s">
         <v>59</v>
       </c>
-      <c r="K1" s="65"/>
-      <c r="L1" s="65"/>
-      <c r="M1" s="65"/>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="65"/>
-      <c r="Q1" s="65"/>
-      <c r="R1" s="65"/>
-      <c r="S1" s="65"/>
-      <c r="T1" s="66"/>
-      <c r="V1" s="87" t="s">
-        <v>60</v>
-      </c>
-      <c r="W1" s="66"/>
+      <c r="W1" s="70"/>
     </row>
     <row r="2" spans="1:23" ht="15.75" customHeight="1">
       <c r="A2" s="11" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B2" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="65"/>
-      <c r="D2" s="65"/>
-      <c r="E2" s="65"/>
-      <c r="F2" s="65"/>
-      <c r="G2" s="65"/>
-      <c r="H2" s="66"/>
+      <c r="C2" s="69"/>
+      <c r="D2" s="69"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="70"/>
       <c r="J2" s="12" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="K2" s="13">
         <v>1</v>
@@ -3082,10 +3082,10 @@
         <v>10</v>
       </c>
       <c r="V2" s="14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="W2" s="14" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:23" ht="15.75" customHeight="1">
@@ -3112,7 +3112,7 @@
         <v>2.8</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="K3" s="18">
         <v>100</v>
@@ -3154,7 +3154,7 @@
         <v>65</v>
       </c>
       <c r="V3" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="W3" s="20">
         <v>70</v>
@@ -3186,7 +3186,7 @@
         <v>1.3599999999999999E-2</v>
       </c>
       <c r="J4" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K4" s="18">
         <v>120</v>
@@ -3228,7 +3228,7 @@
         <v>85</v>
       </c>
       <c r="V4" s="19" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="W4" s="20">
         <v>72</v>
@@ -3260,7 +3260,7 @@
         <v>1.34E-2</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="K5" s="18">
         <v>150</v>
@@ -3302,7 +3302,7 @@
         <v>115</v>
       </c>
       <c r="V5" s="19" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="W5" s="20">
         <v>80</v>
@@ -3334,7 +3334,7 @@
         <v>1.32E-2</v>
       </c>
       <c r="J6" s="17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K6" s="18">
         <v>100</v>
@@ -3376,7 +3376,7 @@
         <v>65</v>
       </c>
       <c r="V6" s="19" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="W6" s="20">
         <v>100</v>
@@ -3408,7 +3408,7 @@
         <v>1.3100000000000001E-2</v>
       </c>
       <c r="J7" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="K7" s="18">
         <v>70</v>
@@ -3476,7 +3476,7 @@
         <v>1.29E-2</v>
       </c>
       <c r="J8" s="17" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="K8" s="18">
         <v>80</v>
@@ -3544,7 +3544,7 @@
         <v>1.2800000000000001E-2</v>
       </c>
       <c r="J9" s="17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K9" s="18">
         <v>150</v>

</xml_diff>